<commit_message>
remove transaction type from ui fill spreadsheet
</commit_message>
<xml_diff>
--- a/Regression/templates/PriceProductGroups.xlsx
+++ b/Regression/templates/PriceProductGroups.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="AlphazoneMakeCounties" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3717" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3493" uniqueCount="396">
   <si>
     <t>KBB Elite</t>
   </si>
@@ -3037,8 +3037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FR21"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+    <sheetView topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="BA2" sqref="BA2:BA21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3383,9 +3383,7 @@
         <v>1</v>
       </c>
       <c r="AZ2" s="36"/>
-      <c r="BA2" s="70" t="s">
-        <v>191</v>
-      </c>
+      <c r="BA2" s="70"/>
       <c r="BB2" s="36"/>
       <c r="BC2" s="36"/>
       <c r="BD2" s="36"/>
@@ -3617,9 +3615,7 @@
         <v>1</v>
       </c>
       <c r="AZ3" s="8"/>
-      <c r="BA3" s="10" t="s">
-        <v>191</v>
-      </c>
+      <c r="BA3" s="10"/>
       <c r="BB3" s="8"/>
       <c r="BC3" s="8"/>
       <c r="BD3" s="8"/>
@@ -3851,9 +3847,7 @@
         <v>1</v>
       </c>
       <c r="AZ4" s="8"/>
-      <c r="BA4" s="10" t="s">
-        <v>191</v>
-      </c>
+      <c r="BA4" s="10"/>
       <c r="BB4" s="8"/>
       <c r="BC4" s="8"/>
       <c r="BD4" s="8"/>
@@ -4083,9 +4077,7 @@
         <v>1</v>
       </c>
       <c r="AZ5" s="8"/>
-      <c r="BA5" s="10" t="s">
-        <v>191</v>
-      </c>
+      <c r="BA5" s="10"/>
       <c r="BB5" s="8"/>
       <c r="BC5" s="8"/>
       <c r="BD5" s="8"/>
@@ -4317,9 +4309,7 @@
         <v>1</v>
       </c>
       <c r="AZ6" s="8"/>
-      <c r="BA6" s="10" t="s">
-        <v>191</v>
-      </c>
+      <c r="BA6" s="10"/>
       <c r="BB6" s="8"/>
       <c r="BC6" s="8"/>
       <c r="BD6" s="8"/>
@@ -4549,9 +4539,7 @@
         <v>1</v>
       </c>
       <c r="AZ7" s="8"/>
-      <c r="BA7" s="10" t="s">
-        <v>191</v>
-      </c>
+      <c r="BA7" s="10"/>
       <c r="BB7" s="8"/>
       <c r="BC7" s="8"/>
       <c r="BD7" s="8"/>
@@ -4797,9 +4785,7 @@
       <c r="AZ8" s="10">
         <v>100</v>
       </c>
-      <c r="BA8" s="10" t="s">
-        <v>191</v>
-      </c>
+      <c r="BA8" s="10"/>
       <c r="BB8" s="10">
         <v>2</v>
       </c>
@@ -5051,9 +5037,7 @@
       <c r="AZ9" s="10">
         <v>100</v>
       </c>
-      <c r="BA9" s="10" t="s">
-        <v>191</v>
-      </c>
+      <c r="BA9" s="10"/>
       <c r="BB9" s="10">
         <v>2</v>
       </c>
@@ -5301,9 +5285,7 @@
       <c r="AZ10" s="35">
         <v>100</v>
       </c>
-      <c r="BA10" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="BA10" s="35"/>
       <c r="BB10" s="35">
         <v>2</v>
       </c>
@@ -5424,9 +5406,7 @@
         <v>1</v>
       </c>
       <c r="AZ11" s="8"/>
-      <c r="BA11" s="10" t="s">
-        <v>191</v>
-      </c>
+      <c r="BA11" s="10"/>
       <c r="BB11" s="8"/>
       <c r="BC11" s="8"/>
       <c r="BD11" s="8"/>
@@ -5660,9 +5640,7 @@
         <v>1</v>
       </c>
       <c r="AZ12" s="8"/>
-      <c r="BA12" s="10" t="s">
-        <v>191</v>
-      </c>
+      <c r="BA12" s="10"/>
       <c r="BB12" s="8"/>
       <c r="BC12" s="8"/>
       <c r="BD12" s="8"/>
@@ -5894,9 +5872,7 @@
         <v>1</v>
       </c>
       <c r="AZ13" s="8"/>
-      <c r="BA13" s="10" t="s">
-        <v>191</v>
-      </c>
+      <c r="BA13" s="10"/>
       <c r="BB13" s="8"/>
       <c r="BC13" s="8"/>
       <c r="BD13" s="8"/>
@@ -6126,9 +6102,7 @@
         <v>1</v>
       </c>
       <c r="AZ14" s="8"/>
-      <c r="BA14" s="10" t="s">
-        <v>191</v>
-      </c>
+      <c r="BA14" s="10"/>
       <c r="BB14" s="8"/>
       <c r="BC14" s="8"/>
       <c r="BD14" s="8"/>
@@ -6360,9 +6334,7 @@
         <v>1</v>
       </c>
       <c r="AZ15" s="8"/>
-      <c r="BA15" s="10" t="s">
-        <v>191</v>
-      </c>
+      <c r="BA15" s="10"/>
       <c r="BB15" s="8"/>
       <c r="BC15" s="8"/>
       <c r="BD15" s="8"/>
@@ -6594,9 +6566,7 @@
         <v>1</v>
       </c>
       <c r="AZ16" s="8"/>
-      <c r="BA16" s="10" t="s">
-        <v>191</v>
-      </c>
+      <c r="BA16" s="10"/>
       <c r="BB16" s="8"/>
       <c r="BC16" s="8"/>
       <c r="BD16" s="8"/>
@@ -6830,9 +6800,7 @@
         <v>1</v>
       </c>
       <c r="AZ17" s="8"/>
-      <c r="BA17" s="10" t="s">
-        <v>191</v>
-      </c>
+      <c r="BA17" s="10"/>
       <c r="BB17" s="8"/>
       <c r="BC17" s="8"/>
       <c r="BD17" s="8"/>
@@ -7064,9 +7032,7 @@
         <v>1</v>
       </c>
       <c r="AZ18" s="8"/>
-      <c r="BA18" s="10" t="s">
-        <v>191</v>
-      </c>
+      <c r="BA18" s="10"/>
       <c r="BB18" s="8"/>
       <c r="BC18" s="8"/>
       <c r="BD18" s="8"/>
@@ -7292,9 +7258,7 @@
         <v>1</v>
       </c>
       <c r="AZ19" s="8"/>
-      <c r="BA19" s="10" t="s">
-        <v>191</v>
-      </c>
+      <c r="BA19" s="10"/>
       <c r="BB19" s="8"/>
       <c r="BC19" s="8"/>
       <c r="BD19" s="8"/>
@@ -7522,9 +7486,7 @@
         <v>1</v>
       </c>
       <c r="AZ20" s="8"/>
-      <c r="BA20" s="10" t="s">
-        <v>191</v>
-      </c>
+      <c r="BA20" s="10"/>
       <c r="BB20" s="8"/>
       <c r="BC20" s="8"/>
       <c r="BD20" s="8"/>
@@ -7750,9 +7712,7 @@
         <v>1</v>
       </c>
       <c r="AZ21" s="8"/>
-      <c r="BA21" s="10" t="s">
-        <v>191</v>
-      </c>
+      <c r="BA21" s="10"/>
       <c r="BB21" s="8"/>
       <c r="BC21" s="8"/>
       <c r="BD21" s="8"/>
@@ -7887,8 +7847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="I4:K4"/>
+    <sheetView topLeftCell="AW1" workbookViewId="0">
+      <selection activeCell="BB2" sqref="BB2:BB20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="54.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8209,9 +8169,7 @@
       <c r="AX2" s="15"/>
       <c r="AY2" s="12"/>
       <c r="AZ2" s="37"/>
-      <c r="BB2" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="BB2" s="35"/>
       <c r="BC2" s="35">
         <v>2</v>
       </c>
@@ -8274,9 +8232,7 @@
       <c r="BA3" s="35">
         <v>20</v>
       </c>
-      <c r="BB3" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="BB3" s="35"/>
       <c r="BD3" s="35" t="s">
         <v>186</v>
       </c>
@@ -8349,9 +8305,7 @@
       </c>
       <c r="AX4" s="36"/>
       <c r="AZ4" s="15"/>
-      <c r="BB4" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="BB4" s="35"/>
       <c r="BD4" s="35" t="s">
         <v>186</v>
       </c>
@@ -8384,9 +8338,7 @@
       <c r="AX5" s="15"/>
       <c r="AY5" s="12"/>
       <c r="AZ5" s="37"/>
-      <c r="BB5" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="BB5" s="35"/>
       <c r="BI5" s="105" t="b">
         <v>1</v>
       </c>
@@ -8440,9 +8392,7 @@
       <c r="BA6" s="35">
         <v>20</v>
       </c>
-      <c r="BB6" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="BB6" s="35"/>
       <c r="BD6" s="35" t="s">
         <v>186</v>
       </c>
@@ -8502,9 +8452,7 @@
       <c r="BA7" s="35">
         <v>20</v>
       </c>
-      <c r="BB7" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="BB7" s="35"/>
       <c r="BD7" s="35" t="s">
         <v>186</v>
       </c>
@@ -8552,9 +8500,7 @@
       <c r="AX8" s="22"/>
       <c r="AY8" s="12"/>
       <c r="AZ8" s="37"/>
-      <c r="BB8" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="BB8" s="35"/>
       <c r="BD8" s="35" t="s">
         <v>186</v>
       </c>
@@ -8611,9 +8557,7 @@
       <c r="BA9" s="35">
         <v>20</v>
       </c>
-      <c r="BB9" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="BB9" s="35"/>
       <c r="BD9" s="35" t="s">
         <v>186</v>
       </c>
@@ -8667,9 +8611,7 @@
       <c r="AX10" s="80"/>
       <c r="AY10" s="26"/>
       <c r="AZ10" s="14"/>
-      <c r="BB10" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="BB10" s="35"/>
       <c r="BI10" s="105" t="b">
         <v>1</v>
       </c>
@@ -8762,9 +8704,7 @@
       <c r="AX11" s="12"/>
       <c r="AY11" s="26"/>
       <c r="AZ11" s="14"/>
-      <c r="BB11" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="BB11" s="35"/>
       <c r="BC11" s="35">
         <v>2</v>
       </c>
@@ -8856,9 +8796,7 @@
       <c r="AX12" s="12"/>
       <c r="AY12" s="37"/>
       <c r="AZ12" s="14"/>
-      <c r="BB12" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="BB12" s="35"/>
       <c r="BC12" s="35">
         <v>2</v>
       </c>
@@ -8907,9 +8845,7 @@
       <c r="AX13" s="12"/>
       <c r="AY13" s="71"/>
       <c r="AZ13" s="14"/>
-      <c r="BB13" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="BB13" s="35"/>
       <c r="BH13" s="32"/>
       <c r="BI13" s="105" t="b">
         <v>1</v>
@@ -8930,9 +8866,7 @@
         <v>180</v>
       </c>
       <c r="AY14" s="36"/>
-      <c r="BB14" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="BB14" s="35"/>
       <c r="BI14" s="105" t="b">
         <v>1</v>
       </c>
@@ -8950,9 +8884,7 @@
       <c r="AO15" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="BB15" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="BB15" s="35"/>
       <c r="BI15" s="105" t="b">
         <v>1</v>
       </c>
@@ -8970,9 +8902,7 @@
       <c r="AO16" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="BB16" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="BB16" s="35"/>
       <c r="BI16" s="105" t="b">
         <v>1</v>
       </c>
@@ -8991,9 +8921,7 @@
         <v>180</v>
       </c>
       <c r="AX17" s="15"/>
-      <c r="BB17" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="BB17" s="35"/>
       <c r="BI17" s="105" t="b">
         <v>1</v>
       </c>
@@ -9047,9 +8975,7 @@
       <c r="BA18" s="35">
         <v>20</v>
       </c>
-      <c r="BB18" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="BB18" s="35"/>
       <c r="BD18" s="35" t="s">
         <v>186</v>
       </c>
@@ -9115,9 +9041,7 @@
       <c r="AX19" s="36"/>
       <c r="AY19" s="12"/>
       <c r="AZ19" s="37"/>
-      <c r="BB19" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="BB19" s="35"/>
       <c r="BC19" s="35">
         <v>2</v>
       </c>
@@ -9188,9 +9112,7 @@
       </c>
       <c r="AY20" s="12"/>
       <c r="AZ20" s="71"/>
-      <c r="BB20" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="BB20" s="35"/>
       <c r="BC20" s="35">
         <v>2</v>
       </c>
@@ -9217,8 +9139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CP138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AL14" sqref="AL14"/>
+    <sheetView topLeftCell="BF1" workbookViewId="0">
+      <selection activeCell="BM2" sqref="BM2:BM24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9640,9 +9562,7 @@
       </c>
       <c r="BK2" s="12"/>
       <c r="BL2" s="37"/>
-      <c r="BM2" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM2" s="24"/>
       <c r="BN2" s="35">
         <v>2</v>
       </c>
@@ -9787,9 +9707,7 @@
       </c>
       <c r="BK3" s="12"/>
       <c r="BL3" s="37"/>
-      <c r="BM3" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM3" s="24"/>
       <c r="BN3" s="35">
         <v>2</v>
       </c>
@@ -9934,9 +9852,7 @@
       </c>
       <c r="BK4" s="12"/>
       <c r="BL4" s="37"/>
-      <c r="BM4" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM4" s="24"/>
       <c r="BN4" s="35">
         <v>2</v>
       </c>
@@ -10003,9 +9919,7 @@
       </c>
       <c r="BK5" s="118"/>
       <c r="BL5" s="37"/>
-      <c r="BM5" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM5" s="24"/>
       <c r="BO5" s="35" t="s">
         <v>186</v>
       </c>
@@ -10063,9 +9977,7 @@
       </c>
       <c r="BK6" s="118"/>
       <c r="BL6" s="37"/>
-      <c r="BM6" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM6" s="24"/>
       <c r="BO6" s="35" t="s">
         <v>186</v>
       </c>
@@ -10184,9 +10096,7 @@
       </c>
       <c r="BK7" s="118"/>
       <c r="BL7" s="37"/>
-      <c r="BM7" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM7" s="24"/>
       <c r="BN7" s="35">
         <v>2</v>
       </c>
@@ -10253,9 +10163,7 @@
       </c>
       <c r="BK8" s="118"/>
       <c r="BL8" s="37"/>
-      <c r="BM8" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM8" s="24"/>
       <c r="BO8" s="35" t="s">
         <v>186</v>
       </c>
@@ -10313,9 +10221,7 @@
       </c>
       <c r="BK9" s="118"/>
       <c r="BL9" s="37"/>
-      <c r="BM9" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM9" s="24"/>
       <c r="BO9" s="35" t="s">
         <v>186</v>
       </c>
@@ -10446,9 +10352,7 @@
       </c>
       <c r="BK10" s="12"/>
       <c r="BL10" s="37"/>
-      <c r="BM10" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM10" s="24"/>
       <c r="BN10" s="35">
         <v>2</v>
       </c>
@@ -10595,9 +10499,7 @@
       </c>
       <c r="BK11" s="12"/>
       <c r="BL11" s="37"/>
-      <c r="BM11" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM11" s="24"/>
       <c r="BN11" s="35">
         <v>2</v>
       </c>
@@ -10742,9 +10644,7 @@
       </c>
       <c r="BK12" s="12"/>
       <c r="BL12" s="37"/>
-      <c r="BM12" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM12" s="24"/>
       <c r="BN12" s="35">
         <v>2</v>
       </c>
@@ -10913,9 +10813,7 @@
         <v>100</v>
       </c>
       <c r="BL13" s="37"/>
-      <c r="BM13" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM13" s="24"/>
       <c r="BN13" s="35">
         <v>2</v>
       </c>
@@ -11060,9 +10958,7 @@
       </c>
       <c r="BK14" s="12"/>
       <c r="BL14" s="37"/>
-      <c r="BM14" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM14" s="24"/>
       <c r="BN14" s="35">
         <v>2</v>
       </c>
@@ -11209,9 +11105,7 @@
       </c>
       <c r="BK15" s="12"/>
       <c r="BL15" s="37"/>
-      <c r="BM15" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM15" s="24"/>
       <c r="BN15" s="35">
         <v>2</v>
       </c>
@@ -11352,9 +11246,7 @@
       </c>
       <c r="BK16" s="12"/>
       <c r="BL16" s="37"/>
-      <c r="BM16" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM16" s="24"/>
       <c r="BN16" s="35">
         <v>2</v>
       </c>
@@ -11495,9 +11387,7 @@
       </c>
       <c r="BK17" s="12"/>
       <c r="BL17" s="37"/>
-      <c r="BM17" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM17" s="24"/>
       <c r="BN17" s="35">
         <v>2</v>
       </c>
@@ -11638,9 +11528,7 @@
       </c>
       <c r="BK18" s="12"/>
       <c r="BL18" s="37"/>
-      <c r="BM18" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM18" s="24"/>
       <c r="BN18" s="35">
         <v>2</v>
       </c>
@@ -11736,9 +11624,7 @@
       </c>
       <c r="BK19" s="118"/>
       <c r="BL19" s="37"/>
-      <c r="BM19" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM19" s="24"/>
       <c r="BN19" s="2"/>
       <c r="BO19" s="35" t="s">
         <v>186</v>
@@ -11855,9 +11741,7 @@
       </c>
       <c r="BK20" s="118"/>
       <c r="BL20" s="37"/>
-      <c r="BM20" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM20" s="24"/>
       <c r="BN20" s="35">
         <v>2</v>
       </c>
@@ -11972,9 +11856,7 @@
       </c>
       <c r="BK21" s="118"/>
       <c r="BL21" s="37"/>
-      <c r="BM21" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM21" s="24"/>
       <c r="BN21" s="35">
         <v>2</v>
       </c>
@@ -12097,9 +11979,7 @@
       </c>
       <c r="BK22" s="118"/>
       <c r="BL22" s="37"/>
-      <c r="BM22" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM22" s="24"/>
       <c r="BN22" s="35">
         <v>2</v>
       </c>
@@ -12222,9 +12102,7 @@
       </c>
       <c r="BK23" s="118"/>
       <c r="BL23" s="37"/>
-      <c r="BM23" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM23" s="24"/>
       <c r="BN23" s="35">
         <v>2</v>
       </c>
@@ -12347,9 +12225,7 @@
       </c>
       <c r="BK24" s="118"/>
       <c r="BL24" s="37"/>
-      <c r="BM24" s="24" t="s">
-        <v>191</v>
-      </c>
+      <c r="BM24" s="24"/>
       <c r="BN24" s="35">
         <v>2</v>
       </c>
@@ -13105,8 +12981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="AY2" sqref="AY2:AY22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13344,9 +13220,7 @@
       <c r="AF2" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AY2" s="34" t="s">
-        <v>191</v>
-      </c>
+      <c r="AY2" s="35"/>
     </row>
     <row r="3" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
@@ -13372,9 +13246,7 @@
       <c r="AF3" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AY3" s="34" t="s">
-        <v>191</v>
-      </c>
+      <c r="AY3" s="35"/>
     </row>
     <row r="4" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
@@ -13430,9 +13302,7 @@
       <c r="AX4" s="35">
         <v>4</v>
       </c>
-      <c r="AY4" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AY4" s="35"/>
       <c r="BA4" s="35" t="s">
         <v>186</v>
       </c>
@@ -13494,9 +13364,7 @@
       <c r="AX5" s="35">
         <v>4</v>
       </c>
-      <c r="AY5" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AY5" s="35"/>
       <c r="BA5" s="35" t="s">
         <v>186</v>
       </c>
@@ -13539,9 +13407,7 @@
         <v>180</v>
       </c>
       <c r="AH6" s="2"/>
-      <c r="AY6" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AY6" s="35"/>
       <c r="BA6" s="35" t="s">
         <v>186</v>
       </c>
@@ -13600,9 +13466,7 @@
       <c r="AX7" s="35">
         <v>4</v>
       </c>
-      <c r="AY7" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AY7" s="35"/>
       <c r="BA7" s="35" t="s">
         <v>186</v>
       </c>
@@ -13632,9 +13496,7 @@
       <c r="AF8" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AY8" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AY8" s="35"/>
     </row>
     <row r="9" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
@@ -13658,9 +13520,7 @@
       <c r="AF9" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AY9" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AY9" s="35"/>
     </row>
     <row r="10" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
@@ -13684,9 +13544,7 @@
       <c r="AF10" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AY10" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AY10" s="35"/>
     </row>
     <row r="11" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
@@ -13708,9 +13566,7 @@
       <c r="AF11" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AY11" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AY11" s="35"/>
     </row>
     <row r="12" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
@@ -13727,6 +13583,7 @@
       <c r="AF12" s="35" t="s">
         <v>180</v>
       </c>
+      <c r="AY12" s="35"/>
     </row>
     <row r="13" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
@@ -13743,6 +13600,7 @@
       <c r="AF13" s="35" t="s">
         <v>180</v>
       </c>
+      <c r="AY13" s="35"/>
     </row>
     <row r="14" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
@@ -13764,9 +13622,7 @@
       <c r="AF14" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AY14" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AY14" s="35"/>
     </row>
     <row r="15" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
@@ -13788,9 +13644,7 @@
       <c r="AF15" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AY15" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AY15" s="35"/>
     </row>
     <row r="16" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
@@ -13812,9 +13666,7 @@
       <c r="AF16" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AY16" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AY16" s="35"/>
     </row>
     <row r="17" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
@@ -13889,9 +13741,7 @@
       <c r="AW17" s="35">
         <v>23789</v>
       </c>
-      <c r="AY17" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AY17" s="35"/>
       <c r="BA17" s="35" t="s">
         <v>186</v>
       </c>
@@ -13921,9 +13771,7 @@
       <c r="AF18" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AY18" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AY18" s="35"/>
     </row>
     <row r="19" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
@@ -13979,9 +13827,7 @@
       <c r="AX19" s="34" t="s">
         <v>197</v>
       </c>
-      <c r="AY19" s="34" t="s">
-        <v>191</v>
-      </c>
+      <c r="AY19" s="35"/>
       <c r="BA19" s="34" t="s">
         <v>186</v>
       </c>
@@ -14008,9 +13854,7 @@
       <c r="AF20" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AY20" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AY20" s="35"/>
     </row>
     <row r="21" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="35" t="s">
@@ -14052,9 +13896,7 @@
       <c r="AF21" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AY21" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AY21" s="35"/>
     </row>
     <row r="22" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="35" t="s">
@@ -14081,9 +13923,7 @@
       <c r="AV22" s="35">
         <v>100</v>
       </c>
-      <c r="AY22" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AY22" s="35"/>
       <c r="BA22" s="35" t="s">
         <v>186</v>
       </c>
@@ -14406,8 +14246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2:AD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14605,9 +14445,7 @@
       <c r="AC2" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AD2" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AD2" s="35"/>
       <c r="AE2" s="35" t="s">
         <v>192</v>
       </c>
@@ -14675,9 +14513,7 @@
       <c r="AC3" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AD3" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AD3" s="35"/>
       <c r="AE3" s="35" t="s">
         <v>192</v>
       </c>
@@ -14741,9 +14577,7 @@
       <c r="AC4" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AD4" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AD4" s="35"/>
       <c r="AE4" s="35" t="s">
         <v>192</v>
       </c>
@@ -14807,9 +14641,7 @@
       <c r="AC5" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AD5" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AD5" s="35"/>
       <c r="AE5" s="35" t="s">
         <v>192</v>
       </c>
@@ -14879,9 +14711,7 @@
       <c r="AC6" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AD6" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AD6" s="35"/>
       <c r="AE6" s="35" t="s">
         <v>192</v>
       </c>
@@ -14951,9 +14781,7 @@
       <c r="AC7" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AD7" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AD7" s="35"/>
       <c r="AE7" s="35" t="s">
         <v>192</v>
       </c>
@@ -15019,9 +14847,7 @@
       <c r="AC8" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AD8" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AD8" s="35"/>
       <c r="AE8" s="35" t="s">
         <v>192</v>
       </c>
@@ -15087,9 +14913,7 @@
       <c r="AC9" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AD9" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AD9" s="35"/>
       <c r="AE9" s="35" t="s">
         <v>192</v>
       </c>
@@ -15141,9 +14965,7 @@
       <c r="AC10" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AD10" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AD10" s="35"/>
       <c r="AE10" s="34"/>
       <c r="AF10" s="105" t="b">
         <v>1</v>
@@ -15195,9 +15017,7 @@
       <c r="AC11" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AD11" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AD11" s="35"/>
       <c r="AE11" s="34"/>
       <c r="AF11" s="105" t="b">
         <v>1</v>
@@ -15247,9 +15067,7 @@
       <c r="AC12" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AD12" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AD12" s="35"/>
       <c r="AE12" s="34"/>
       <c r="AF12" s="105" t="b">
         <v>1</v>
@@ -15299,9 +15117,7 @@
       <c r="AC13" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AD13" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AD13" s="35"/>
       <c r="AE13" s="34"/>
       <c r="AF13" s="105" t="b">
         <v>1</v>
@@ -15353,9 +15169,7 @@
       <c r="AC14" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AD14" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AD14" s="35"/>
       <c r="AE14" s="34"/>
       <c r="AF14" s="105" t="b">
         <v>1</v>
@@ -15407,9 +15221,7 @@
       <c r="AC15" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AD15" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AD15" s="35"/>
       <c r="AE15" s="34"/>
       <c r="AF15" s="105" t="b">
         <v>1</v>
@@ -15461,9 +15273,7 @@
       <c r="AC16" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AD16" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AD16" s="35"/>
       <c r="AE16" s="34"/>
       <c r="AF16" s="105" t="b">
         <v>1</v>
@@ -15515,9 +15325,7 @@
       <c r="AC17" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="AD17" s="35" t="s">
-        <v>191</v>
-      </c>
+      <c r="AD17" s="35"/>
       <c r="AE17" s="34"/>
       <c r="AF17" s="105" t="b">
         <v>1</v>
@@ -15534,7 +15342,7 @@
   <dimension ref="A1:AL13"/>
   <sheetViews>
     <sheetView topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AL2" sqref="AL2:AL13"/>
+      <selection activeCell="AH2" sqref="AH2:AH13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15705,9 +15513,6 @@
       <c r="V2" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="AH2" s="34" t="s">
-        <v>191</v>
-      </c>
       <c r="AL2" s="106" t="b">
         <v>1</v>
       </c>
@@ -15725,9 +15530,6 @@
       <c r="V3" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="AH3" s="34" t="s">
-        <v>191</v>
-      </c>
       <c r="AL3" s="106" t="b">
         <v>1</v>
       </c>
@@ -15760,9 +15562,6 @@
       <c r="AF4" s="34">
         <v>50</v>
       </c>
-      <c r="AH4" s="34" t="s">
-        <v>191</v>
-      </c>
       <c r="AK4" s="34" t="s">
         <v>192</v>
       </c>
@@ -15807,9 +15606,6 @@
       <c r="V5" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="AH5" s="34" t="s">
-        <v>191</v>
-      </c>
       <c r="AK5" s="34" t="s">
         <v>192</v>
       </c>
@@ -15842,9 +15638,6 @@
       <c r="AF6" s="34">
         <v>50</v>
       </c>
-      <c r="AH6" s="34" t="s">
-        <v>191</v>
-      </c>
       <c r="AL6" s="106" t="b">
         <v>1</v>
       </c>
@@ -15883,9 +15676,6 @@
       <c r="AE7" s="34">
         <v>100</v>
       </c>
-      <c r="AH7" s="34" t="s">
-        <v>191</v>
-      </c>
       <c r="AL7" s="106" t="b">
         <v>1</v>
       </c>
@@ -15903,9 +15693,6 @@
       <c r="V8" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="AH8" s="34" t="s">
-        <v>191</v>
-      </c>
       <c r="AL8" s="106" t="b">
         <v>1</v>
       </c>
@@ -15923,9 +15710,6 @@
       <c r="V9" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="AH9" s="34" t="s">
-        <v>191</v>
-      </c>
       <c r="AL9" s="106" t="b">
         <v>1</v>
       </c>
@@ -15943,9 +15727,6 @@
       <c r="V10" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="AH10" s="34" t="s">
-        <v>191</v>
-      </c>
       <c r="AL10" s="106" t="b">
         <v>1</v>
       </c>
@@ -15963,9 +15744,6 @@
       <c r="V11" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="AH11" s="34" t="s">
-        <v>191</v>
-      </c>
       <c r="AL11" s="106" t="b">
         <v>1</v>
       </c>
@@ -15983,9 +15761,6 @@
       <c r="V12" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="AH12" s="34" t="s">
-        <v>191</v>
-      </c>
       <c r="AL12" s="106" t="b">
         <v>1</v>
       </c>
@@ -16038,9 +15813,6 @@
       </c>
       <c r="AG13" s="34" t="s">
         <v>197</v>
-      </c>
-      <c r="AH13" s="34" t="s">
-        <v>191</v>
       </c>
       <c r="AI13" s="34" t="s">
         <v>186</v>
@@ -16062,8 +15834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FY124"/>
   <sheetViews>
-    <sheetView topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="AQ11" sqref="AQ11"/>
+    <sheetView tabSelected="1" topLeftCell="FA1" workbookViewId="0">
+      <selection activeCell="FF2" sqref="FF2:FF118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -16771,7 +16543,7 @@
       <c r="D2" s="51"/>
       <c r="E2" s="52">
         <f t="shared" ref="E2:E33" ca="1" si="0">TODAY()</f>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F2" s="51"/>
       <c r="G2" s="51"/>
@@ -16930,9 +16702,7 @@
       <c r="FC2" s="51"/>
       <c r="FD2" s="51"/>
       <c r="FE2" s="51"/>
-      <c r="FF2" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF2" s="51"/>
       <c r="FG2" s="51"/>
       <c r="FH2" s="51"/>
       <c r="FI2" s="53"/>
@@ -16962,7 +16732,7 @@
       <c r="D3" s="51"/>
       <c r="E3" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F3" s="51"/>
       <c r="G3" s="51"/>
@@ -17121,9 +16891,7 @@
       <c r="FC3" s="51"/>
       <c r="FD3" s="51"/>
       <c r="FE3" s="51"/>
-      <c r="FF3" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF3" s="51"/>
       <c r="FG3" s="51"/>
       <c r="FH3" s="51"/>
       <c r="FI3" s="53"/>
@@ -17153,7 +16921,7 @@
       <c r="D4" s="51"/>
       <c r="E4" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="51"/>
@@ -17312,9 +17080,7 @@
       <c r="FC4" s="51"/>
       <c r="FD4" s="51"/>
       <c r="FE4" s="51"/>
-      <c r="FF4" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF4" s="51"/>
       <c r="FG4" s="51"/>
       <c r="FH4" s="51"/>
       <c r="FI4" s="53"/>
@@ -17344,7 +17110,7 @@
       <c r="D5" s="51"/>
       <c r="E5" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F5" s="51"/>
       <c r="G5" s="51"/>
@@ -17503,9 +17269,7 @@
       <c r="FC5" s="51"/>
       <c r="FD5" s="51"/>
       <c r="FE5" s="51"/>
-      <c r="FF5" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF5" s="51"/>
       <c r="FG5" s="51"/>
       <c r="FH5" s="51"/>
       <c r="FI5" s="53"/>
@@ -17537,7 +17301,7 @@
       <c r="D6" s="51"/>
       <c r="E6" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F6" s="51" t="s">
         <v>265</v>
@@ -17720,9 +17484,7 @@
       <c r="FC6" s="51"/>
       <c r="FD6" s="51"/>
       <c r="FE6" s="51"/>
-      <c r="FF6" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF6" s="51"/>
       <c r="FG6" s="51"/>
       <c r="FH6" s="51"/>
       <c r="FI6" s="53"/>
@@ -17754,7 +17516,7 @@
       <c r="D7" s="51"/>
       <c r="E7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
@@ -17923,9 +17685,7 @@
       </c>
       <c r="FD7" s="51"/>
       <c r="FE7" s="51"/>
-      <c r="FF7" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF7" s="51"/>
       <c r="FG7" s="51"/>
       <c r="FH7" s="51"/>
       <c r="FI7" s="53"/>
@@ -17957,7 +17717,7 @@
       <c r="D8" s="51"/>
       <c r="E8" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F8" s="51"/>
       <c r="G8" s="51"/>
@@ -18130,9 +17890,7 @@
       <c r="FC8" s="51"/>
       <c r="FD8" s="51"/>
       <c r="FE8" s="51"/>
-      <c r="FF8" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF8" s="51"/>
       <c r="FG8" s="51"/>
       <c r="FH8" s="51"/>
       <c r="FI8" s="53"/>
@@ -18162,7 +17920,7 @@
       <c r="D9" s="51"/>
       <c r="E9" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
@@ -18329,9 +18087,7 @@
       </c>
       <c r="FD9" s="51"/>
       <c r="FE9" s="51"/>
-      <c r="FF9" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF9" s="51"/>
       <c r="FG9" s="51"/>
       <c r="FH9" s="51"/>
       <c r="FI9" s="53"/>
@@ -18361,7 +18117,7 @@
       <c r="D10" s="51"/>
       <c r="E10" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
@@ -18574,9 +18330,7 @@
       </c>
       <c r="FD10" s="51"/>
       <c r="FE10" s="51"/>
-      <c r="FF10" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF10" s="51"/>
       <c r="FG10" s="51" t="s">
         <v>197</v>
       </c>
@@ -18614,7 +18368,7 @@
       <c r="D11" s="51"/>
       <c r="E11" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
@@ -18829,9 +18583,7 @@
       </c>
       <c r="FD11" s="51"/>
       <c r="FE11" s="51"/>
-      <c r="FF11" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF11" s="51"/>
       <c r="FG11" s="51" t="s">
         <v>197</v>
       </c>
@@ -18869,7 +18621,7 @@
       <c r="D12" s="51"/>
       <c r="E12" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
@@ -19084,9 +18836,7 @@
       </c>
       <c r="FD12" s="51"/>
       <c r="FE12" s="51"/>
-      <c r="FF12" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF12" s="51"/>
       <c r="FG12" s="51" t="s">
         <v>197</v>
       </c>
@@ -19124,7 +18874,7 @@
       <c r="D13" s="51"/>
       <c r="E13" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F13" s="51"/>
       <c r="G13" s="51"/>
@@ -19327,9 +19077,7 @@
       <c r="FC13" s="51"/>
       <c r="FD13" s="51"/>
       <c r="FE13" s="51"/>
-      <c r="FF13" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF13" s="51"/>
       <c r="FG13" s="51"/>
       <c r="FH13" s="51"/>
       <c r="FI13" s="53"/>
@@ -19359,7 +19107,7 @@
       <c r="D14" s="51"/>
       <c r="E14" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F14" s="51"/>
       <c r="G14" s="51"/>
@@ -19566,9 +19314,7 @@
       <c r="FC14" s="51"/>
       <c r="FD14" s="51"/>
       <c r="FE14" s="51"/>
-      <c r="FF14" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF14" s="51"/>
       <c r="FG14" s="51"/>
       <c r="FH14" s="51"/>
       <c r="FI14" s="53"/>
@@ -19598,7 +19344,7 @@
       <c r="D15" s="51"/>
       <c r="E15" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F15" s="51"/>
       <c r="G15" s="51"/>
@@ -19801,9 +19547,7 @@
       <c r="FC15" s="51"/>
       <c r="FD15" s="51"/>
       <c r="FE15" s="51"/>
-      <c r="FF15" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF15" s="51"/>
       <c r="FG15" s="51"/>
       <c r="FH15" s="51"/>
       <c r="FI15" s="53"/>
@@ -19833,7 +19577,7 @@
       <c r="D16" s="51"/>
       <c r="E16" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F16" s="51"/>
       <c r="G16" s="51"/>
@@ -20020,9 +19764,7 @@
       </c>
       <c r="FD16" s="51"/>
       <c r="FE16" s="51"/>
-      <c r="FF16" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF16" s="51"/>
       <c r="FG16" s="51" t="s">
         <v>197</v>
       </c>
@@ -20060,7 +19802,7 @@
       <c r="D17" s="51"/>
       <c r="E17" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F17" s="51"/>
       <c r="G17" s="51"/>
@@ -20247,9 +19989,7 @@
       </c>
       <c r="FD17" s="51"/>
       <c r="FE17" s="51"/>
-      <c r="FF17" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF17" s="51"/>
       <c r="FG17" s="51" t="s">
         <v>197</v>
       </c>
@@ -20287,7 +20027,7 @@
       <c r="D18" s="51"/>
       <c r="E18" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F18" s="51"/>
       <c r="G18" s="51"/>
@@ -20447,9 +20187,7 @@
       </c>
       <c r="FD18" s="51"/>
       <c r="FE18" s="51"/>
-      <c r="FF18" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF18" s="51"/>
       <c r="FG18" s="51"/>
       <c r="FH18" s="51" t="s">
         <v>186</v>
@@ -20481,7 +20219,7 @@
       <c r="D19" s="51"/>
       <c r="E19" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F19" s="51"/>
       <c r="G19" s="51"/>
@@ -20640,9 +20378,7 @@
       <c r="FC19" s="51"/>
       <c r="FD19" s="51"/>
       <c r="FE19" s="51"/>
-      <c r="FF19" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF19" s="51"/>
       <c r="FG19" s="51"/>
       <c r="FH19" s="51"/>
       <c r="FI19" s="53"/>
@@ -20672,7 +20408,7 @@
       <c r="D20" s="51"/>
       <c r="E20" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F20" s="51"/>
       <c r="G20" s="51"/>
@@ -20831,9 +20567,7 @@
       <c r="FC20" s="51"/>
       <c r="FD20" s="51"/>
       <c r="FE20" s="51"/>
-      <c r="FF20" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF20" s="51"/>
       <c r="FG20" s="51"/>
       <c r="FH20" s="51"/>
       <c r="FI20" s="53"/>
@@ -20863,7 +20597,7 @@
       <c r="D21" s="51"/>
       <c r="E21" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F21" s="51"/>
       <c r="G21" s="51"/>
@@ -21024,9 +20758,7 @@
       <c r="FC21" s="51"/>
       <c r="FD21" s="51"/>
       <c r="FE21" s="51"/>
-      <c r="FF21" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF21" s="51"/>
       <c r="FG21" s="51"/>
       <c r="FH21" s="51"/>
       <c r="FI21" s="53"/>
@@ -21056,7 +20788,7 @@
       <c r="D22" s="51"/>
       <c r="E22" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F22" s="51"/>
       <c r="G22" s="51"/>
@@ -21215,9 +20947,7 @@
       <c r="FC22" s="51"/>
       <c r="FD22" s="51"/>
       <c r="FE22" s="51"/>
-      <c r="FF22" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF22" s="51"/>
       <c r="FG22" s="51"/>
       <c r="FH22" s="51"/>
       <c r="FI22" s="53"/>
@@ -21247,7 +20977,7 @@
       <c r="D23" s="51"/>
       <c r="E23" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F23" s="51"/>
       <c r="G23" s="51"/>
@@ -21442,9 +21172,7 @@
         <v>197</v>
       </c>
       <c r="FE23" s="51"/>
-      <c r="FF23" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF23" s="51"/>
       <c r="FG23" s="51"/>
       <c r="FH23" s="51" t="s">
         <v>186</v>
@@ -21476,7 +21204,7 @@
       <c r="D24" s="51"/>
       <c r="E24" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F24" s="51"/>
       <c r="G24" s="51"/>
@@ -21655,9 +21383,7 @@
       </c>
       <c r="FD24" s="51"/>
       <c r="FE24" s="51"/>
-      <c r="FF24" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF24" s="51"/>
       <c r="FG24" s="51"/>
       <c r="FH24" s="51" t="s">
         <v>186</v>
@@ -21691,7 +21417,7 @@
       <c r="D25" s="51"/>
       <c r="E25" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F25" s="51"/>
       <c r="G25" s="51"/>
@@ -21870,9 +21596,7 @@
       </c>
       <c r="FD25" s="51"/>
       <c r="FE25" s="51"/>
-      <c r="FF25" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF25" s="51"/>
       <c r="FG25" s="51"/>
       <c r="FH25" s="51" t="s">
         <v>186</v>
@@ -21906,7 +21630,7 @@
       <c r="D26" s="51"/>
       <c r="E26" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F26" s="51"/>
       <c r="G26" s="51"/>
@@ -22123,9 +21847,7 @@
       </c>
       <c r="FD26" s="51"/>
       <c r="FE26" s="51"/>
-      <c r="FF26" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF26" s="51"/>
       <c r="FG26" s="51" t="s">
         <v>197</v>
       </c>
@@ -22165,7 +21887,7 @@
       <c r="D27" s="51"/>
       <c r="E27" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F27" s="51"/>
       <c r="G27" s="51"/>
@@ -22382,9 +22104,7 @@
       </c>
       <c r="FD27" s="51"/>
       <c r="FE27" s="51"/>
-      <c r="FF27" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF27" s="51"/>
       <c r="FG27" s="51" t="s">
         <v>197</v>
       </c>
@@ -22424,7 +22144,7 @@
       <c r="D28" s="51"/>
       <c r="E28" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F28" s="51"/>
       <c r="G28" s="51"/>
@@ -22623,9 +22343,7 @@
       </c>
       <c r="FD28" s="51"/>
       <c r="FE28" s="51"/>
-      <c r="FF28" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF28" s="51"/>
       <c r="FG28" s="51" t="s">
         <v>197</v>
       </c>
@@ -22665,7 +22383,7 @@
       <c r="D29" s="51"/>
       <c r="E29" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F29" s="51"/>
       <c r="G29" s="51"/>
@@ -22870,9 +22588,7 @@
       <c r="FC29" s="51"/>
       <c r="FD29" s="51"/>
       <c r="FE29" s="51"/>
-      <c r="FF29" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF29" s="51"/>
       <c r="FG29" s="51"/>
       <c r="FH29" s="51"/>
       <c r="FI29" s="53"/>
@@ -22902,7 +22618,7 @@
       <c r="D30" s="51"/>
       <c r="E30" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F30" s="51"/>
       <c r="G30" s="51"/>
@@ -23111,9 +22827,7 @@
       <c r="FC30" s="51"/>
       <c r="FD30" s="51"/>
       <c r="FE30" s="51"/>
-      <c r="FF30" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF30" s="51"/>
       <c r="FG30" s="51"/>
       <c r="FH30" s="51"/>
       <c r="FI30" s="53"/>
@@ -23143,7 +22857,7 @@
       <c r="D31" s="51"/>
       <c r="E31" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F31" s="51"/>
       <c r="G31" s="51"/>
@@ -23348,9 +23062,7 @@
       <c r="FC31" s="51"/>
       <c r="FD31" s="51"/>
       <c r="FE31" s="51"/>
-      <c r="FF31" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF31" s="51"/>
       <c r="FG31" s="51"/>
       <c r="FH31" s="51"/>
       <c r="FI31" s="53"/>
@@ -23382,7 +23094,7 @@
       </c>
       <c r="E32" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F32" s="51"/>
       <c r="G32" s="51"/>
@@ -23559,9 +23271,7 @@
       <c r="FC32" s="51"/>
       <c r="FD32" s="51"/>
       <c r="FE32" s="51"/>
-      <c r="FF32" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF32" s="51"/>
       <c r="FG32" s="51"/>
       <c r="FH32" s="51"/>
       <c r="FI32" s="53"/>
@@ -23593,7 +23303,7 @@
       <c r="D33" s="51"/>
       <c r="E33" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F33" s="51"/>
       <c r="G33" s="51"/>
@@ -23768,9 +23478,7 @@
       <c r="FC33" s="51"/>
       <c r="FD33" s="51"/>
       <c r="FE33" s="51"/>
-      <c r="FF33" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF33" s="51"/>
       <c r="FG33" s="51"/>
       <c r="FH33" s="51"/>
       <c r="FI33" s="53"/>
@@ -23802,7 +23510,7 @@
       <c r="D34" s="51"/>
       <c r="E34" s="52">
         <f t="shared" ref="E34:E65" ca="1" si="1">TODAY()</f>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F34" s="51"/>
       <c r="G34" s="51"/>
@@ -24017,9 +23725,7 @@
       </c>
       <c r="FD34" s="51"/>
       <c r="FE34" s="51"/>
-      <c r="FF34" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF34" s="51"/>
       <c r="FG34" s="51" t="s">
         <v>197</v>
       </c>
@@ -24059,7 +23765,7 @@
       <c r="D35" s="51"/>
       <c r="E35" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F35" s="51"/>
       <c r="G35" s="51"/>
@@ -24284,9 +23990,7 @@
       </c>
       <c r="FD35" s="51"/>
       <c r="FE35" s="51"/>
-      <c r="FF35" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF35" s="51"/>
       <c r="FG35" s="51" t="s">
         <v>197</v>
       </c>
@@ -24326,7 +24030,7 @@
       <c r="D36" s="51"/>
       <c r="E36" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F36" s="51"/>
       <c r="G36" s="51"/>
@@ -24551,9 +24255,7 @@
       </c>
       <c r="FD36" s="51"/>
       <c r="FE36" s="51"/>
-      <c r="FF36" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF36" s="51"/>
       <c r="FG36" s="51" t="s">
         <v>197</v>
       </c>
@@ -24593,7 +24295,7 @@
       <c r="D37" s="51"/>
       <c r="E37" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F37" s="51"/>
       <c r="G37" s="51"/>
@@ -24852,9 +24554,7 @@
       </c>
       <c r="FD37" s="51"/>
       <c r="FE37" s="51"/>
-      <c r="FF37" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF37" s="51"/>
       <c r="FG37" s="51" t="s">
         <v>197</v>
       </c>
@@ -24894,7 +24594,7 @@
       <c r="D38" s="51"/>
       <c r="E38" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F38" s="51"/>
       <c r="G38" s="51"/>
@@ -25073,9 +24773,7 @@
       <c r="FC38" s="51"/>
       <c r="FD38" s="51"/>
       <c r="FE38" s="51"/>
-      <c r="FF38" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF38" s="51"/>
       <c r="FG38" s="51"/>
       <c r="FH38" s="51"/>
       <c r="FI38" s="53"/>
@@ -25105,7 +24803,7 @@
       <c r="D39" s="51"/>
       <c r="E39" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F39" s="51"/>
       <c r="G39" s="51"/>
@@ -25314,9 +25012,7 @@
       <c r="FC39" s="51"/>
       <c r="FD39" s="51"/>
       <c r="FE39" s="51"/>
-      <c r="FF39" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF39" s="51"/>
       <c r="FG39" s="51" t="s">
         <v>197</v>
       </c>
@@ -25352,7 +25048,7 @@
       <c r="D40" s="51"/>
       <c r="E40" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F40" s="51"/>
       <c r="G40" s="51"/>
@@ -25533,9 +25229,7 @@
       <c r="FC40" s="51"/>
       <c r="FD40" s="51"/>
       <c r="FE40" s="51"/>
-      <c r="FF40" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF40" s="51"/>
       <c r="FG40" s="51"/>
       <c r="FH40" s="51"/>
       <c r="FI40" s="53"/>
@@ -25565,7 +25259,7 @@
       <c r="D41" s="51"/>
       <c r="E41" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F41" s="51"/>
       <c r="G41" s="51"/>
@@ -25740,9 +25434,7 @@
       </c>
       <c r="FD41" s="51"/>
       <c r="FE41" s="51"/>
-      <c r="FF41" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF41" s="51"/>
       <c r="FG41" s="51"/>
       <c r="FH41" s="51" t="s">
         <v>186</v>
@@ -25774,7 +25466,7 @@
       <c r="D42" s="51"/>
       <c r="E42" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F42" s="51"/>
       <c r="G42" s="51"/>
@@ -25963,9 +25655,7 @@
       </c>
       <c r="FD42" s="51"/>
       <c r="FE42" s="51"/>
-      <c r="FF42" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF42" s="51"/>
       <c r="FG42" s="51"/>
       <c r="FH42" s="51" t="s">
         <v>186</v>
@@ -25997,7 +25687,7 @@
       <c r="D43" s="51"/>
       <c r="E43" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F43" s="51"/>
       <c r="G43" s="51"/>
@@ -26226,9 +25916,7 @@
       <c r="FC43" s="51"/>
       <c r="FD43" s="51"/>
       <c r="FE43" s="51"/>
-      <c r="FF43" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF43" s="51"/>
       <c r="FG43" s="51" t="s">
         <v>197</v>
       </c>
@@ -26264,7 +25952,7 @@
       <c r="D44" s="51"/>
       <c r="E44" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F44" s="51"/>
       <c r="G44" s="51"/>
@@ -26493,9 +26181,7 @@
       <c r="FC44" s="51"/>
       <c r="FD44" s="51"/>
       <c r="FE44" s="51"/>
-      <c r="FF44" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF44" s="51"/>
       <c r="FG44" s="51" t="s">
         <v>197</v>
       </c>
@@ -26531,7 +26217,7 @@
       <c r="D45" s="51"/>
       <c r="E45" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F45" s="51"/>
       <c r="G45" s="51"/>
@@ -26760,9 +26446,7 @@
       <c r="FC45" s="51"/>
       <c r="FD45" s="51"/>
       <c r="FE45" s="51"/>
-      <c r="FF45" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF45" s="51"/>
       <c r="FG45" s="51" t="s">
         <v>197</v>
       </c>
@@ -26800,7 +26484,7 @@
       </c>
       <c r="E46" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F46" s="51"/>
       <c r="G46" s="51"/>
@@ -26979,9 +26663,7 @@
       <c r="FC46" s="51"/>
       <c r="FD46" s="51"/>
       <c r="FE46" s="51"/>
-      <c r="FF46" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF46" s="51"/>
       <c r="FG46" s="51"/>
       <c r="FH46" s="51"/>
       <c r="FI46" s="53"/>
@@ -27015,7 +26697,7 @@
       </c>
       <c r="E47" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F47" s="51"/>
       <c r="G47" s="51"/>
@@ -27194,9 +26876,7 @@
       <c r="FC47" s="51"/>
       <c r="FD47" s="51"/>
       <c r="FE47" s="51"/>
-      <c r="FF47" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF47" s="51"/>
       <c r="FG47" s="51"/>
       <c r="FH47" s="51"/>
       <c r="FI47" s="53"/>
@@ -27230,7 +26910,7 @@
       </c>
       <c r="E48" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F48" s="51"/>
       <c r="G48" s="51"/>
@@ -27407,9 +27087,7 @@
       <c r="FC48" s="51"/>
       <c r="FD48" s="51"/>
       <c r="FE48" s="51"/>
-      <c r="FF48" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF48" s="51"/>
       <c r="FG48" s="51"/>
       <c r="FH48" s="51"/>
       <c r="FI48" s="53"/>
@@ -27443,7 +27121,7 @@
       </c>
       <c r="E49" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F49" s="51"/>
       <c r="G49" s="51"/>
@@ -27620,9 +27298,7 @@
       <c r="FC49" s="51"/>
       <c r="FD49" s="51"/>
       <c r="FE49" s="51"/>
-      <c r="FF49" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF49" s="51"/>
       <c r="FG49" s="51"/>
       <c r="FH49" s="51"/>
       <c r="FI49" s="53"/>
@@ -27654,7 +27330,7 @@
       <c r="D50" s="51"/>
       <c r="E50" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F50" s="51"/>
       <c r="G50" s="51"/>
@@ -27813,9 +27489,7 @@
       <c r="FC50" s="51"/>
       <c r="FD50" s="51"/>
       <c r="FE50" s="51"/>
-      <c r="FF50" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF50" s="51"/>
       <c r="FG50" s="51"/>
       <c r="FH50" s="51"/>
       <c r="FI50" s="53"/>
@@ -27847,7 +27521,7 @@
       <c r="D51" s="51"/>
       <c r="E51" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F51" s="51"/>
       <c r="G51" s="51"/>
@@ -28010,9 +27684,7 @@
       <c r="FC51" s="51"/>
       <c r="FD51" s="51"/>
       <c r="FE51" s="51"/>
-      <c r="FF51" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF51" s="51"/>
       <c r="FG51" s="51"/>
       <c r="FH51" s="51"/>
       <c r="FI51" s="53"/>
@@ -28046,7 +27718,7 @@
       <c r="D52" s="51"/>
       <c r="E52" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F52" s="51"/>
       <c r="G52" s="51"/>
@@ -28209,9 +27881,7 @@
       <c r="FC52" s="51"/>
       <c r="FD52" s="51"/>
       <c r="FE52" s="51"/>
-      <c r="FF52" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF52" s="51"/>
       <c r="FG52" s="51"/>
       <c r="FH52" s="51"/>
       <c r="FI52" s="53"/>
@@ -28241,7 +27911,7 @@
       <c r="D53" s="51"/>
       <c r="E53" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F53" s="51"/>
       <c r="G53" s="51"/>
@@ -28415,9 +28085,7 @@
       <c r="FC53" s="51"/>
       <c r="FD53" s="51"/>
       <c r="FE53" s="51"/>
-      <c r="FF53" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF53" s="51"/>
       <c r="FG53" s="51"/>
       <c r="FH53" s="51"/>
       <c r="FI53" s="53"/>
@@ -28449,7 +28117,7 @@
       <c r="D54" s="51"/>
       <c r="E54" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F54" s="51"/>
       <c r="G54" s="51"/>
@@ -28622,9 +28290,7 @@
       <c r="FC54" s="51"/>
       <c r="FD54" s="51"/>
       <c r="FE54" s="51"/>
-      <c r="FF54" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF54" s="51"/>
       <c r="FG54" s="51"/>
       <c r="FH54" s="51"/>
       <c r="FI54" s="53"/>
@@ -28656,7 +28322,7 @@
       <c r="D55" s="51"/>
       <c r="E55" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F55" s="51"/>
       <c r="G55" s="51"/>
@@ -28859,9 +28525,7 @@
       <c r="FC55" s="51"/>
       <c r="FD55" s="51"/>
       <c r="FE55" s="51"/>
-      <c r="FF55" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF55" s="51"/>
       <c r="FG55" s="51" t="s">
         <v>197</v>
       </c>
@@ -28899,7 +28563,7 @@
       <c r="D56" s="51"/>
       <c r="E56" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F56" s="51"/>
       <c r="G56" s="51"/>
@@ -29074,9 +28738,7 @@
       <c r="FC56" s="51"/>
       <c r="FD56" s="51"/>
       <c r="FE56" s="51"/>
-      <c r="FF56" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF56" s="51"/>
       <c r="FG56" s="51"/>
       <c r="FH56" s="51"/>
       <c r="FI56" s="53"/>
@@ -29106,7 +28768,7 @@
       <c r="D57" s="51"/>
       <c r="E57" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F57" s="51"/>
       <c r="G57" s="51"/>
@@ -29270,9 +28932,7 @@
       <c r="FC57" s="51"/>
       <c r="FD57" s="51"/>
       <c r="FE57" s="51"/>
-      <c r="FF57" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF57" s="51"/>
       <c r="FG57" s="51"/>
       <c r="FH57" s="51"/>
       <c r="FI57" s="53"/>
@@ -29302,7 +28962,7 @@
       <c r="D58" s="51"/>
       <c r="E58" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F58" s="51"/>
       <c r="G58" s="51"/>
@@ -29472,9 +29132,7 @@
       <c r="FC58" s="51"/>
       <c r="FD58" s="51"/>
       <c r="FE58" s="51"/>
-      <c r="FF58" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF58" s="51"/>
       <c r="FG58" s="51"/>
       <c r="FH58" s="51"/>
       <c r="FI58" s="53"/>
@@ -29504,7 +29162,7 @@
       <c r="D59" s="51"/>
       <c r="E59" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F59" s="51"/>
       <c r="G59" s="51"/>
@@ -29676,9 +29334,7 @@
       <c r="FC59" s="51"/>
       <c r="FD59" s="51"/>
       <c r="FE59" s="51"/>
-      <c r="FF59" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF59" s="51"/>
       <c r="FG59" s="51"/>
       <c r="FH59" s="51"/>
       <c r="FI59" s="53"/>
@@ -29708,7 +29364,7 @@
       <c r="D60" s="51"/>
       <c r="E60" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F60" s="51"/>
       <c r="G60" s="51"/>
@@ -29875,9 +29531,7 @@
       </c>
       <c r="FD60" s="51"/>
       <c r="FE60" s="51"/>
-      <c r="FF60" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF60" s="51"/>
       <c r="FG60" s="51"/>
       <c r="FH60" s="51"/>
       <c r="FI60" s="53"/>
@@ -29907,7 +29561,7 @@
       <c r="D61" s="51"/>
       <c r="E61" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F61" s="51"/>
       <c r="G61" s="51"/>
@@ -30104,9 +29758,7 @@
       </c>
       <c r="FD61" s="51"/>
       <c r="FE61" s="51"/>
-      <c r="FF61" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF61" s="51"/>
       <c r="FG61" s="51" t="s">
         <v>197</v>
       </c>
@@ -30142,7 +29794,7 @@
       <c r="D62" s="51"/>
       <c r="E62" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F62" s="51"/>
       <c r="G62" s="51"/>
@@ -30345,9 +29997,7 @@
       <c r="FC62" s="51"/>
       <c r="FD62" s="51"/>
       <c r="FE62" s="51"/>
-      <c r="FF62" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF62" s="51"/>
       <c r="FG62" s="51"/>
       <c r="FH62" s="51"/>
       <c r="FI62" s="53"/>
@@ -30377,7 +30027,7 @@
       <c r="D63" s="51"/>
       <c r="E63" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F63" s="51"/>
       <c r="G63" s="51"/>
@@ -30584,9 +30234,7 @@
       <c r="FC63" s="51"/>
       <c r="FD63" s="51"/>
       <c r="FE63" s="51"/>
-      <c r="FF63" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF63" s="51"/>
       <c r="FG63" s="51"/>
       <c r="FH63" s="51"/>
       <c r="FI63" s="53"/>
@@ -30616,7 +30264,7 @@
       <c r="D64" s="51"/>
       <c r="E64" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F64" s="51"/>
       <c r="G64" s="51"/>
@@ -30819,9 +30467,7 @@
       <c r="FC64" s="51"/>
       <c r="FD64" s="51"/>
       <c r="FE64" s="51"/>
-      <c r="FF64" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF64" s="51"/>
       <c r="FG64" s="51"/>
       <c r="FH64" s="51"/>
       <c r="FI64" s="53"/>
@@ -30851,7 +30497,7 @@
       <c r="D65" s="51"/>
       <c r="E65" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F65" s="51"/>
       <c r="G65" s="51"/>
@@ -31062,9 +30708,7 @@
       </c>
       <c r="FD65" s="51"/>
       <c r="FE65" s="51"/>
-      <c r="FF65" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF65" s="51"/>
       <c r="FG65" s="51" t="s">
         <v>197</v>
       </c>
@@ -31102,7 +30746,7 @@
       <c r="D66" s="51"/>
       <c r="E66" s="52">
         <f t="shared" ref="E66:E89" ca="1" si="2">TODAY()</f>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F66" s="51"/>
       <c r="G66" s="51"/>
@@ -31315,9 +30959,7 @@
       </c>
       <c r="FD66" s="51"/>
       <c r="FE66" s="51"/>
-      <c r="FF66" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF66" s="51"/>
       <c r="FG66" s="51" t="s">
         <v>197</v>
       </c>
@@ -31357,7 +30999,7 @@
       <c r="D67" s="51"/>
       <c r="E67" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F67" s="51"/>
       <c r="G67" s="51"/>
@@ -31562,9 +31204,7 @@
       <c r="FC67" s="51"/>
       <c r="FD67" s="51"/>
       <c r="FE67" s="51"/>
-      <c r="FF67" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF67" s="51"/>
       <c r="FG67" s="51"/>
       <c r="FH67" s="51"/>
       <c r="FI67" s="53"/>
@@ -31596,7 +31236,7 @@
       <c r="D68" s="51"/>
       <c r="E68" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F68" s="51"/>
       <c r="G68" s="51"/>
@@ -31803,9 +31443,7 @@
       <c r="FC68" s="51"/>
       <c r="FD68" s="51"/>
       <c r="FE68" s="51"/>
-      <c r="FF68" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF68" s="51"/>
       <c r="FG68" s="51"/>
       <c r="FH68" s="51"/>
       <c r="FI68" s="53"/>
@@ -31837,7 +31475,7 @@
       <c r="D69" s="51"/>
       <c r="E69" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F69" s="51"/>
       <c r="G69" s="51"/>
@@ -32044,9 +31682,7 @@
       <c r="FC69" s="51"/>
       <c r="FD69" s="51"/>
       <c r="FE69" s="51"/>
-      <c r="FF69" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF69" s="51"/>
       <c r="FG69" s="51"/>
       <c r="FH69" s="51"/>
       <c r="FI69" s="53"/>
@@ -32078,7 +31714,7 @@
       <c r="D70" s="51"/>
       <c r="E70" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F70" s="51"/>
       <c r="G70" s="51"/>
@@ -32287,9 +31923,7 @@
       <c r="FC70" s="51"/>
       <c r="FD70" s="51"/>
       <c r="FE70" s="51"/>
-      <c r="FF70" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF70" s="51"/>
       <c r="FG70" s="51"/>
       <c r="FH70" s="51"/>
       <c r="FI70" s="53"/>
@@ -32321,7 +31955,7 @@
       <c r="D71" s="51"/>
       <c r="E71" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F71" s="51"/>
       <c r="G71" s="51"/>
@@ -32528,9 +32162,7 @@
       <c r="FC71" s="51"/>
       <c r="FD71" s="51"/>
       <c r="FE71" s="51"/>
-      <c r="FF71" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF71" s="51"/>
       <c r="FG71" s="51"/>
       <c r="FH71" s="51"/>
       <c r="FI71" s="53"/>
@@ -32560,7 +32192,7 @@
       <c r="D72" s="51"/>
       <c r="E72" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F72" s="51"/>
       <c r="G72" s="51"/>
@@ -32719,9 +32351,7 @@
       <c r="FC72" s="51"/>
       <c r="FD72" s="51"/>
       <c r="FE72" s="51"/>
-      <c r="FF72" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF72" s="51"/>
       <c r="FG72" s="51"/>
       <c r="FH72" s="51"/>
       <c r="FI72" s="53"/>
@@ -32751,7 +32381,7 @@
       <c r="D73" s="51"/>
       <c r="E73" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F73" s="51"/>
       <c r="G73" s="51"/>
@@ -32910,9 +32540,7 @@
       <c r="FC73" s="51"/>
       <c r="FD73" s="51"/>
       <c r="FE73" s="51"/>
-      <c r="FF73" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF73" s="51"/>
       <c r="FG73" s="51"/>
       <c r="FH73" s="51"/>
       <c r="FI73" s="53"/>
@@ -32942,7 +32570,7 @@
       <c r="D74" s="51"/>
       <c r="E74" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F74" s="51"/>
       <c r="G74" s="51"/>
@@ -33101,9 +32729,7 @@
       <c r="FC74" s="51"/>
       <c r="FD74" s="51"/>
       <c r="FE74" s="51"/>
-      <c r="FF74" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF74" s="51"/>
       <c r="FG74" s="51"/>
       <c r="FH74" s="51"/>
       <c r="FI74" s="53"/>
@@ -33133,7 +32759,7 @@
       <c r="D75" s="51"/>
       <c r="E75" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F75" s="51"/>
       <c r="G75" s="51"/>
@@ -33344,9 +32970,7 @@
       </c>
       <c r="FD75" s="51"/>
       <c r="FE75" s="51"/>
-      <c r="FF75" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF75" s="51"/>
       <c r="FG75" s="51" t="s">
         <v>197</v>
       </c>
@@ -33384,7 +33008,7 @@
       <c r="D76" s="51"/>
       <c r="E76" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F76" s="51"/>
       <c r="G76" s="51"/>
@@ -33597,9 +33221,7 @@
       </c>
       <c r="FD76" s="51"/>
       <c r="FE76" s="51"/>
-      <c r="FF76" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF76" s="51"/>
       <c r="FG76" s="51" t="s">
         <v>197</v>
       </c>
@@ -33637,7 +33259,7 @@
       <c r="D77" s="51"/>
       <c r="E77" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F77" s="51"/>
       <c r="G77" s="51"/>
@@ -33850,9 +33472,7 @@
       </c>
       <c r="FD77" s="51"/>
       <c r="FE77" s="51"/>
-      <c r="FF77" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF77" s="51"/>
       <c r="FG77" s="51" t="s">
         <v>197</v>
       </c>
@@ -33890,7 +33510,7 @@
       <c r="D78" s="51"/>
       <c r="E78" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F78" s="51"/>
       <c r="G78" s="51"/>
@@ -34091,9 +33711,7 @@
       <c r="FC78" s="51"/>
       <c r="FD78" s="51"/>
       <c r="FE78" s="51"/>
-      <c r="FF78" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF78" s="51"/>
       <c r="FG78" s="51"/>
       <c r="FH78" s="51"/>
       <c r="FI78" s="53"/>
@@ -34123,7 +33741,7 @@
       <c r="D79" s="51"/>
       <c r="E79" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F79" s="51"/>
       <c r="G79" s="51"/>
@@ -34328,9 +33946,7 @@
       <c r="FC79" s="51"/>
       <c r="FD79" s="51"/>
       <c r="FE79" s="51"/>
-      <c r="FF79" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF79" s="51"/>
       <c r="FG79" s="51"/>
       <c r="FH79" s="51"/>
       <c r="FI79" s="53"/>
@@ -34360,7 +33976,7 @@
       <c r="D80" s="51"/>
       <c r="E80" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F80" s="51"/>
       <c r="G80" s="51"/>
@@ -34561,9 +34177,7 @@
       <c r="FC80" s="51"/>
       <c r="FD80" s="51"/>
       <c r="FE80" s="51"/>
-      <c r="FF80" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF80" s="51"/>
       <c r="FG80" s="51"/>
       <c r="FH80" s="51"/>
       <c r="FI80" s="53"/>
@@ -34593,7 +34207,7 @@
       <c r="D81" s="51"/>
       <c r="E81" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F81" s="51"/>
       <c r="G81" s="51"/>
@@ -34796,9 +34410,7 @@
       </c>
       <c r="FD81" s="51"/>
       <c r="FE81" s="51"/>
-      <c r="FF81" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF81" s="51"/>
       <c r="FG81" s="51" t="s">
         <v>197</v>
       </c>
@@ -34838,7 +34450,7 @@
       <c r="D82" s="51"/>
       <c r="E82" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F82" s="51"/>
       <c r="G82" s="51"/>
@@ -35025,9 +34637,7 @@
       </c>
       <c r="FD82" s="51"/>
       <c r="FE82" s="51"/>
-      <c r="FF82" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF82" s="51"/>
       <c r="FG82" s="51"/>
       <c r="FH82" s="51" t="s">
         <v>186</v>
@@ -35061,7 +34671,7 @@
       <c r="D83" s="51"/>
       <c r="E83" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F83" s="51"/>
       <c r="G83" s="51"/>
@@ -35270,9 +34880,7 @@
       </c>
       <c r="FD83" s="51"/>
       <c r="FE83" s="51"/>
-      <c r="FF83" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF83" s="51"/>
       <c r="FG83" s="51" t="s">
         <v>197</v>
       </c>
@@ -35312,7 +34920,7 @@
       <c r="D84" s="51"/>
       <c r="E84" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F84" s="51"/>
       <c r="G84" s="51"/>
@@ -35521,9 +35129,7 @@
       </c>
       <c r="FD84" s="51"/>
       <c r="FE84" s="51"/>
-      <c r="FF84" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF84" s="51"/>
       <c r="FG84" s="51" t="s">
         <v>197</v>
       </c>
@@ -35563,7 +35169,7 @@
       <c r="D85" s="51"/>
       <c r="E85" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F85" s="51"/>
       <c r="G85" s="51"/>
@@ -35772,9 +35378,7 @@
       </c>
       <c r="FD85" s="51"/>
       <c r="FE85" s="51"/>
-      <c r="FF85" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF85" s="51"/>
       <c r="FG85" s="51" t="s">
         <v>197</v>
       </c>
@@ -35814,7 +35418,7 @@
       <c r="D86" s="51"/>
       <c r="E86" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F86" s="51"/>
       <c r="G86" s="51"/>
@@ -36023,9 +35627,7 @@
       </c>
       <c r="FD86" s="51"/>
       <c r="FE86" s="51"/>
-      <c r="FF86" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF86" s="51"/>
       <c r="FG86" s="51" t="s">
         <v>197</v>
       </c>
@@ -36065,7 +35667,7 @@
       <c r="D87" s="51"/>
       <c r="E87" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F87" s="51"/>
       <c r="G87" s="51"/>
@@ -36226,9 +35828,7 @@
       <c r="FC87" s="51"/>
       <c r="FD87" s="51"/>
       <c r="FE87" s="51"/>
-      <c r="FF87" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF87" s="51"/>
       <c r="FG87" s="51"/>
       <c r="FH87" s="51"/>
       <c r="FI87" s="53"/>
@@ -36258,7 +35858,7 @@
       <c r="D88" s="51"/>
       <c r="E88" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F88" s="51"/>
       <c r="G88" s="51"/>
@@ -36419,9 +36019,7 @@
       <c r="FC88" s="51"/>
       <c r="FD88" s="51"/>
       <c r="FE88" s="51"/>
-      <c r="FF88" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF88" s="51"/>
       <c r="FG88" s="51"/>
       <c r="FH88" s="51"/>
       <c r="FI88" s="53"/>
@@ -36451,7 +36049,7 @@
       <c r="D89" s="51"/>
       <c r="E89" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F89" s="51"/>
       <c r="G89" s="51"/>
@@ -36612,9 +36210,7 @@
       <c r="FC89" s="51"/>
       <c r="FD89" s="51"/>
       <c r="FE89" s="51"/>
-      <c r="FF89" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF89" s="51"/>
       <c r="FG89" s="51"/>
       <c r="FH89" s="51"/>
       <c r="FI89" s="53"/>
@@ -36828,7 +36424,7 @@
       <c r="D91" s="51"/>
       <c r="E91" s="52">
         <f ca="1">TODAY()</f>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F91" s="51"/>
       <c r="G91" s="51"/>
@@ -36987,9 +36583,7 @@
       <c r="FC91" s="51"/>
       <c r="FD91" s="51"/>
       <c r="FE91" s="51"/>
-      <c r="FF91" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF91" s="51"/>
       <c r="FG91" s="51"/>
       <c r="FH91" s="51"/>
       <c r="FI91" s="53"/>
@@ -37205,7 +36799,7 @@
       <c r="D93" s="51"/>
       <c r="E93" s="52">
         <f t="shared" ref="E93:E118" ca="1" si="3">TODAY()</f>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F93" s="51"/>
       <c r="G93" s="51"/>
@@ -37388,9 +36982,7 @@
       <c r="FC93" s="51"/>
       <c r="FD93" s="51"/>
       <c r="FE93" s="51"/>
-      <c r="FF93" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF93" s="51"/>
       <c r="FG93" s="51"/>
       <c r="FH93" s="51"/>
       <c r="FI93" s="53"/>
@@ -37424,7 +37016,7 @@
       <c r="D94" s="51"/>
       <c r="E94" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F94" s="51"/>
       <c r="G94" s="51"/>
@@ -37607,9 +37199,7 @@
       <c r="FC94" s="51"/>
       <c r="FD94" s="51"/>
       <c r="FE94" s="51"/>
-      <c r="FF94" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF94" s="51"/>
       <c r="FG94" s="51"/>
       <c r="FH94" s="51"/>
       <c r="FI94" s="53"/>
@@ -37643,7 +37233,7 @@
       <c r="D95" s="51"/>
       <c r="E95" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F95" s="51"/>
       <c r="G95" s="51"/>
@@ -37824,9 +37414,7 @@
       <c r="FC95" s="51"/>
       <c r="FD95" s="51"/>
       <c r="FE95" s="51"/>
-      <c r="FF95" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF95" s="51"/>
       <c r="FG95" s="51"/>
       <c r="FH95" s="51"/>
       <c r="FI95" s="53"/>
@@ -37860,7 +37448,7 @@
       <c r="D96" s="51"/>
       <c r="E96" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F96" s="51"/>
       <c r="G96" s="51"/>
@@ -38041,9 +37629,7 @@
       <c r="FC96" s="51"/>
       <c r="FD96" s="51"/>
       <c r="FE96" s="51"/>
-      <c r="FF96" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF96" s="51"/>
       <c r="FG96" s="51"/>
       <c r="FH96" s="51"/>
       <c r="FI96" s="53"/>
@@ -38075,7 +37661,7 @@
       <c r="D97" s="51"/>
       <c r="E97" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F97" s="51"/>
       <c r="G97" s="51"/>
@@ -38245,9 +37831,7 @@
       <c r="FC97" s="51"/>
       <c r="FD97" s="51"/>
       <c r="FE97" s="51"/>
-      <c r="FF97" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF97" s="51"/>
       <c r="FG97" s="51"/>
       <c r="FH97" s="51"/>
       <c r="FI97" s="53"/>
@@ -38277,7 +37861,7 @@
       <c r="D98" s="51"/>
       <c r="E98" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F98" s="51"/>
       <c r="G98" s="51"/>
@@ -38447,9 +38031,7 @@
       <c r="FC98" s="51"/>
       <c r="FD98" s="51"/>
       <c r="FE98" s="51"/>
-      <c r="FF98" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF98" s="51"/>
       <c r="FG98" s="51"/>
       <c r="FH98" s="51"/>
       <c r="FI98" s="53"/>
@@ -38479,7 +38061,7 @@
       <c r="D99" s="51"/>
       <c r="E99" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F99" s="51"/>
       <c r="G99" s="51"/>
@@ -38651,9 +38233,7 @@
       <c r="FC99" s="51"/>
       <c r="FD99" s="51"/>
       <c r="FE99" s="51"/>
-      <c r="FF99" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF99" s="51"/>
       <c r="FG99" s="51"/>
       <c r="FH99" s="51"/>
       <c r="FI99" s="53"/>
@@ -38683,7 +38263,7 @@
       <c r="D100" s="51"/>
       <c r="E100" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F100" s="51"/>
       <c r="G100" s="51"/>
@@ -38855,9 +38435,7 @@
       <c r="FC100" s="51"/>
       <c r="FD100" s="51"/>
       <c r="FE100" s="51"/>
-      <c r="FF100" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF100" s="51"/>
       <c r="FG100" s="51"/>
       <c r="FH100" s="51"/>
       <c r="FI100" s="53"/>
@@ -38887,7 +38465,7 @@
       <c r="D101" s="51"/>
       <c r="E101" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F101" s="51"/>
       <c r="G101" s="51"/>
@@ -39059,9 +38637,7 @@
       <c r="FC101" s="51"/>
       <c r="FD101" s="51"/>
       <c r="FE101" s="51"/>
-      <c r="FF101" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF101" s="51"/>
       <c r="FG101" s="51"/>
       <c r="FH101" s="51"/>
       <c r="FI101" s="53"/>
@@ -39091,7 +38667,7 @@
       <c r="D102" s="51"/>
       <c r="E102" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F102" s="51"/>
       <c r="G102" s="51"/>
@@ -39263,9 +38839,7 @@
       <c r="FC102" s="51"/>
       <c r="FD102" s="51"/>
       <c r="FE102" s="51"/>
-      <c r="FF102" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF102" s="51"/>
       <c r="FG102" s="51"/>
       <c r="FH102" s="51"/>
       <c r="FI102" s="53"/>
@@ -39295,7 +38869,7 @@
       <c r="D103" s="51"/>
       <c r="E103" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F103" s="51"/>
       <c r="G103" s="51"/>
@@ -39464,9 +39038,7 @@
       <c r="FC103" s="51"/>
       <c r="FD103" s="51"/>
       <c r="FE103" s="51"/>
-      <c r="FF103" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF103" s="51"/>
       <c r="FG103" s="51"/>
       <c r="FH103" s="51" t="s">
         <v>186</v>
@@ -39498,7 +39070,7 @@
       <c r="D104" s="51"/>
       <c r="E104" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F104" s="51"/>
       <c r="G104" s="51"/>
@@ -39681,9 +39253,7 @@
       <c r="FE104" s="51" t="s">
         <v>197</v>
       </c>
-      <c r="FF104" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF104" s="51"/>
       <c r="FG104" s="51"/>
       <c r="FH104" s="51" t="s">
         <v>186</v>
@@ -39717,7 +39287,7 @@
       <c r="D105" s="51"/>
       <c r="E105" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F105" s="51"/>
       <c r="G105" s="51"/>
@@ -39900,9 +39470,7 @@
       <c r="FE105" s="51" t="s">
         <v>197</v>
       </c>
-      <c r="FF105" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF105" s="51"/>
       <c r="FG105" s="51"/>
       <c r="FH105" s="51" t="s">
         <v>186</v>
@@ -39936,7 +39504,7 @@
       <c r="D106" s="51"/>
       <c r="E106" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F106" s="51"/>
       <c r="G106" s="51"/>
@@ -40119,9 +39687,7 @@
       <c r="FE106" s="51" t="s">
         <v>197</v>
       </c>
-      <c r="FF106" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF106" s="51"/>
       <c r="FG106" s="51"/>
       <c r="FH106" s="51" t="s">
         <v>186</v>
@@ -40155,7 +39721,7 @@
       <c r="D107" s="51"/>
       <c r="E107" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F107" s="51"/>
       <c r="G107" s="51"/>
@@ -40338,9 +39904,7 @@
       <c r="FE107" s="51" t="s">
         <v>197</v>
       </c>
-      <c r="FF107" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF107" s="51"/>
       <c r="FG107" s="51"/>
       <c r="FH107" s="51" t="s">
         <v>186</v>
@@ -40374,7 +39938,7 @@
       <c r="D108" s="51"/>
       <c r="E108" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F108" s="51"/>
       <c r="G108" s="51"/>
@@ -40557,9 +40121,7 @@
       <c r="FE108" s="51" t="s">
         <v>197</v>
       </c>
-      <c r="FF108" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF108" s="51"/>
       <c r="FG108" s="51"/>
       <c r="FH108" s="51" t="s">
         <v>186</v>
@@ -40593,7 +40155,7 @@
       <c r="D109" s="51"/>
       <c r="E109" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F109" s="51"/>
       <c r="G109" s="51"/>
@@ -40776,9 +40338,7 @@
       <c r="FE109" s="51" t="s">
         <v>197</v>
       </c>
-      <c r="FF109" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF109" s="51"/>
       <c r="FG109" s="51"/>
       <c r="FH109" s="51" t="s">
         <v>186</v>
@@ -40812,7 +40372,7 @@
       <c r="D110" s="51"/>
       <c r="E110" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F110" s="51"/>
       <c r="G110" s="51"/>
@@ -40995,9 +40555,7 @@
       <c r="FE110" s="51" t="s">
         <v>197</v>
       </c>
-      <c r="FF110" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF110" s="51"/>
       <c r="FG110" s="51"/>
       <c r="FH110" s="51" t="s">
         <v>186</v>
@@ -41031,7 +40589,7 @@
       <c r="D111" s="51"/>
       <c r="E111" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F111" s="51"/>
       <c r="G111" s="51"/>
@@ -41214,9 +40772,7 @@
       <c r="FE111" s="51" t="s">
         <v>197</v>
       </c>
-      <c r="FF111" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF111" s="51"/>
       <c r="FG111" s="51"/>
       <c r="FH111" s="51" t="s">
         <v>186</v>
@@ -41250,7 +40806,7 @@
       <c r="D112" s="51"/>
       <c r="E112" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F112" s="51"/>
       <c r="G112" s="51"/>
@@ -41433,9 +40989,7 @@
       <c r="FE112" s="51" t="s">
         <v>197</v>
       </c>
-      <c r="FF112" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF112" s="51"/>
       <c r="FG112" s="51"/>
       <c r="FH112" s="51" t="s">
         <v>186</v>
@@ -41469,7 +41023,7 @@
       <c r="D113" s="51"/>
       <c r="E113" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F113" s="51"/>
       <c r="G113" s="51"/>
@@ -41652,9 +41206,7 @@
       <c r="FE113" s="51" t="s">
         <v>197</v>
       </c>
-      <c r="FF113" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF113" s="51"/>
       <c r="FG113" s="51"/>
       <c r="FH113" s="51" t="s">
         <v>186</v>
@@ -41688,7 +41240,7 @@
       <c r="D114" s="51"/>
       <c r="E114" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F114" s="51"/>
       <c r="G114" s="51"/>
@@ -41847,9 +41399,7 @@
       <c r="FC114" s="51"/>
       <c r="FD114" s="51"/>
       <c r="FE114" s="51"/>
-      <c r="FF114" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF114" s="51"/>
       <c r="FG114" s="51"/>
       <c r="FH114" s="51"/>
       <c r="FI114" s="53"/>
@@ -41879,7 +41429,7 @@
       <c r="D115" s="51"/>
       <c r="E115" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F115" s="51"/>
       <c r="G115" s="51"/>
@@ -42038,9 +41588,7 @@
       <c r="FC115" s="51"/>
       <c r="FD115" s="51"/>
       <c r="FE115" s="51"/>
-      <c r="FF115" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF115" s="51"/>
       <c r="FG115" s="51"/>
       <c r="FH115" s="51"/>
       <c r="FI115" s="53"/>
@@ -42070,7 +41618,7 @@
       <c r="D116" s="51"/>
       <c r="E116" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F116" s="51"/>
       <c r="G116" s="51"/>
@@ -42229,9 +41777,7 @@
       <c r="FC116" s="51"/>
       <c r="FD116" s="51"/>
       <c r="FE116" s="51"/>
-      <c r="FF116" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF116" s="51"/>
       <c r="FG116" s="51"/>
       <c r="FH116" s="51"/>
       <c r="FI116" s="53"/>
@@ -42261,7 +41807,7 @@
       <c r="D117" s="51"/>
       <c r="E117" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F117" s="51"/>
       <c r="G117" s="51"/>
@@ -42420,9 +41966,7 @@
       <c r="FC117" s="51"/>
       <c r="FD117" s="51"/>
       <c r="FE117" s="51"/>
-      <c r="FF117" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF117" s="51"/>
       <c r="FG117" s="51"/>
       <c r="FH117" s="51"/>
       <c r="FI117" s="53"/>
@@ -42452,7 +41996,7 @@
       <c r="D118" s="51"/>
       <c r="E118" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42475</v>
+        <v>42479</v>
       </c>
       <c r="F118" s="51"/>
       <c r="G118" s="51"/>
@@ -42611,9 +42155,7 @@
       <c r="FC118" s="51"/>
       <c r="FD118" s="51"/>
       <c r="FE118" s="51"/>
-      <c r="FF118" s="51" t="s">
-        <v>191</v>
-      </c>
+      <c r="FF118" s="51"/>
       <c r="FG118" s="51"/>
       <c r="FH118" s="51"/>
       <c r="FI118" s="53"/>

</xml_diff>

<commit_message>
modify price tests for dynamic price data
</commit_message>
<xml_diff>
--- a/Regression/templates/PriceProductGroups.xlsx
+++ b/Regression/templates/PriceProductGroups.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="22995" windowHeight="10035" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="AlphazoneMakeCounties" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="Skyscraper-Spotlight" sheetId="6" r:id="rId6"/>
     <sheet name="Not Priceable-Unclassified" sheetId="7" r:id="rId7"/>
     <sheet name="All" sheetId="8" r:id="rId8"/>
+    <sheet name="Pricing" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3380" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3596" uniqueCount="478">
   <si>
     <t>KBB Elite</t>
   </si>
@@ -1206,12 +1207,264 @@
   </si>
   <si>
     <t>Sent EQS</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>BMWNewCarPriceTotal</t>
+  </si>
+  <si>
+    <t>Dollars</t>
+  </si>
+  <si>
+    <t>AlphazoneMakePriceTotal</t>
+  </si>
+  <si>
+    <t>$650.00</t>
+  </si>
+  <si>
+    <t>$2,895.00</t>
+  </si>
+  <si>
+    <t>$2,885.00</t>
+  </si>
+  <si>
+    <t>$1,050.00</t>
+  </si>
+  <si>
+    <t>$4,135.00</t>
+  </si>
+  <si>
+    <t>$2,545.00</t>
+  </si>
+  <si>
+    <t>$400.00</t>
+  </si>
+  <si>
+    <t>$600.00</t>
+  </si>
+  <si>
+    <t>$1,200.00</t>
+  </si>
+  <si>
+    <t>$4,195.00</t>
+  </si>
+  <si>
+    <t>$2,995.00</t>
+  </si>
+  <si>
+    <t>$450.00</t>
+  </si>
+  <si>
+    <t>$200.00</t>
+  </si>
+  <si>
+    <t>$300.00</t>
+  </si>
+  <si>
+    <t>$1,500.00</t>
+  </si>
+  <si>
+    <t>$1,100.00</t>
+  </si>
+  <si>
+    <t>$1,000.00</t>
+  </si>
+  <si>
+    <t>$800.00</t>
+  </si>
+  <si>
+    <t>$500.00</t>
+  </si>
+  <si>
+    <t>$99.00</t>
+  </si>
+  <si>
+    <t>$4,830.00</t>
+  </si>
+  <si>
+    <t>$7,945.00</t>
+  </si>
+  <si>
+    <t>$700.00</t>
+  </si>
+  <si>
+    <t>$1,342.00</t>
+  </si>
+  <si>
+    <t>$7,730.00</t>
+  </si>
+  <si>
+    <t>$242.00</t>
+  </si>
+  <si>
+    <t>BMWUsedCarPremiumPriceTotal</t>
+  </si>
+  <si>
+    <t>$5,780.00</t>
+  </si>
+  <si>
+    <t>Test Totals</t>
+  </si>
+  <si>
+    <t>FlatTypePriceTotal</t>
+  </si>
+  <si>
+    <t>FordNewCarPriceTotal</t>
+  </si>
+  <si>
+    <t>$8,390.00</t>
+  </si>
+  <si>
+    <t>GMNewCarPriceTotal</t>
+  </si>
+  <si>
+    <t>GMCertifiedPremPriceTotal</t>
+  </si>
+  <si>
+    <t>GMUsedPremAndNewPriceTotal</t>
+  </si>
+  <si>
+    <t>InventoryMakeMarketPriceTotal</t>
+  </si>
+  <si>
+    <t>InventoryMarketPriceTotal</t>
+  </si>
+  <si>
+    <t>InventoryOnlyPriceTotal</t>
+  </si>
+  <si>
+    <t>MININewPriceTotal</t>
+  </si>
+  <si>
+    <t>MINIUsedPremiumPriceTotal</t>
+  </si>
+  <si>
+    <t>NewCarPriceTotal</t>
+  </si>
+  <si>
+    <t>PorcheNewCarPriceTotal</t>
+  </si>
+  <si>
+    <t>PorcheUsedPremiumPriceTotal</t>
+  </si>
+  <si>
+    <t>PremiumPriceTotal</t>
+  </si>
+  <si>
+    <t>SkyscraperBucketsPriceTotal</t>
+  </si>
+  <si>
+    <t>SkyscraperSlotsPriceTotal</t>
+  </si>
+  <si>
+    <t>SpotlightPriceTotal</t>
+  </si>
+  <si>
+    <t>UsedCarNonPremiumPriceTotal</t>
+  </si>
+  <si>
+    <t>$2,025.00</t>
+  </si>
+  <si>
+    <t>$270.00</t>
+  </si>
+  <si>
+    <t>$1,700.00</t>
+  </si>
+  <si>
+    <t>$3,995.00</t>
+  </si>
+  <si>
+    <t>$6,235.00</t>
+  </si>
+  <si>
+    <t>$2,375.00</t>
+  </si>
+  <si>
+    <t>$2,070.00</t>
+  </si>
+  <si>
+    <t>$4,445.00</t>
+  </si>
+  <si>
+    <t>$190.00</t>
+  </si>
+  <si>
+    <t>$265.00</t>
+  </si>
+  <si>
+    <t>$230.00</t>
+  </si>
+  <si>
+    <t>$305.00</t>
+  </si>
+  <si>
+    <t>$990.00</t>
+  </si>
+  <si>
+    <t>$2,265.00</t>
+  </si>
+  <si>
+    <t>$770.00</t>
+  </si>
+  <si>
+    <t>$1,710.00</t>
+  </si>
+  <si>
+    <t>$5,595.00</t>
+  </si>
+  <si>
+    <t>$18,245.00</t>
+  </si>
+  <si>
+    <t>$250.00</t>
+  </si>
+  <si>
+    <t>$350.00</t>
+  </si>
+  <si>
+    <t>$6,425.00</t>
+  </si>
+  <si>
+    <t>$490.00</t>
+  </si>
+  <si>
+    <t>$1,960.00</t>
+  </si>
+  <si>
+    <t>$1,175.00</t>
+  </si>
+  <si>
+    <t>$3,625.00</t>
+  </si>
+  <si>
+    <t>$680.00</t>
+  </si>
+  <si>
+    <t>$895.00</t>
+  </si>
+  <si>
+    <t>$1,715.00</t>
+  </si>
+  <si>
+    <t>$3,575.00</t>
+  </si>
+  <si>
+    <t>$2,145.00</t>
+  </si>
+  <si>
+    <t>$9,010.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1935,7 +2188,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2255,6 +2508,35 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -7781,8 +8063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH20"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AS29" sqref="AS29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="54.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8285,7 +8567,7 @@
       <c r="AP6" s="35" t="s">
         <v>328</v>
       </c>
-      <c r="AQ6" s="77" t="s">
+      <c r="AQ6" s="130" t="s">
         <v>343</v>
       </c>
       <c r="AR6" s="35" t="s">
@@ -8343,7 +8625,7 @@
       <c r="AP7" s="35" t="s">
         <v>328</v>
       </c>
-      <c r="AQ7" s="77" t="s">
+      <c r="AQ7" s="130" t="s">
         <v>343</v>
       </c>
       <c r="AR7" s="35" t="s">
@@ -9027,8 +9309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CP138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AP1" sqref="AP1"/>
+    <sheetView topLeftCell="BO1" workbookViewId="0">
+      <selection activeCell="BS5" sqref="BS5:BS9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9751,8 +10033,8 @@
         <v>186</v>
       </c>
       <c r="BP5" s="2"/>
-      <c r="BS5" s="35" t="s">
-        <v>223</v>
+      <c r="BS5" s="86" t="s">
+        <v>394</v>
       </c>
       <c r="BT5" s="105" t="b">
         <v>1</v>
@@ -9807,8 +10089,8 @@
         <v>186</v>
       </c>
       <c r="BP6" s="2"/>
-      <c r="BS6" s="35" t="s">
-        <v>223</v>
+      <c r="BS6" s="86" t="s">
+        <v>394</v>
       </c>
       <c r="BT6" s="105" t="b">
         <v>1</v>
@@ -9933,8 +10215,8 @@
       <c r="BR7" s="35">
         <v>1</v>
       </c>
-      <c r="BS7" s="35" t="s">
-        <v>223</v>
+      <c r="BS7" s="86" t="s">
+        <v>394</v>
       </c>
       <c r="BT7" s="105" t="b">
         <v>1</v>
@@ -9989,8 +10271,8 @@
         <v>186</v>
       </c>
       <c r="BP8" s="2"/>
-      <c r="BS8" s="35" t="s">
-        <v>223</v>
+      <c r="BS8" s="86" t="s">
+        <v>394</v>
       </c>
       <c r="BT8" s="105" t="b">
         <v>1</v>
@@ -10045,8 +10327,8 @@
         <v>186</v>
       </c>
       <c r="BP9" s="2"/>
-      <c r="BS9" s="35" t="s">
-        <v>223</v>
+      <c r="BS9" s="86" t="s">
+        <v>394</v>
       </c>
       <c r="BT9" s="105" t="b">
         <v>1</v>
@@ -11432,7 +11714,7 @@
       <c r="BQ19" s="2"/>
       <c r="BR19" s="2"/>
       <c r="BS19" s="86" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
       <c r="BT19" s="105" t="b">
         <v>1</v>
@@ -11553,7 +11835,7 @@
         <v>1</v>
       </c>
       <c r="BS20" s="86" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
       <c r="BT20" s="105" t="b">
         <v>1</v>
@@ -11787,7 +12069,7 @@
         <v>1</v>
       </c>
       <c r="BS22" s="86" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
       <c r="BT22" s="105" t="b">
         <v>1</v>
@@ -11908,7 +12190,7 @@
         <v>1</v>
       </c>
       <c r="BS23" s="86" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
       <c r="BT23" s="105" t="b">
         <v>1</v>
@@ -12029,7 +12311,7 @@
         <v>1</v>
       </c>
       <c r="BS24" s="86" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
       <c r="BT24" s="105" t="b">
         <v>1</v>
@@ -12770,8 +13052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AL4" sqref="AL4"/>
+    <sheetView topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AH7" sqref="AH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15549,8 +15831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FY124"/>
   <sheetViews>
-    <sheetView topLeftCell="FA1" workbookViewId="0">
-      <selection activeCell="FF2" sqref="FF2:FF118"/>
+    <sheetView topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -16258,7 +16540,7 @@
       <c r="D2" s="51"/>
       <c r="E2" s="52">
         <f t="shared" ref="E2:E33" ca="1" si="0">TODAY()</f>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F2" s="51"/>
       <c r="G2" s="51"/>
@@ -16447,7 +16729,7 @@
       <c r="D3" s="51"/>
       <c r="E3" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F3" s="51"/>
       <c r="G3" s="51"/>
@@ -16636,7 +16918,7 @@
       <c r="D4" s="51"/>
       <c r="E4" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="51"/>
@@ -16825,7 +17107,7 @@
       <c r="D5" s="51"/>
       <c r="E5" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F5" s="51"/>
       <c r="G5" s="51"/>
@@ -17016,7 +17298,7 @@
       <c r="D6" s="51"/>
       <c r="E6" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F6" s="51" t="s">
         <v>263</v>
@@ -17231,7 +17513,7 @@
       <c r="D7" s="51"/>
       <c r="E7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
@@ -17432,7 +17714,7 @@
       <c r="D8" s="51"/>
       <c r="E8" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F8" s="51"/>
       <c r="G8" s="51"/>
@@ -17635,7 +17917,7 @@
       <c r="D9" s="51"/>
       <c r="E9" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
@@ -17832,7 +18114,7 @@
       <c r="D10" s="51"/>
       <c r="E10" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
@@ -18083,7 +18365,7 @@
       <c r="D11" s="51"/>
       <c r="E11" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
@@ -18336,7 +18618,7 @@
       <c r="D12" s="51"/>
       <c r="E12" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
@@ -18589,7 +18871,7 @@
       <c r="D13" s="51"/>
       <c r="E13" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F13" s="51"/>
       <c r="G13" s="51"/>
@@ -18822,7 +19104,7 @@
       <c r="D14" s="51"/>
       <c r="E14" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F14" s="51"/>
       <c r="G14" s="51"/>
@@ -19059,7 +19341,7 @@
       <c r="D15" s="51"/>
       <c r="E15" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F15" s="51"/>
       <c r="G15" s="51"/>
@@ -19292,7 +19574,7 @@
       <c r="D16" s="51"/>
       <c r="E16" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F16" s="51"/>
       <c r="G16" s="51"/>
@@ -19517,7 +19799,7 @@
       <c r="D17" s="51"/>
       <c r="E17" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F17" s="51"/>
       <c r="G17" s="51"/>
@@ -19742,7 +20024,7 @@
       <c r="D18" s="51"/>
       <c r="E18" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F18" s="51"/>
       <c r="G18" s="51"/>
@@ -19934,7 +20216,7 @@
       <c r="D19" s="51"/>
       <c r="E19" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F19" s="51"/>
       <c r="G19" s="51"/>
@@ -20123,7 +20405,7 @@
       <c r="D20" s="51"/>
       <c r="E20" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F20" s="51"/>
       <c r="G20" s="51"/>
@@ -20312,7 +20594,7 @@
       <c r="D21" s="51"/>
       <c r="E21" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F21" s="51"/>
       <c r="G21" s="51"/>
@@ -20503,7 +20785,7 @@
       <c r="D22" s="51"/>
       <c r="E22" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F22" s="51"/>
       <c r="G22" s="51"/>
@@ -20692,7 +20974,7 @@
       <c r="D23" s="51"/>
       <c r="E23" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F23" s="51"/>
       <c r="G23" s="51"/>
@@ -20919,7 +21201,7 @@
       <c r="D24" s="51"/>
       <c r="E24" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F24" s="51"/>
       <c r="G24" s="51"/>
@@ -21132,7 +21414,7 @@
       <c r="D25" s="51"/>
       <c r="E25" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F25" s="51"/>
       <c r="G25" s="51"/>
@@ -21345,7 +21627,7 @@
       <c r="D26" s="51"/>
       <c r="E26" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F26" s="51"/>
       <c r="G26" s="51"/>
@@ -21602,7 +21884,7 @@
       <c r="D27" s="51"/>
       <c r="E27" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F27" s="51"/>
       <c r="G27" s="51"/>
@@ -21859,7 +22141,7 @@
       <c r="D28" s="51"/>
       <c r="E28" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F28" s="51"/>
       <c r="G28" s="51"/>
@@ -22098,7 +22380,7 @@
       <c r="D29" s="51"/>
       <c r="E29" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F29" s="51"/>
       <c r="G29" s="51"/>
@@ -22333,7 +22615,7 @@
       <c r="D30" s="51"/>
       <c r="E30" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F30" s="51"/>
       <c r="G30" s="51"/>
@@ -22572,7 +22854,7 @@
       <c r="D31" s="51"/>
       <c r="E31" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F31" s="51"/>
       <c r="G31" s="51"/>
@@ -22809,7 +23091,7 @@
       </c>
       <c r="E32" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F32" s="51"/>
       <c r="G32" s="51"/>
@@ -23018,7 +23300,7 @@
       <c r="D33" s="51"/>
       <c r="E33" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F33" s="51"/>
       <c r="G33" s="51"/>
@@ -23225,7 +23507,7 @@
       <c r="D34" s="51"/>
       <c r="E34" s="52">
         <f t="shared" ref="E34:E65" ca="1" si="1">TODAY()</f>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F34" s="51"/>
       <c r="G34" s="51"/>
@@ -23480,7 +23762,7 @@
       <c r="D35" s="51"/>
       <c r="E35" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F35" s="51"/>
       <c r="G35" s="51"/>
@@ -23745,7 +24027,7 @@
       <c r="D36" s="51"/>
       <c r="E36" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F36" s="51"/>
       <c r="G36" s="51"/>
@@ -24010,7 +24292,7 @@
       <c r="D37" s="51"/>
       <c r="E37" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F37" s="51"/>
       <c r="G37" s="51"/>
@@ -24309,7 +24591,7 @@
       <c r="D38" s="51"/>
       <c r="E38" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F38" s="51"/>
       <c r="G38" s="51"/>
@@ -24518,7 +24800,7 @@
       <c r="D39" s="51"/>
       <c r="E39" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F39" s="51"/>
       <c r="G39" s="51"/>
@@ -24763,7 +25045,7 @@
       <c r="D40" s="51"/>
       <c r="E40" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F40" s="51"/>
       <c r="G40" s="51"/>
@@ -24974,7 +25256,7 @@
       <c r="D41" s="51"/>
       <c r="E41" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F41" s="51"/>
       <c r="G41" s="51"/>
@@ -25181,7 +25463,7 @@
       <c r="D42" s="51"/>
       <c r="E42" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F42" s="51"/>
       <c r="G42" s="51"/>
@@ -25402,7 +25684,7 @@
       <c r="D43" s="51"/>
       <c r="E43" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F43" s="51"/>
       <c r="G43" s="51"/>
@@ -25667,7 +25949,7 @@
       <c r="D44" s="51"/>
       <c r="E44" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F44" s="51"/>
       <c r="G44" s="51"/>
@@ -25932,7 +26214,7 @@
       <c r="D45" s="51"/>
       <c r="E45" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F45" s="51"/>
       <c r="G45" s="51"/>
@@ -26199,7 +26481,7 @@
       </c>
       <c r="E46" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F46" s="51"/>
       <c r="G46" s="51"/>
@@ -26412,7 +26694,7 @@
       </c>
       <c r="E47" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F47" s="51"/>
       <c r="G47" s="51"/>
@@ -26625,7 +26907,7 @@
       </c>
       <c r="E48" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F48" s="51"/>
       <c r="G48" s="51"/>
@@ -26836,7 +27118,7 @@
       </c>
       <c r="E49" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F49" s="51"/>
       <c r="G49" s="51"/>
@@ -27045,7 +27327,7 @@
       <c r="D50" s="51"/>
       <c r="E50" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F50" s="51"/>
       <c r="G50" s="51"/>
@@ -27236,7 +27518,7 @@
       <c r="D51" s="51"/>
       <c r="E51" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F51" s="51"/>
       <c r="G51" s="51"/>
@@ -27433,7 +27715,7 @@
       <c r="D52" s="51"/>
       <c r="E52" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F52" s="51"/>
       <c r="G52" s="51"/>
@@ -27626,7 +27908,7 @@
       <c r="D53" s="51"/>
       <c r="E53" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F53" s="51"/>
       <c r="G53" s="51"/>
@@ -27832,7 +28114,7 @@
       <c r="D54" s="51"/>
       <c r="E54" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F54" s="51"/>
       <c r="G54" s="51"/>
@@ -28037,7 +28319,7 @@
       <c r="D55" s="51"/>
       <c r="E55" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F55" s="51"/>
       <c r="G55" s="51"/>
@@ -28278,7 +28560,7 @@
       <c r="D56" s="51"/>
       <c r="E56" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F56" s="51"/>
       <c r="G56" s="51"/>
@@ -28483,7 +28765,7 @@
       <c r="D57" s="51"/>
       <c r="E57" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F57" s="51"/>
       <c r="G57" s="51"/>
@@ -28677,7 +28959,7 @@
       <c r="D58" s="51"/>
       <c r="E58" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F58" s="51"/>
       <c r="G58" s="51"/>
@@ -28877,7 +29159,7 @@
       <c r="D59" s="51"/>
       <c r="E59" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F59" s="51"/>
       <c r="G59" s="51"/>
@@ -29079,7 +29361,7 @@
       <c r="D60" s="51"/>
       <c r="E60" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F60" s="51"/>
       <c r="G60" s="51"/>
@@ -29276,7 +29558,7 @@
       <c r="D61" s="51"/>
       <c r="E61" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F61" s="51"/>
       <c r="G61" s="51"/>
@@ -29509,7 +29791,7 @@
       <c r="D62" s="51"/>
       <c r="E62" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F62" s="51"/>
       <c r="G62" s="51"/>
@@ -29742,7 +30024,7 @@
       <c r="D63" s="51"/>
       <c r="E63" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F63" s="51"/>
       <c r="G63" s="51"/>
@@ -29979,7 +30261,7 @@
       <c r="D64" s="51"/>
       <c r="E64" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F64" s="51"/>
       <c r="G64" s="51"/>
@@ -30212,7 +30494,7 @@
       <c r="D65" s="51"/>
       <c r="E65" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F65" s="51"/>
       <c r="G65" s="51"/>
@@ -30461,7 +30743,7 @@
       <c r="D66" s="51"/>
       <c r="E66" s="52">
         <f t="shared" ref="E66:E89" ca="1" si="2">TODAY()</f>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F66" s="51"/>
       <c r="G66" s="51"/>
@@ -30714,7 +30996,7 @@
       <c r="D67" s="51"/>
       <c r="E67" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F67" s="51"/>
       <c r="G67" s="51"/>
@@ -30951,7 +31233,7 @@
       <c r="D68" s="51"/>
       <c r="E68" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F68" s="51"/>
       <c r="G68" s="51"/>
@@ -31190,7 +31472,7 @@
       <c r="D69" s="51"/>
       <c r="E69" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F69" s="51"/>
       <c r="G69" s="51"/>
@@ -31429,7 +31711,7 @@
       <c r="D70" s="51"/>
       <c r="E70" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F70" s="51"/>
       <c r="G70" s="51"/>
@@ -31670,7 +31952,7 @@
       <c r="D71" s="51"/>
       <c r="E71" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F71" s="51"/>
       <c r="G71" s="51"/>
@@ -31907,7 +32189,7 @@
       <c r="D72" s="51"/>
       <c r="E72" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F72" s="51"/>
       <c r="G72" s="51"/>
@@ -32096,7 +32378,7 @@
       <c r="D73" s="51"/>
       <c r="E73" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F73" s="51"/>
       <c r="G73" s="51"/>
@@ -32285,7 +32567,7 @@
       <c r="D74" s="51"/>
       <c r="E74" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F74" s="51"/>
       <c r="G74" s="51"/>
@@ -32474,7 +32756,7 @@
       <c r="D75" s="51"/>
       <c r="E75" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F75" s="51"/>
       <c r="G75" s="51"/>
@@ -32723,7 +33005,7 @@
       <c r="D76" s="51"/>
       <c r="E76" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F76" s="51"/>
       <c r="G76" s="51"/>
@@ -32974,7 +33256,7 @@
       <c r="D77" s="51"/>
       <c r="E77" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F77" s="51"/>
       <c r="G77" s="51"/>
@@ -33225,7 +33507,7 @@
       <c r="D78" s="51"/>
       <c r="E78" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F78" s="51"/>
       <c r="G78" s="51"/>
@@ -33456,7 +33738,7 @@
       <c r="D79" s="51"/>
       <c r="E79" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F79" s="51"/>
       <c r="G79" s="51"/>
@@ -33691,7 +33973,7 @@
       <c r="D80" s="51"/>
       <c r="E80" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F80" s="51"/>
       <c r="G80" s="51"/>
@@ -33922,7 +34204,7 @@
       <c r="D81" s="51"/>
       <c r="E81" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F81" s="51"/>
       <c r="G81" s="51"/>
@@ -34165,7 +34447,7 @@
       <c r="D82" s="51"/>
       <c r="E82" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F82" s="51"/>
       <c r="G82" s="51"/>
@@ -34386,7 +34668,7 @@
       <c r="D83" s="51"/>
       <c r="E83" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F83" s="51"/>
       <c r="G83" s="51"/>
@@ -34635,7 +34917,7 @@
       <c r="D84" s="51"/>
       <c r="E84" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F84" s="51"/>
       <c r="G84" s="51"/>
@@ -34884,7 +35166,7 @@
       <c r="D85" s="51"/>
       <c r="E85" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F85" s="51"/>
       <c r="G85" s="51"/>
@@ -35133,7 +35415,7 @@
       <c r="D86" s="51"/>
       <c r="E86" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F86" s="51"/>
       <c r="G86" s="51"/>
@@ -35382,7 +35664,7 @@
       <c r="D87" s="51"/>
       <c r="E87" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F87" s="51"/>
       <c r="G87" s="51"/>
@@ -35573,7 +35855,7 @@
       <c r="D88" s="51"/>
       <c r="E88" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F88" s="51"/>
       <c r="G88" s="51"/>
@@ -35764,7 +36046,7 @@
       <c r="D89" s="51"/>
       <c r="E89" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F89" s="51"/>
       <c r="G89" s="51"/>
@@ -36139,7 +36421,7 @@
       <c r="D91" s="51"/>
       <c r="E91" s="52">
         <f ca="1">TODAY()</f>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F91" s="51"/>
       <c r="G91" s="51"/>
@@ -36514,7 +36796,7 @@
       <c r="D93" s="51"/>
       <c r="E93" s="52">
         <f t="shared" ref="E93:E118" ca="1" si="3">TODAY()</f>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F93" s="51"/>
       <c r="G93" s="51"/>
@@ -36731,7 +37013,7 @@
       <c r="D94" s="51"/>
       <c r="E94" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F94" s="51"/>
       <c r="G94" s="51"/>
@@ -36948,7 +37230,7 @@
       <c r="D95" s="51"/>
       <c r="E95" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F95" s="51"/>
       <c r="G95" s="51"/>
@@ -37163,7 +37445,7 @@
       <c r="D96" s="51"/>
       <c r="E96" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F96" s="51"/>
       <c r="G96" s="51"/>
@@ -37376,7 +37658,7 @@
       <c r="D97" s="51"/>
       <c r="E97" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F97" s="51"/>
       <c r="G97" s="51"/>
@@ -37576,7 +37858,7 @@
       <c r="D98" s="51"/>
       <c r="E98" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F98" s="51"/>
       <c r="G98" s="51"/>
@@ -37776,7 +38058,7 @@
       <c r="D99" s="51"/>
       <c r="E99" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F99" s="51"/>
       <c r="G99" s="51"/>
@@ -37978,7 +38260,7 @@
       <c r="D100" s="51"/>
       <c r="E100" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F100" s="51"/>
       <c r="G100" s="51"/>
@@ -38180,7 +38462,7 @@
       <c r="D101" s="51"/>
       <c r="E101" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F101" s="51"/>
       <c r="G101" s="51"/>
@@ -38382,7 +38664,7 @@
       <c r="D102" s="51"/>
       <c r="E102" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F102" s="51"/>
       <c r="G102" s="51"/>
@@ -38584,7 +38866,7 @@
       <c r="D103" s="51"/>
       <c r="E103" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F103" s="51"/>
       <c r="G103" s="51"/>
@@ -38785,7 +39067,7 @@
       <c r="D104" s="51"/>
       <c r="E104" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F104" s="51"/>
       <c r="G104" s="51"/>
@@ -39002,7 +39284,7 @@
       <c r="D105" s="51"/>
       <c r="E105" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F105" s="51"/>
       <c r="G105" s="51"/>
@@ -39219,7 +39501,7 @@
       <c r="D106" s="51"/>
       <c r="E106" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F106" s="51"/>
       <c r="G106" s="51"/>
@@ -39436,7 +39718,7 @@
       <c r="D107" s="51"/>
       <c r="E107" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F107" s="51"/>
       <c r="G107" s="51"/>
@@ -39653,7 +39935,7 @@
       <c r="D108" s="51"/>
       <c r="E108" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F108" s="51"/>
       <c r="G108" s="51"/>
@@ -39870,7 +40152,7 @@
       <c r="D109" s="51"/>
       <c r="E109" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F109" s="51"/>
       <c r="G109" s="51"/>
@@ -40087,7 +40369,7 @@
       <c r="D110" s="51"/>
       <c r="E110" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F110" s="51"/>
       <c r="G110" s="51"/>
@@ -40304,7 +40586,7 @@
       <c r="D111" s="51"/>
       <c r="E111" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F111" s="51"/>
       <c r="G111" s="51"/>
@@ -40521,7 +40803,7 @@
       <c r="D112" s="51"/>
       <c r="E112" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F112" s="51"/>
       <c r="G112" s="51"/>
@@ -40738,7 +41020,7 @@
       <c r="D113" s="51"/>
       <c r="E113" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F113" s="51"/>
       <c r="G113" s="51"/>
@@ -40955,7 +41237,7 @@
       <c r="D114" s="51"/>
       <c r="E114" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F114" s="51"/>
       <c r="G114" s="51"/>
@@ -41144,7 +41426,7 @@
       <c r="D115" s="51"/>
       <c r="E115" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F115" s="51"/>
       <c r="G115" s="51"/>
@@ -41333,7 +41615,7 @@
       <c r="D116" s="51"/>
       <c r="E116" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F116" s="51"/>
       <c r="G116" s="51"/>
@@ -41522,7 +41804,7 @@
       <c r="D117" s="51"/>
       <c r="E117" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F117" s="51"/>
       <c r="G117" s="51"/>
@@ -41711,7 +41993,7 @@
       <c r="D118" s="51"/>
       <c r="E118" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42493</v>
+        <v>42496</v>
       </c>
       <c r="F118" s="51"/>
       <c r="G118" s="51"/>
@@ -41915,4 +42197,1819 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K200"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="52.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>395</v>
+      </c>
+      <c r="C1" s="120" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="120"/>
+      <c r="C2" s="126">
+        <f t="shared" ref="C2:C66" si="0">B2</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="121"/>
+      <c r="J2" s="122"/>
+      <c r="K2" s="123"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="120"/>
+      <c r="C3" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I3" s="121"/>
+      <c r="J3" s="122"/>
+      <c r="K3" s="123"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="120"/>
+      <c r="C4" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I4" s="121"/>
+      <c r="J4" s="122"/>
+      <c r="K4" s="123"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="48" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="120"/>
+      <c r="C5" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I5" s="121"/>
+      <c r="J5" s="122"/>
+      <c r="K5" s="123"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="120">
+        <v>650</v>
+      </c>
+      <c r="C6" s="126" t="s">
+        <v>399</v>
+      </c>
+      <c r="I6" s="121"/>
+      <c r="J6" s="122"/>
+      <c r="K6" s="123"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="120"/>
+      <c r="C7" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="121"/>
+      <c r="J7" s="122"/>
+      <c r="K7" s="123"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="120"/>
+      <c r="C8" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="121"/>
+      <c r="J8" s="122"/>
+      <c r="K8" s="123"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="120"/>
+      <c r="C9" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="121"/>
+      <c r="J9" s="122"/>
+      <c r="K9" s="123"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="120"/>
+      <c r="C10" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="120">
+        <v>2895</v>
+      </c>
+      <c r="C11" s="126" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="120">
+        <v>2885</v>
+      </c>
+      <c r="C12" s="126" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="120">
+        <v>1050</v>
+      </c>
+      <c r="C13" s="126" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="120">
+        <v>4135</v>
+      </c>
+      <c r="C14" s="126" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="120">
+        <v>2545</v>
+      </c>
+      <c r="C15" s="126" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="120">
+        <v>300</v>
+      </c>
+      <c r="C16" s="126" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="120">
+        <v>250</v>
+      </c>
+      <c r="C17" s="126" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="120">
+        <v>400</v>
+      </c>
+      <c r="C18" s="126" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="120"/>
+      <c r="C19" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="48" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" s="120"/>
+      <c r="C20" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="120"/>
+      <c r="C21" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="120"/>
+      <c r="C22" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="120">
+        <v>600</v>
+      </c>
+      <c r="C23" s="126" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="120"/>
+      <c r="C24" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="120"/>
+      <c r="C25" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="120"/>
+      <c r="C26" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="120"/>
+      <c r="C27" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="120"/>
+      <c r="C28" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="120">
+        <v>1200</v>
+      </c>
+      <c r="C29" s="126" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="120">
+        <v>4195</v>
+      </c>
+      <c r="C30" s="126" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="120">
+        <v>2995</v>
+      </c>
+      <c r="C31" s="126" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="120">
+        <v>242</v>
+      </c>
+      <c r="C32" s="126" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="48" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="120"/>
+      <c r="C33" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="120"/>
+      <c r="C34" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="120">
+        <v>2375</v>
+      </c>
+      <c r="C35" s="126" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="120">
+        <v>2070</v>
+      </c>
+      <c r="C36" s="126" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="120">
+        <v>6235</v>
+      </c>
+      <c r="C37" s="126" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="120">
+        <v>265</v>
+      </c>
+      <c r="C38" s="126" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="120">
+        <v>305</v>
+      </c>
+      <c r="C39" s="126" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="120">
+        <v>305</v>
+      </c>
+      <c r="C40" s="126" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" s="120">
+        <v>770</v>
+      </c>
+      <c r="C41" s="126" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" s="120">
+        <v>770</v>
+      </c>
+      <c r="C42" s="126" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="120">
+        <v>270</v>
+      </c>
+      <c r="C43" s="126" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" s="120">
+        <v>2025</v>
+      </c>
+      <c r="C44" s="126" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" s="120">
+        <v>1700</v>
+      </c>
+      <c r="C45" s="126" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" s="120"/>
+      <c r="C46" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" s="120"/>
+      <c r="C47" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" s="120"/>
+      <c r="C48" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="B49" s="120"/>
+      <c r="C49" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="B50" s="120"/>
+      <c r="C50" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="120">
+        <v>450</v>
+      </c>
+      <c r="C51" s="126" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="120"/>
+      <c r="C52" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="B53" s="120">
+        <v>200</v>
+      </c>
+      <c r="C53" s="126" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="B54" s="120">
+        <v>190</v>
+      </c>
+      <c r="C54" s="126" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55" s="120">
+        <v>230</v>
+      </c>
+      <c r="C55" s="126" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="120"/>
+      <c r="C56" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B57" s="120">
+        <v>300</v>
+      </c>
+      <c r="C57" s="126" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="B58" s="120"/>
+      <c r="C58" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="B59" s="120"/>
+      <c r="C59" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="B60" s="120">
+        <v>770</v>
+      </c>
+      <c r="C60" s="126" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" s="120">
+        <v>770</v>
+      </c>
+      <c r="C61" s="126" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="B62" s="120">
+        <v>490</v>
+      </c>
+      <c r="C62" s="126" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B63" s="120">
+        <v>1960</v>
+      </c>
+      <c r="C63" s="126" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" s="120">
+        <v>1175</v>
+      </c>
+      <c r="C64" s="126" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="B65" s="120"/>
+      <c r="C65" s="126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B66" s="120">
+        <v>6425</v>
+      </c>
+      <c r="C66" s="126" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B67" s="120">
+        <v>680</v>
+      </c>
+      <c r="C67" s="126" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68" s="120">
+        <v>895</v>
+      </c>
+      <c r="C68" s="126" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="B69" s="120">
+        <v>1715</v>
+      </c>
+      <c r="C69" s="126" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B70" s="120">
+        <v>3575</v>
+      </c>
+      <c r="C70" s="126" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="B71" s="120">
+        <v>2145</v>
+      </c>
+      <c r="C71" s="126" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72" s="120">
+        <v>1500</v>
+      </c>
+      <c r="C72" s="126" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="B73" s="120">
+        <v>1100</v>
+      </c>
+      <c r="C73" s="126" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="B74" s="120">
+        <v>1000</v>
+      </c>
+      <c r="C74" s="126" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B75" s="120"/>
+      <c r="C75" s="126">
+        <f t="shared" ref="C67:C117" si="1">B75</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B76" s="120"/>
+      <c r="C76" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B77" s="120"/>
+      <c r="C77" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="B78" s="120"/>
+      <c r="C78" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B79" s="120"/>
+      <c r="C79" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="B80" s="120"/>
+      <c r="C80" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="B81" s="120"/>
+      <c r="C81" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="B82" s="120"/>
+      <c r="C82" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="B83" s="120"/>
+      <c r="C83" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="B84" s="120"/>
+      <c r="C84" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="B85" s="120"/>
+      <c r="C85" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="B86" s="120"/>
+      <c r="C86" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="B87" s="120">
+        <v>400</v>
+      </c>
+      <c r="C87" s="126" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="B88" s="120">
+        <v>800</v>
+      </c>
+      <c r="C88" s="126" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="B89" s="120">
+        <v>600</v>
+      </c>
+      <c r="C89" s="126" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="B90" s="120">
+        <v>0</v>
+      </c>
+      <c r="C90" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="B91" s="120">
+        <v>500</v>
+      </c>
+      <c r="C91" s="126" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="B92" s="120">
+        <v>0</v>
+      </c>
+      <c r="C92" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="B93" s="120"/>
+      <c r="C93" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="B94" s="120"/>
+      <c r="C94" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="B95" s="120"/>
+      <c r="C95" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="B96" s="120"/>
+      <c r="C96" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="B97" s="120"/>
+      <c r="C97" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="48" t="s">
+        <v>99</v>
+      </c>
+      <c r="B98" s="120"/>
+      <c r="C98" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="B99" s="120"/>
+      <c r="C99" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="B100" s="120"/>
+      <c r="C100" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="B101" s="120"/>
+      <c r="C101" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="B102" s="120"/>
+      <c r="C102" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="B103" s="120">
+        <v>99</v>
+      </c>
+      <c r="C103" s="126" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="B104" s="120">
+        <v>4830</v>
+      </c>
+      <c r="C104" s="126" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="B105" s="120">
+        <v>7945</v>
+      </c>
+      <c r="C105" s="126" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B106" s="120"/>
+      <c r="C106" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B107" s="120">
+        <v>2265</v>
+      </c>
+      <c r="C107" s="126" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="48" t="s">
+        <v>116</v>
+      </c>
+      <c r="B108" s="120"/>
+      <c r="C108" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="B109" s="120">
+        <v>700</v>
+      </c>
+      <c r="C109" s="126" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A110" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="B110" s="120">
+        <v>5595</v>
+      </c>
+      <c r="C110" s="126" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A111" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="B111" s="120">
+        <v>5595</v>
+      </c>
+      <c r="C111" s="126" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="B112" s="120"/>
+      <c r="C112" s="126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="B113" s="120">
+        <v>1710</v>
+      </c>
+      <c r="C113" s="126" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="B114" s="120">
+        <v>300</v>
+      </c>
+      <c r="C114" s="126" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B115" s="120">
+        <v>250</v>
+      </c>
+      <c r="C115" s="126" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B116" s="120">
+        <v>250</v>
+      </c>
+      <c r="C116" s="126" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="B117" s="120">
+        <v>350</v>
+      </c>
+      <c r="C117" s="126" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="B118" s="120">
+        <v>400</v>
+      </c>
+      <c r="C118" s="126" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="74"/>
+      <c r="B119" s="74"/>
+      <c r="C119" s="129"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="74"/>
+      <c r="B120" s="74"/>
+      <c r="C120" s="129"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="74"/>
+      <c r="B121" s="74"/>
+      <c r="C121" s="129"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="74"/>
+      <c r="B122" s="74"/>
+      <c r="C122" s="129"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="49"/>
+      <c r="B123" s="120"/>
+      <c r="C123" s="120"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="49"/>
+      <c r="B124" s="120"/>
+      <c r="C124" s="120"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="49"/>
+      <c r="B125" s="120"/>
+      <c r="C125" s="120"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="49"/>
+      <c r="B126" s="120"/>
+      <c r="C126" s="120"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="49"/>
+      <c r="B127" s="120"/>
+      <c r="C127" s="120"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="49"/>
+      <c r="B128" s="120"/>
+      <c r="C128" s="120"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="49"/>
+      <c r="B129" s="120"/>
+      <c r="C129" s="120"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="49"/>
+      <c r="B130" s="120"/>
+      <c r="C130" s="120"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="49"/>
+      <c r="B131" s="120"/>
+      <c r="C131" s="120"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="49"/>
+      <c r="B132" s="120"/>
+      <c r="C132" s="120"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="49"/>
+      <c r="B133" s="120"/>
+      <c r="C133" s="120"/>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="49"/>
+      <c r="B134" s="120"/>
+      <c r="C134" s="120"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="49"/>
+      <c r="B135" s="120"/>
+      <c r="C135" s="120"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="49"/>
+      <c r="B136" s="120"/>
+      <c r="C136" s="120"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="49"/>
+      <c r="B137" s="120"/>
+      <c r="C137" s="120"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="49"/>
+      <c r="B138" s="120"/>
+      <c r="C138" s="120"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="49"/>
+      <c r="B139" s="49"/>
+      <c r="C139" s="120"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="49"/>
+      <c r="B140" s="49"/>
+      <c r="C140" s="120"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="49"/>
+      <c r="B141" s="49"/>
+      <c r="C141" s="120"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="49"/>
+      <c r="B142" s="49"/>
+      <c r="C142" s="120"/>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="49"/>
+      <c r="B143" s="49"/>
+      <c r="C143" s="120"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="49"/>
+      <c r="B144" s="49"/>
+      <c r="C144" s="120"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="49"/>
+      <c r="B145" s="49"/>
+      <c r="C145" s="120"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="49"/>
+      <c r="B146" s="49"/>
+      <c r="C146" s="120"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="49"/>
+      <c r="B147" s="49"/>
+      <c r="C147" s="120"/>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="49"/>
+      <c r="B148" s="49"/>
+      <c r="C148" s="120"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="49" t="s">
+        <v>427</v>
+      </c>
+      <c r="B149" s="49"/>
+      <c r="C149" s="120"/>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="124" t="s">
+        <v>398</v>
+      </c>
+      <c r="B150" s="127">
+        <f>SUM(B6,B32,B51)</f>
+        <v>1342</v>
+      </c>
+      <c r="C150" s="128" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="34" t="s">
+        <v>396</v>
+      </c>
+      <c r="B151" s="120">
+        <f>SUM(B13:B15)</f>
+        <v>7730</v>
+      </c>
+      <c r="C151" s="126" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="34" t="s">
+        <v>425</v>
+      </c>
+      <c r="B152" s="120">
+        <f>SUM(B11:B12)</f>
+        <v>5780</v>
+      </c>
+      <c r="C152" s="126" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="34" t="s">
+        <v>428</v>
+      </c>
+      <c r="B153" s="49"/>
+      <c r="C153" s="126"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="34" t="s">
+        <v>429</v>
+      </c>
+      <c r="B154" s="120">
+        <f>SUM(B29:B31)</f>
+        <v>8390</v>
+      </c>
+      <c r="C154" s="126" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="34" t="s">
+        <v>432</v>
+      </c>
+      <c r="B155" s="120">
+        <f>SUM(B37)</f>
+        <v>6235</v>
+      </c>
+      <c r="C155" s="126" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="34" t="s">
+        <v>431</v>
+      </c>
+      <c r="B156" s="120">
+        <f>SUM(B43:B45)</f>
+        <v>3995</v>
+      </c>
+      <c r="C156" s="126" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="34" t="s">
+        <v>433</v>
+      </c>
+      <c r="B157" s="120">
+        <f>SUM(B35:B36)</f>
+        <v>4445</v>
+      </c>
+      <c r="C157" s="126" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="34" t="s">
+        <v>434</v>
+      </c>
+      <c r="B158" s="120">
+        <f>SUM(B54,B38,B55,B39)</f>
+        <v>990</v>
+      </c>
+      <c r="C158" s="126" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="34" t="s">
+        <v>435</v>
+      </c>
+      <c r="B159" s="120">
+        <f>SUM(B113,B111,B110,B107,B60,B61,B42,B41)</f>
+        <v>18245</v>
+      </c>
+      <c r="C159" s="126" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="34" t="s">
+        <v>436</v>
+      </c>
+      <c r="B160" s="120">
+        <f>SUM(B114:B117,B16,B17)</f>
+        <v>1700</v>
+      </c>
+      <c r="C160" s="126" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="34" t="s">
+        <v>437</v>
+      </c>
+      <c r="B161" s="129">
+        <f>SUM(B62:B64)</f>
+        <v>3625</v>
+      </c>
+      <c r="C161" s="126" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="34" t="s">
+        <v>438</v>
+      </c>
+      <c r="B162" s="120">
+        <f>SUM(B66)</f>
+        <v>6425</v>
+      </c>
+      <c r="C162" s="126" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="34" t="s">
+        <v>439</v>
+      </c>
+      <c r="B163" s="120">
+        <f>SUM(B67:B71)</f>
+        <v>9010</v>
+      </c>
+      <c r="C163" s="126" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="34" t="s">
+        <v>440</v>
+      </c>
+      <c r="B164" s="49"/>
+      <c r="C164" s="126"/>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="34" t="s">
+        <v>441</v>
+      </c>
+      <c r="B165" s="49"/>
+      <c r="C165" s="126"/>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="34" t="s">
+        <v>442</v>
+      </c>
+      <c r="B166" s="49"/>
+      <c r="C166" s="126"/>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="34" t="s">
+        <v>443</v>
+      </c>
+      <c r="B167" s="49"/>
+      <c r="C167" s="126"/>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="34" t="s">
+        <v>444</v>
+      </c>
+      <c r="B168" s="49"/>
+      <c r="C168" s="126"/>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="34" t="s">
+        <v>445</v>
+      </c>
+      <c r="B169" s="49"/>
+      <c r="C169" s="126"/>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="34" t="s">
+        <v>446</v>
+      </c>
+      <c r="B170" s="49"/>
+      <c r="C170" s="126"/>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="49"/>
+      <c r="B171" s="49"/>
+      <c r="C171" s="126"/>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="49"/>
+      <c r="B172" s="49"/>
+      <c r="C172" s="126"/>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="49"/>
+      <c r="B173" s="49"/>
+      <c r="C173" s="126"/>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="49"/>
+      <c r="B174" s="49"/>
+      <c r="C174" s="126"/>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="49"/>
+      <c r="B175" s="49"/>
+      <c r="C175" s="126"/>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="49"/>
+      <c r="B176" s="49"/>
+      <c r="C176" s="126"/>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="49"/>
+      <c r="B177" s="49"/>
+      <c r="C177" s="126"/>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="49"/>
+      <c r="B178" s="49"/>
+      <c r="C178" s="126"/>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="49"/>
+      <c r="B179" s="49"/>
+      <c r="C179" s="126"/>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="49"/>
+      <c r="B180" s="49"/>
+      <c r="C180" s="126"/>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="49"/>
+      <c r="B181" s="49"/>
+      <c r="C181" s="126"/>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="49"/>
+      <c r="B182" s="49"/>
+      <c r="C182" s="126"/>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="49"/>
+      <c r="B183" s="49"/>
+      <c r="C183" s="126"/>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="49"/>
+      <c r="B184" s="49"/>
+      <c r="C184" s="126"/>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" s="49"/>
+      <c r="B185" s="49"/>
+      <c r="C185" s="126"/>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" s="49"/>
+      <c r="B186" s="49"/>
+      <c r="C186" s="126"/>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="49"/>
+      <c r="B187" s="49"/>
+      <c r="C187" s="126"/>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="49"/>
+      <c r="B188" s="49"/>
+      <c r="C188" s="126"/>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="49"/>
+      <c r="B189" s="49"/>
+      <c r="C189" s="126"/>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" s="49"/>
+      <c r="B190" s="49"/>
+      <c r="C190" s="126"/>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" s="49"/>
+      <c r="B191" s="49"/>
+      <c r="C191" s="126"/>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="49"/>
+      <c r="B192" s="49"/>
+      <c r="C192" s="126"/>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" s="49"/>
+      <c r="B193" s="49"/>
+      <c r="C193" s="126"/>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" s="49"/>
+      <c r="B194" s="49"/>
+      <c r="C194" s="126"/>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" s="49"/>
+      <c r="B195" s="49"/>
+      <c r="C195" s="126"/>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" s="49"/>
+      <c r="B196" s="49"/>
+      <c r="C196" s="126"/>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" s="49"/>
+      <c r="B197" s="49"/>
+      <c r="C197" s="126"/>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" s="49"/>
+      <c r="B198" s="49"/>
+      <c r="C198" s="126"/>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" s="49"/>
+      <c r="B199" s="49"/>
+      <c r="C199" s="126"/>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" s="49"/>
+      <c r="B200" s="49"/>
+      <c r="C200" s="126"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B151:B152 B154 B156:B157 B160:B161 B163" formulaRange="1"/>
+    <ignoredError sqref="C29:C32 C23 C18 C11:C15 C6 C51 C53 C57 C72:C74 C91 C87:C89 C103:C105 C109 C118 C150:C152 C154 C43:C44 C156 C45 C37" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
correct column heading in priceproductgroups spreadsheet
</commit_message>
<xml_diff>
--- a/Regression/templates/PriceProductGroups.xlsx
+++ b/Regression/templates/PriceProductGroups.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="22995" windowHeight="10035" tabRatio="706" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="22995" windowHeight="10035" tabRatio="706" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="AlphazoneMakeCounties" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3698" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3698" uniqueCount="513">
   <si>
     <t>KBB Elite</t>
   </si>
@@ -1560,6 +1560,9 @@
   </si>
   <si>
     <t>Connect Core</t>
+  </si>
+  <si>
+    <t>LeaderboardUsedClickThruURL</t>
   </si>
 </sst>
 </file>
@@ -3417,7 +3420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
@@ -9651,8 +9654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CP138"/>
   <sheetViews>
-    <sheetView topLeftCell="BD1" workbookViewId="0">
-      <selection activeCell="BF9" sqref="BF9"/>
+    <sheetView tabSelected="1" topLeftCell="BC1" workbookViewId="0">
+      <selection activeCell="BG1" sqref="BG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9783,7 +9786,7 @@
         <v>242</v>
       </c>
       <c r="AI1" s="68" t="s">
-        <v>212</v>
+        <v>512</v>
       </c>
       <c r="AJ1" s="119" t="s">
         <v>243</v>
@@ -9855,7 +9858,7 @@
         <v>215</v>
       </c>
       <c r="BG1" s="68" t="s">
-        <v>508</v>
+        <v>216</v>
       </c>
       <c r="BH1" s="68" t="s">
         <v>217</v>
@@ -16902,7 +16905,7 @@
       <c r="D2" s="51"/>
       <c r="E2" s="52">
         <f t="shared" ref="E2:E33" ca="1" si="0">TODAY()</f>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F2" s="51"/>
       <c r="G2" s="51"/>
@@ -17091,7 +17094,7 @@
       <c r="D3" s="51"/>
       <c r="E3" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F3" s="51"/>
       <c r="G3" s="51"/>
@@ -17280,7 +17283,7 @@
       <c r="D4" s="51"/>
       <c r="E4" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="51"/>
@@ -17469,7 +17472,7 @@
       <c r="D5" s="51"/>
       <c r="E5" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F5" s="51"/>
       <c r="G5" s="51"/>
@@ -17660,7 +17663,7 @@
       <c r="D6" s="51"/>
       <c r="E6" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F6" s="51" t="s">
         <v>263</v>
@@ -17875,7 +17878,7 @@
       <c r="D7" s="51"/>
       <c r="E7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
@@ -18076,7 +18079,7 @@
       <c r="D8" s="51"/>
       <c r="E8" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F8" s="51"/>
       <c r="G8" s="51"/>
@@ -18279,7 +18282,7 @@
       <c r="D9" s="51"/>
       <c r="E9" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
@@ -18476,7 +18479,7 @@
       <c r="D10" s="51"/>
       <c r="E10" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
@@ -18727,7 +18730,7 @@
       <c r="D11" s="51"/>
       <c r="E11" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
@@ -18980,7 +18983,7 @@
       <c r="D12" s="51"/>
       <c r="E12" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
@@ -19233,7 +19236,7 @@
       <c r="D13" s="51"/>
       <c r="E13" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F13" s="51"/>
       <c r="G13" s="51"/>
@@ -19466,7 +19469,7 @@
       <c r="D14" s="51"/>
       <c r="E14" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F14" s="51"/>
       <c r="G14" s="51"/>
@@ -19703,7 +19706,7 @@
       <c r="D15" s="51"/>
       <c r="E15" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F15" s="51"/>
       <c r="G15" s="51"/>
@@ -19936,7 +19939,7 @@
       <c r="D16" s="51"/>
       <c r="E16" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F16" s="51"/>
       <c r="G16" s="51"/>
@@ -20161,7 +20164,7 @@
       <c r="D17" s="51"/>
       <c r="E17" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F17" s="51"/>
       <c r="G17" s="51"/>
@@ -20386,7 +20389,7 @@
       <c r="D18" s="51"/>
       <c r="E18" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F18" s="51"/>
       <c r="G18" s="51"/>
@@ -20578,7 +20581,7 @@
       <c r="D19" s="51"/>
       <c r="E19" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F19" s="51"/>
       <c r="G19" s="51"/>
@@ -20767,7 +20770,7 @@
       <c r="D20" s="51"/>
       <c r="E20" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F20" s="51"/>
       <c r="G20" s="51"/>
@@ -20956,7 +20959,7 @@
       <c r="D21" s="51"/>
       <c r="E21" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F21" s="51"/>
       <c r="G21" s="51"/>
@@ -21147,7 +21150,7 @@
       <c r="D22" s="51"/>
       <c r="E22" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F22" s="51"/>
       <c r="G22" s="51"/>
@@ -21336,7 +21339,7 @@
       <c r="D23" s="51"/>
       <c r="E23" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F23" s="51"/>
       <c r="G23" s="51"/>
@@ -21563,7 +21566,7 @@
       <c r="D24" s="51"/>
       <c r="E24" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F24" s="51"/>
       <c r="G24" s="51"/>
@@ -21776,7 +21779,7 @@
       <c r="D25" s="51"/>
       <c r="E25" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F25" s="51"/>
       <c r="G25" s="51"/>
@@ -21989,7 +21992,7 @@
       <c r="D26" s="51"/>
       <c r="E26" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F26" s="51"/>
       <c r="G26" s="51"/>
@@ -22246,7 +22249,7 @@
       <c r="D27" s="51"/>
       <c r="E27" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F27" s="51"/>
       <c r="G27" s="51"/>
@@ -22503,7 +22506,7 @@
       <c r="D28" s="51"/>
       <c r="E28" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F28" s="51"/>
       <c r="G28" s="51"/>
@@ -22742,7 +22745,7 @@
       <c r="D29" s="51"/>
       <c r="E29" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F29" s="51"/>
       <c r="G29" s="51"/>
@@ -22977,7 +22980,7 @@
       <c r="D30" s="51"/>
       <c r="E30" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F30" s="51"/>
       <c r="G30" s="51"/>
@@ -23216,7 +23219,7 @@
       <c r="D31" s="51"/>
       <c r="E31" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F31" s="51"/>
       <c r="G31" s="51"/>
@@ -23453,7 +23456,7 @@
       </c>
       <c r="E32" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F32" s="51"/>
       <c r="G32" s="51"/>
@@ -23662,7 +23665,7 @@
       <c r="D33" s="51"/>
       <c r="E33" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F33" s="51"/>
       <c r="G33" s="51"/>
@@ -23869,7 +23872,7 @@
       <c r="D34" s="51"/>
       <c r="E34" s="52">
         <f t="shared" ref="E34:E65" ca="1" si="1">TODAY()</f>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F34" s="51"/>
       <c r="G34" s="51"/>
@@ -24124,7 +24127,7 @@
       <c r="D35" s="51"/>
       <c r="E35" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F35" s="51"/>
       <c r="G35" s="51"/>
@@ -24389,7 +24392,7 @@
       <c r="D36" s="51"/>
       <c r="E36" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F36" s="51"/>
       <c r="G36" s="51"/>
@@ -24654,7 +24657,7 @@
       <c r="D37" s="51"/>
       <c r="E37" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F37" s="51"/>
       <c r="G37" s="51"/>
@@ -24953,7 +24956,7 @@
       <c r="D38" s="51"/>
       <c r="E38" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F38" s="51"/>
       <c r="G38" s="51"/>
@@ -25162,7 +25165,7 @@
       <c r="D39" s="51"/>
       <c r="E39" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F39" s="51"/>
       <c r="G39" s="51"/>
@@ -25407,7 +25410,7 @@
       <c r="D40" s="51"/>
       <c r="E40" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F40" s="51"/>
       <c r="G40" s="51"/>
@@ -25618,7 +25621,7 @@
       <c r="D41" s="51"/>
       <c r="E41" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F41" s="51"/>
       <c r="G41" s="51"/>
@@ -25825,7 +25828,7 @@
       <c r="D42" s="51"/>
       <c r="E42" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F42" s="51"/>
       <c r="G42" s="51"/>
@@ -26046,7 +26049,7 @@
       <c r="D43" s="51"/>
       <c r="E43" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F43" s="51"/>
       <c r="G43" s="51"/>
@@ -26311,7 +26314,7 @@
       <c r="D44" s="51"/>
       <c r="E44" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F44" s="51"/>
       <c r="G44" s="51"/>
@@ -26576,7 +26579,7 @@
       <c r="D45" s="51"/>
       <c r="E45" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F45" s="51"/>
       <c r="G45" s="51"/>
@@ -26843,7 +26846,7 @@
       </c>
       <c r="E46" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F46" s="51"/>
       <c r="G46" s="51"/>
@@ -27056,7 +27059,7 @@
       </c>
       <c r="E47" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F47" s="51"/>
       <c r="G47" s="51"/>
@@ -27269,7 +27272,7 @@
       </c>
       <c r="E48" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F48" s="51"/>
       <c r="G48" s="51"/>
@@ -27480,7 +27483,7 @@
       </c>
       <c r="E49" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F49" s="51"/>
       <c r="G49" s="51"/>
@@ -27689,7 +27692,7 @@
       <c r="D50" s="51"/>
       <c r="E50" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F50" s="51"/>
       <c r="G50" s="51"/>
@@ -27880,7 +27883,7 @@
       <c r="D51" s="51"/>
       <c r="E51" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F51" s="51"/>
       <c r="G51" s="51"/>
@@ -28077,7 +28080,7 @@
       <c r="D52" s="51"/>
       <c r="E52" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F52" s="51"/>
       <c r="G52" s="51"/>
@@ -28270,7 +28273,7 @@
       <c r="D53" s="51"/>
       <c r="E53" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F53" s="51"/>
       <c r="G53" s="51"/>
@@ -28476,7 +28479,7 @@
       <c r="D54" s="51"/>
       <c r="E54" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F54" s="51"/>
       <c r="G54" s="51"/>
@@ -28681,7 +28684,7 @@
       <c r="D55" s="51"/>
       <c r="E55" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F55" s="51"/>
       <c r="G55" s="51"/>
@@ -28922,7 +28925,7 @@
       <c r="D56" s="51"/>
       <c r="E56" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F56" s="51"/>
       <c r="G56" s="51"/>
@@ -29127,7 +29130,7 @@
       <c r="D57" s="51"/>
       <c r="E57" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F57" s="51"/>
       <c r="G57" s="51"/>
@@ -29321,7 +29324,7 @@
       <c r="D58" s="51"/>
       <c r="E58" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F58" s="51"/>
       <c r="G58" s="51"/>
@@ -29521,7 +29524,7 @@
       <c r="D59" s="51"/>
       <c r="E59" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F59" s="51"/>
       <c r="G59" s="51"/>
@@ -29723,7 +29726,7 @@
       <c r="D60" s="51"/>
       <c r="E60" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F60" s="51"/>
       <c r="G60" s="51"/>
@@ -29920,7 +29923,7 @@
       <c r="D61" s="51"/>
       <c r="E61" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F61" s="51"/>
       <c r="G61" s="51"/>
@@ -30153,7 +30156,7 @@
       <c r="D62" s="51"/>
       <c r="E62" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F62" s="51"/>
       <c r="G62" s="51"/>
@@ -30386,7 +30389,7 @@
       <c r="D63" s="51"/>
       <c r="E63" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F63" s="51"/>
       <c r="G63" s="51"/>
@@ -30623,7 +30626,7 @@
       <c r="D64" s="51"/>
       <c r="E64" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F64" s="51"/>
       <c r="G64" s="51"/>
@@ -30856,7 +30859,7 @@
       <c r="D65" s="51"/>
       <c r="E65" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F65" s="51"/>
       <c r="G65" s="51"/>
@@ -31105,7 +31108,7 @@
       <c r="D66" s="51"/>
       <c r="E66" s="52">
         <f t="shared" ref="E66:E89" ca="1" si="2">TODAY()</f>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F66" s="51"/>
       <c r="G66" s="51"/>
@@ -31358,7 +31361,7 @@
       <c r="D67" s="51"/>
       <c r="E67" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F67" s="51"/>
       <c r="G67" s="51"/>
@@ -31595,7 +31598,7 @@
       <c r="D68" s="51"/>
       <c r="E68" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F68" s="51"/>
       <c r="G68" s="51"/>
@@ -31834,7 +31837,7 @@
       <c r="D69" s="51"/>
       <c r="E69" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F69" s="51"/>
       <c r="G69" s="51"/>
@@ -32073,7 +32076,7 @@
       <c r="D70" s="51"/>
       <c r="E70" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F70" s="51"/>
       <c r="G70" s="51"/>
@@ -32314,7 +32317,7 @@
       <c r="D71" s="51"/>
       <c r="E71" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F71" s="51"/>
       <c r="G71" s="51"/>
@@ -32551,7 +32554,7 @@
       <c r="D72" s="51"/>
       <c r="E72" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F72" s="51"/>
       <c r="G72" s="51"/>
@@ -32740,7 +32743,7 @@
       <c r="D73" s="51"/>
       <c r="E73" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F73" s="51"/>
       <c r="G73" s="51"/>
@@ -32929,7 +32932,7 @@
       <c r="D74" s="51"/>
       <c r="E74" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F74" s="51"/>
       <c r="G74" s="51"/>
@@ -33118,7 +33121,7 @@
       <c r="D75" s="51"/>
       <c r="E75" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F75" s="51"/>
       <c r="G75" s="51"/>
@@ -33367,7 +33370,7 @@
       <c r="D76" s="51"/>
       <c r="E76" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F76" s="51"/>
       <c r="G76" s="51"/>
@@ -33618,7 +33621,7 @@
       <c r="D77" s="51"/>
       <c r="E77" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F77" s="51"/>
       <c r="G77" s="51"/>
@@ -33869,7 +33872,7 @@
       <c r="D78" s="51"/>
       <c r="E78" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F78" s="51"/>
       <c r="G78" s="51"/>
@@ -34100,7 +34103,7 @@
       <c r="D79" s="51"/>
       <c r="E79" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F79" s="51"/>
       <c r="G79" s="51"/>
@@ -34335,7 +34338,7 @@
       <c r="D80" s="51"/>
       <c r="E80" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F80" s="51"/>
       <c r="G80" s="51"/>
@@ -34566,7 +34569,7 @@
       <c r="D81" s="51"/>
       <c r="E81" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F81" s="51"/>
       <c r="G81" s="51"/>
@@ -34809,7 +34812,7 @@
       <c r="D82" s="51"/>
       <c r="E82" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F82" s="51"/>
       <c r="G82" s="51"/>
@@ -35030,7 +35033,7 @@
       <c r="D83" s="51"/>
       <c r="E83" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F83" s="51"/>
       <c r="G83" s="51"/>
@@ -35279,7 +35282,7 @@
       <c r="D84" s="51"/>
       <c r="E84" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F84" s="51"/>
       <c r="G84" s="51"/>
@@ -35528,7 +35531,7 @@
       <c r="D85" s="51"/>
       <c r="E85" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F85" s="51"/>
       <c r="G85" s="51"/>
@@ -35777,7 +35780,7 @@
       <c r="D86" s="51"/>
       <c r="E86" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F86" s="51"/>
       <c r="G86" s="51"/>
@@ -36026,7 +36029,7 @@
       <c r="D87" s="51"/>
       <c r="E87" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F87" s="51"/>
       <c r="G87" s="51"/>
@@ -36217,7 +36220,7 @@
       <c r="D88" s="51"/>
       <c r="E88" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F88" s="51"/>
       <c r="G88" s="51"/>
@@ -36408,7 +36411,7 @@
       <c r="D89" s="51"/>
       <c r="E89" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F89" s="51"/>
       <c r="G89" s="51"/>
@@ -36783,7 +36786,7 @@
       <c r="D91" s="51"/>
       <c r="E91" s="52">
         <f ca="1">TODAY()</f>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F91" s="51"/>
       <c r="G91" s="51"/>
@@ -37158,7 +37161,7 @@
       <c r="D93" s="51"/>
       <c r="E93" s="52">
         <f t="shared" ref="E93:E118" ca="1" si="3">TODAY()</f>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F93" s="51"/>
       <c r="G93" s="51"/>
@@ -37375,7 +37378,7 @@
       <c r="D94" s="51"/>
       <c r="E94" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F94" s="51"/>
       <c r="G94" s="51"/>
@@ -37592,7 +37595,7 @@
       <c r="D95" s="51"/>
       <c r="E95" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F95" s="51"/>
       <c r="G95" s="51"/>
@@ -37807,7 +37810,7 @@
       <c r="D96" s="51"/>
       <c r="E96" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F96" s="51"/>
       <c r="G96" s="51"/>
@@ -38020,7 +38023,7 @@
       <c r="D97" s="51"/>
       <c r="E97" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F97" s="51"/>
       <c r="G97" s="51"/>
@@ -38220,7 +38223,7 @@
       <c r="D98" s="51"/>
       <c r="E98" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F98" s="51"/>
       <c r="G98" s="51"/>
@@ -38420,7 +38423,7 @@
       <c r="D99" s="51"/>
       <c r="E99" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F99" s="51"/>
       <c r="G99" s="51"/>
@@ -38622,7 +38625,7 @@
       <c r="D100" s="51"/>
       <c r="E100" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F100" s="51"/>
       <c r="G100" s="51"/>
@@ -38824,7 +38827,7 @@
       <c r="D101" s="51"/>
       <c r="E101" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F101" s="51"/>
       <c r="G101" s="51"/>
@@ -39026,7 +39029,7 @@
       <c r="D102" s="51"/>
       <c r="E102" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F102" s="51"/>
       <c r="G102" s="51"/>
@@ -39228,7 +39231,7 @@
       <c r="D103" s="51"/>
       <c r="E103" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F103" s="51"/>
       <c r="G103" s="51"/>
@@ -39429,7 +39432,7 @@
       <c r="D104" s="51"/>
       <c r="E104" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F104" s="51"/>
       <c r="G104" s="51"/>
@@ -39646,7 +39649,7 @@
       <c r="D105" s="51"/>
       <c r="E105" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F105" s="51"/>
       <c r="G105" s="51"/>
@@ -39863,7 +39866,7 @@
       <c r="D106" s="51"/>
       <c r="E106" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F106" s="51"/>
       <c r="G106" s="51"/>
@@ -40080,7 +40083,7 @@
       <c r="D107" s="51"/>
       <c r="E107" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F107" s="51"/>
       <c r="G107" s="51"/>
@@ -40297,7 +40300,7 @@
       <c r="D108" s="51"/>
       <c r="E108" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F108" s="51"/>
       <c r="G108" s="51"/>
@@ -40514,7 +40517,7 @@
       <c r="D109" s="51"/>
       <c r="E109" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F109" s="51"/>
       <c r="G109" s="51"/>
@@ -40731,7 +40734,7 @@
       <c r="D110" s="51"/>
       <c r="E110" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F110" s="51"/>
       <c r="G110" s="51"/>
@@ -40948,7 +40951,7 @@
       <c r="D111" s="51"/>
       <c r="E111" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F111" s="51"/>
       <c r="G111" s="51"/>
@@ -41165,7 +41168,7 @@
       <c r="D112" s="51"/>
       <c r="E112" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F112" s="51"/>
       <c r="G112" s="51"/>
@@ -41382,7 +41385,7 @@
       <c r="D113" s="51"/>
       <c r="E113" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F113" s="51"/>
       <c r="G113" s="51"/>
@@ -41599,7 +41602,7 @@
       <c r="D114" s="51"/>
       <c r="E114" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F114" s="51"/>
       <c r="G114" s="51"/>
@@ -41788,7 +41791,7 @@
       <c r="D115" s="51"/>
       <c r="E115" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F115" s="51"/>
       <c r="G115" s="51"/>
@@ -41977,7 +41980,7 @@
       <c r="D116" s="51"/>
       <c r="E116" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F116" s="51"/>
       <c r="G116" s="51"/>
@@ -42166,7 +42169,7 @@
       <c r="D117" s="51"/>
       <c r="E117" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F117" s="51"/>
       <c r="G117" s="51"/>
@@ -42355,7 +42358,7 @@
       <c r="D118" s="51"/>
       <c r="E118" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="F118" s="51"/>
       <c r="G118" s="51"/>

</xml_diff>

<commit_message>
fixing scenario and pricing tests
</commit_message>
<xml_diff>
--- a/Regression/templates/PriceProductGroups.xlsx
+++ b/Regression/templates/PriceProductGroups.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="22995" windowHeight="10035" tabRatio="706" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="22995" windowHeight="10035" tabRatio="706" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="AlphazoneMakeCounties" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3696" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3696" uniqueCount="513">
   <si>
     <t>KBB Elite</t>
   </si>
@@ -1346,18 +1346,9 @@
     <t>UsedCarNonPremiumPriceTotal</t>
   </si>
   <si>
-    <t>$2,025.00</t>
-  </si>
-  <si>
-    <t>$270.00</t>
-  </si>
-  <si>
     <t>$1,700.00</t>
   </si>
   <si>
-    <t>$3,995.00</t>
-  </si>
-  <si>
     <t>$2,375.00</t>
   </si>
   <si>
@@ -1532,9 +1523,6 @@
     <t>/Trade In Marketplace - KBB Buying Center</t>
   </si>
   <si>
-    <t>$4,625.00</t>
-  </si>
-  <si>
     <t>Escape</t>
   </si>
   <si>
@@ -1560,6 +1548,21 @@
   </si>
   <si>
     <t>$5,975.00</t>
+  </si>
+  <si>
+    <t>$4,790.00</t>
+  </si>
+  <si>
+    <t>$2,175.00</t>
+  </si>
+  <si>
+    <t>$235.00</t>
+  </si>
+  <si>
+    <t>$1,490.00</t>
+  </si>
+  <si>
+    <t>$3,900.00</t>
   </si>
 </sst>
 </file>
@@ -3654,12 +3657,12 @@
     </row>
     <row r="2" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
   </sheetData>
@@ -3672,7 +3675,7 @@
   <dimension ref="A1:FQ21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4864,7 +4867,7 @@
       <c r="U6" s="8"/>
       <c r="V6" s="8"/>
       <c r="W6" s="132" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="X6" s="8"/>
       <c r="Y6" s="8"/>
@@ -5781,7 +5784,9 @@
       <c r="B10" s="81">
         <v>42622</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="35">
+        <v>345</v>
+      </c>
       <c r="D10" s="35"/>
       <c r="E10" s="31"/>
       <c r="F10" s="31"/>
@@ -5802,7 +5807,9 @@
       </c>
       <c r="L10" s="31"/>
       <c r="M10" s="31"/>
-      <c r="N10" s="2"/>
+      <c r="N10" s="35">
+        <v>789</v>
+      </c>
       <c r="O10" s="35" t="s">
         <v>192</v>
       </c>
@@ -8584,7 +8591,7 @@
         <v>215</v>
       </c>
       <c r="AL1" s="68" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="AM1" s="68" t="s">
         <v>217</v>
@@ -9786,7 +9793,7 @@
         <v>242</v>
       </c>
       <c r="AI1" s="68" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="AJ1" s="119" t="s">
         <v>243</v>
@@ -9858,7 +9865,7 @@
         <v>215</v>
       </c>
       <c r="BG1" s="68" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="BH1" s="68" t="s">
         <v>217</v>
@@ -13617,7 +13624,7 @@
     </row>
     <row r="2" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B2" s="93" t="s">
         <v>382</v>
@@ -13639,7 +13646,7 @@
     </row>
     <row r="3" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B3" s="93" t="s">
         <v>382</v>
@@ -14158,7 +14165,7 @@
     </row>
     <row r="19" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B19" s="93" t="s">
         <v>382</v>
@@ -14640,7 +14647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
@@ -16903,7 +16910,7 @@
       <c r="D2" s="51"/>
       <c r="E2" s="52">
         <f t="shared" ref="E2:E33" ca="1" si="0">TODAY()</f>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F2" s="51"/>
       <c r="G2" s="51"/>
@@ -17092,7 +17099,7 @@
       <c r="D3" s="51"/>
       <c r="E3" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F3" s="51"/>
       <c r="G3" s="51"/>
@@ -17281,7 +17288,7 @@
       <c r="D4" s="51"/>
       <c r="E4" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="51"/>
@@ -17470,7 +17477,7 @@
       <c r="D5" s="51"/>
       <c r="E5" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F5" s="51"/>
       <c r="G5" s="51"/>
@@ -17661,7 +17668,7 @@
       <c r="D6" s="51"/>
       <c r="E6" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F6" s="51" t="s">
         <v>263</v>
@@ -17876,7 +17883,7 @@
       <c r="D7" s="51"/>
       <c r="E7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
@@ -18077,7 +18084,7 @@
       <c r="D8" s="51"/>
       <c r="E8" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F8" s="51"/>
       <c r="G8" s="51"/>
@@ -18280,7 +18287,7 @@
       <c r="D9" s="51"/>
       <c r="E9" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
@@ -18477,7 +18484,7 @@
       <c r="D10" s="51"/>
       <c r="E10" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
@@ -18728,7 +18735,7 @@
       <c r="D11" s="51"/>
       <c r="E11" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
@@ -18981,7 +18988,7 @@
       <c r="D12" s="51"/>
       <c r="E12" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
@@ -19234,7 +19241,7 @@
       <c r="D13" s="51"/>
       <c r="E13" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F13" s="51"/>
       <c r="G13" s="51"/>
@@ -19467,7 +19474,7 @@
       <c r="D14" s="51"/>
       <c r="E14" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F14" s="51"/>
       <c r="G14" s="51"/>
@@ -19704,7 +19711,7 @@
       <c r="D15" s="51"/>
       <c r="E15" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F15" s="51"/>
       <c r="G15" s="51"/>
@@ -19937,7 +19944,7 @@
       <c r="D16" s="51"/>
       <c r="E16" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F16" s="51"/>
       <c r="G16" s="51"/>
@@ -20162,7 +20169,7 @@
       <c r="D17" s="51"/>
       <c r="E17" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F17" s="51"/>
       <c r="G17" s="51"/>
@@ -20387,7 +20394,7 @@
       <c r="D18" s="51"/>
       <c r="E18" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F18" s="51"/>
       <c r="G18" s="51"/>
@@ -20579,7 +20586,7 @@
       <c r="D19" s="51"/>
       <c r="E19" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F19" s="51"/>
       <c r="G19" s="51"/>
@@ -20768,7 +20775,7 @@
       <c r="D20" s="51"/>
       <c r="E20" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F20" s="51"/>
       <c r="G20" s="51"/>
@@ -20957,7 +20964,7 @@
       <c r="D21" s="51"/>
       <c r="E21" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F21" s="51"/>
       <c r="G21" s="51"/>
@@ -21148,7 +21155,7 @@
       <c r="D22" s="51"/>
       <c r="E22" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F22" s="51"/>
       <c r="G22" s="51"/>
@@ -21337,7 +21344,7 @@
       <c r="D23" s="51"/>
       <c r="E23" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F23" s="51"/>
       <c r="G23" s="51"/>
@@ -21564,7 +21571,7 @@
       <c r="D24" s="51"/>
       <c r="E24" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F24" s="51"/>
       <c r="G24" s="51"/>
@@ -21777,7 +21784,7 @@
       <c r="D25" s="51"/>
       <c r="E25" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F25" s="51"/>
       <c r="G25" s="51"/>
@@ -21990,7 +21997,7 @@
       <c r="D26" s="51"/>
       <c r="E26" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F26" s="51"/>
       <c r="G26" s="51"/>
@@ -22247,7 +22254,7 @@
       <c r="D27" s="51"/>
       <c r="E27" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F27" s="51"/>
       <c r="G27" s="51"/>
@@ -22504,7 +22511,7 @@
       <c r="D28" s="51"/>
       <c r="E28" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F28" s="51"/>
       <c r="G28" s="51"/>
@@ -22743,7 +22750,7 @@
       <c r="D29" s="51"/>
       <c r="E29" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F29" s="51"/>
       <c r="G29" s="51"/>
@@ -22978,7 +22985,7 @@
       <c r="D30" s="51"/>
       <c r="E30" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F30" s="51"/>
       <c r="G30" s="51"/>
@@ -23217,7 +23224,7 @@
       <c r="D31" s="51"/>
       <c r="E31" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F31" s="51"/>
       <c r="G31" s="51"/>
@@ -23454,7 +23461,7 @@
       </c>
       <c r="E32" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F32" s="51"/>
       <c r="G32" s="51"/>
@@ -23663,7 +23670,7 @@
       <c r="D33" s="51"/>
       <c r="E33" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F33" s="51"/>
       <c r="G33" s="51"/>
@@ -23870,7 +23877,7 @@
       <c r="D34" s="51"/>
       <c r="E34" s="52">
         <f t="shared" ref="E34:E65" ca="1" si="1">TODAY()</f>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F34" s="51"/>
       <c r="G34" s="51"/>
@@ -24125,7 +24132,7 @@
       <c r="D35" s="51"/>
       <c r="E35" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F35" s="51"/>
       <c r="G35" s="51"/>
@@ -24390,7 +24397,7 @@
       <c r="D36" s="51"/>
       <c r="E36" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F36" s="51"/>
       <c r="G36" s="51"/>
@@ -24655,7 +24662,7 @@
       <c r="D37" s="51"/>
       <c r="E37" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F37" s="51"/>
       <c r="G37" s="51"/>
@@ -24954,7 +24961,7 @@
       <c r="D38" s="51"/>
       <c r="E38" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F38" s="51"/>
       <c r="G38" s="51"/>
@@ -25163,7 +25170,7 @@
       <c r="D39" s="51"/>
       <c r="E39" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F39" s="51"/>
       <c r="G39" s="51"/>
@@ -25408,7 +25415,7 @@
       <c r="D40" s="51"/>
       <c r="E40" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F40" s="51"/>
       <c r="G40" s="51"/>
@@ -25619,7 +25626,7 @@
       <c r="D41" s="51"/>
       <c r="E41" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F41" s="51"/>
       <c r="G41" s="51"/>
@@ -25826,7 +25833,7 @@
       <c r="D42" s="51"/>
       <c r="E42" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F42" s="51"/>
       <c r="G42" s="51"/>
@@ -26047,7 +26054,7 @@
       <c r="D43" s="51"/>
       <c r="E43" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F43" s="51"/>
       <c r="G43" s="51"/>
@@ -26312,7 +26319,7 @@
       <c r="D44" s="51"/>
       <c r="E44" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F44" s="51"/>
       <c r="G44" s="51"/>
@@ -26577,7 +26584,7 @@
       <c r="D45" s="51"/>
       <c r="E45" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F45" s="51"/>
       <c r="G45" s="51"/>
@@ -26844,7 +26851,7 @@
       </c>
       <c r="E46" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F46" s="51"/>
       <c r="G46" s="51"/>
@@ -27057,7 +27064,7 @@
       </c>
       <c r="E47" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F47" s="51"/>
       <c r="G47" s="51"/>
@@ -27270,7 +27277,7 @@
       </c>
       <c r="E48" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F48" s="51"/>
       <c r="G48" s="51"/>
@@ -27481,7 +27488,7 @@
       </c>
       <c r="E49" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F49" s="51"/>
       <c r="G49" s="51"/>
@@ -27690,7 +27697,7 @@
       <c r="D50" s="51"/>
       <c r="E50" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F50" s="51"/>
       <c r="G50" s="51"/>
@@ -27881,7 +27888,7 @@
       <c r="D51" s="51"/>
       <c r="E51" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F51" s="51"/>
       <c r="G51" s="51"/>
@@ -28078,7 +28085,7 @@
       <c r="D52" s="51"/>
       <c r="E52" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F52" s="51"/>
       <c r="G52" s="51"/>
@@ -28271,7 +28278,7 @@
       <c r="D53" s="51"/>
       <c r="E53" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F53" s="51"/>
       <c r="G53" s="51"/>
@@ -28477,7 +28484,7 @@
       <c r="D54" s="51"/>
       <c r="E54" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F54" s="51"/>
       <c r="G54" s="51"/>
@@ -28682,7 +28689,7 @@
       <c r="D55" s="51"/>
       <c r="E55" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F55" s="51"/>
       <c r="G55" s="51"/>
@@ -28923,7 +28930,7 @@
       <c r="D56" s="51"/>
       <c r="E56" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F56" s="51"/>
       <c r="G56" s="51"/>
@@ -29128,7 +29135,7 @@
       <c r="D57" s="51"/>
       <c r="E57" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F57" s="51"/>
       <c r="G57" s="51"/>
@@ -29322,7 +29329,7 @@
       <c r="D58" s="51"/>
       <c r="E58" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F58" s="51"/>
       <c r="G58" s="51"/>
@@ -29522,7 +29529,7 @@
       <c r="D59" s="51"/>
       <c r="E59" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F59" s="51"/>
       <c r="G59" s="51"/>
@@ -29724,7 +29731,7 @@
       <c r="D60" s="51"/>
       <c r="E60" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F60" s="51"/>
       <c r="G60" s="51"/>
@@ -29921,7 +29928,7 @@
       <c r="D61" s="51"/>
       <c r="E61" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F61" s="51"/>
       <c r="G61" s="51"/>
@@ -30154,7 +30161,7 @@
       <c r="D62" s="51"/>
       <c r="E62" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F62" s="51"/>
       <c r="G62" s="51"/>
@@ -30387,7 +30394,7 @@
       <c r="D63" s="51"/>
       <c r="E63" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F63" s="51"/>
       <c r="G63" s="51"/>
@@ -30624,7 +30631,7 @@
       <c r="D64" s="51"/>
       <c r="E64" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F64" s="51"/>
       <c r="G64" s="51"/>
@@ -30857,7 +30864,7 @@
       <c r="D65" s="51"/>
       <c r="E65" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F65" s="51"/>
       <c r="G65" s="51"/>
@@ -31106,7 +31113,7 @@
       <c r="D66" s="51"/>
       <c r="E66" s="52">
         <f t="shared" ref="E66:E89" ca="1" si="2">TODAY()</f>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F66" s="51"/>
       <c r="G66" s="51"/>
@@ -31359,7 +31366,7 @@
       <c r="D67" s="51"/>
       <c r="E67" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F67" s="51"/>
       <c r="G67" s="51"/>
@@ -31596,7 +31603,7 @@
       <c r="D68" s="51"/>
       <c r="E68" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F68" s="51"/>
       <c r="G68" s="51"/>
@@ -31835,7 +31842,7 @@
       <c r="D69" s="51"/>
       <c r="E69" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F69" s="51"/>
       <c r="G69" s="51"/>
@@ -32074,7 +32081,7 @@
       <c r="D70" s="51"/>
       <c r="E70" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F70" s="51"/>
       <c r="G70" s="51"/>
@@ -32315,7 +32322,7 @@
       <c r="D71" s="51"/>
       <c r="E71" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F71" s="51"/>
       <c r="G71" s="51"/>
@@ -32552,7 +32559,7 @@
       <c r="D72" s="51"/>
       <c r="E72" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F72" s="51"/>
       <c r="G72" s="51"/>
@@ -32741,7 +32748,7 @@
       <c r="D73" s="51"/>
       <c r="E73" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F73" s="51"/>
       <c r="G73" s="51"/>
@@ -32930,7 +32937,7 @@
       <c r="D74" s="51"/>
       <c r="E74" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F74" s="51"/>
       <c r="G74" s="51"/>
@@ -33119,7 +33126,7 @@
       <c r="D75" s="51"/>
       <c r="E75" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F75" s="51"/>
       <c r="G75" s="51"/>
@@ -33368,7 +33375,7 @@
       <c r="D76" s="51"/>
       <c r="E76" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F76" s="51"/>
       <c r="G76" s="51"/>
@@ -33619,7 +33626,7 @@
       <c r="D77" s="51"/>
       <c r="E77" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F77" s="51"/>
       <c r="G77" s="51"/>
@@ -33870,7 +33877,7 @@
       <c r="D78" s="51"/>
       <c r="E78" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F78" s="51"/>
       <c r="G78" s="51"/>
@@ -34101,7 +34108,7 @@
       <c r="D79" s="51"/>
       <c r="E79" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F79" s="51"/>
       <c r="G79" s="51"/>
@@ -34336,7 +34343,7 @@
       <c r="D80" s="51"/>
       <c r="E80" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F80" s="51"/>
       <c r="G80" s="51"/>
@@ -34567,7 +34574,7 @@
       <c r="D81" s="51"/>
       <c r="E81" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F81" s="51"/>
       <c r="G81" s="51"/>
@@ -34810,7 +34817,7 @@
       <c r="D82" s="51"/>
       <c r="E82" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F82" s="51"/>
       <c r="G82" s="51"/>
@@ -35031,7 +35038,7 @@
       <c r="D83" s="51"/>
       <c r="E83" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F83" s="51"/>
       <c r="G83" s="51"/>
@@ -35280,7 +35287,7 @@
       <c r="D84" s="51"/>
       <c r="E84" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F84" s="51"/>
       <c r="G84" s="51"/>
@@ -35529,7 +35536,7 @@
       <c r="D85" s="51"/>
       <c r="E85" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F85" s="51"/>
       <c r="G85" s="51"/>
@@ -35778,7 +35785,7 @@
       <c r="D86" s="51"/>
       <c r="E86" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F86" s="51"/>
       <c r="G86" s="51"/>
@@ -36027,7 +36034,7 @@
       <c r="D87" s="51"/>
       <c r="E87" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F87" s="51"/>
       <c r="G87" s="51"/>
@@ -36218,7 +36225,7 @@
       <c r="D88" s="51"/>
       <c r="E88" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F88" s="51"/>
       <c r="G88" s="51"/>
@@ -36409,7 +36416,7 @@
       <c r="D89" s="51"/>
       <c r="E89" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F89" s="51"/>
       <c r="G89" s="51"/>
@@ -36784,7 +36791,7 @@
       <c r="D91" s="51"/>
       <c r="E91" s="52">
         <f ca="1">TODAY()</f>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F91" s="51"/>
       <c r="G91" s="51"/>
@@ -37159,7 +37166,7 @@
       <c r="D93" s="51"/>
       <c r="E93" s="52">
         <f t="shared" ref="E93:E118" ca="1" si="3">TODAY()</f>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F93" s="51"/>
       <c r="G93" s="51"/>
@@ -37376,7 +37383,7 @@
       <c r="D94" s="51"/>
       <c r="E94" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F94" s="51"/>
       <c r="G94" s="51"/>
@@ -37593,7 +37600,7 @@
       <c r="D95" s="51"/>
       <c r="E95" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F95" s="51"/>
       <c r="G95" s="51"/>
@@ -37808,7 +37815,7 @@
       <c r="D96" s="51"/>
       <c r="E96" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F96" s="51"/>
       <c r="G96" s="51"/>
@@ -38021,7 +38028,7 @@
       <c r="D97" s="51"/>
       <c r="E97" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F97" s="51"/>
       <c r="G97" s="51"/>
@@ -38221,7 +38228,7 @@
       <c r="D98" s="51"/>
       <c r="E98" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F98" s="51"/>
       <c r="G98" s="51"/>
@@ -38421,7 +38428,7 @@
       <c r="D99" s="51"/>
       <c r="E99" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F99" s="51"/>
       <c r="G99" s="51"/>
@@ -38623,7 +38630,7 @@
       <c r="D100" s="51"/>
       <c r="E100" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F100" s="51"/>
       <c r="G100" s="51"/>
@@ -38825,7 +38832,7 @@
       <c r="D101" s="51"/>
       <c r="E101" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F101" s="51"/>
       <c r="G101" s="51"/>
@@ -39027,7 +39034,7 @@
       <c r="D102" s="51"/>
       <c r="E102" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F102" s="51"/>
       <c r="G102" s="51"/>
@@ -39229,7 +39236,7 @@
       <c r="D103" s="51"/>
       <c r="E103" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F103" s="51"/>
       <c r="G103" s="51"/>
@@ -39430,7 +39437,7 @@
       <c r="D104" s="51"/>
       <c r="E104" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F104" s="51"/>
       <c r="G104" s="51"/>
@@ -39647,7 +39654,7 @@
       <c r="D105" s="51"/>
       <c r="E105" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F105" s="51"/>
       <c r="G105" s="51"/>
@@ -39864,7 +39871,7 @@
       <c r="D106" s="51"/>
       <c r="E106" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F106" s="51"/>
       <c r="G106" s="51"/>
@@ -40081,7 +40088,7 @@
       <c r="D107" s="51"/>
       <c r="E107" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F107" s="51"/>
       <c r="G107" s="51"/>
@@ -40298,7 +40305,7 @@
       <c r="D108" s="51"/>
       <c r="E108" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F108" s="51"/>
       <c r="G108" s="51"/>
@@ -40515,7 +40522,7 @@
       <c r="D109" s="51"/>
       <c r="E109" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F109" s="51"/>
       <c r="G109" s="51"/>
@@ -40732,7 +40739,7 @@
       <c r="D110" s="51"/>
       <c r="E110" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F110" s="51"/>
       <c r="G110" s="51"/>
@@ -40949,7 +40956,7 @@
       <c r="D111" s="51"/>
       <c r="E111" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F111" s="51"/>
       <c r="G111" s="51"/>
@@ -41166,7 +41173,7 @@
       <c r="D112" s="51"/>
       <c r="E112" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F112" s="51"/>
       <c r="G112" s="51"/>
@@ -41383,7 +41390,7 @@
       <c r="D113" s="51"/>
       <c r="E113" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F113" s="51"/>
       <c r="G113" s="51"/>
@@ -41600,7 +41607,7 @@
       <c r="D114" s="51"/>
       <c r="E114" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F114" s="51"/>
       <c r="G114" s="51"/>
@@ -41789,7 +41796,7 @@
       <c r="D115" s="51"/>
       <c r="E115" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F115" s="51"/>
       <c r="G115" s="51"/>
@@ -41978,7 +41985,7 @@
       <c r="D116" s="51"/>
       <c r="E116" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F116" s="51"/>
       <c r="G116" s="51"/>
@@ -42167,7 +42174,7 @@
       <c r="D117" s="51"/>
       <c r="E117" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F117" s="51"/>
       <c r="G117" s="51"/>
@@ -42356,7 +42363,7 @@
       <c r="D118" s="51"/>
       <c r="E118" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42592</v>
+        <v>42593</v>
       </c>
       <c r="F118" s="51"/>
       <c r="G118" s="51"/>
@@ -42566,8 +42573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K202"/>
   <sheetViews>
-    <sheetView topLeftCell="A149" workbookViewId="0">
-      <selection activeCell="C154" sqref="C154"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="C158" sqref="C158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42702,7 +42709,7 @@
         <v>2685</v>
       </c>
       <c r="C10" s="126" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -42724,7 +42731,7 @@
         <v>2980</v>
       </c>
       <c r="C12" s="126" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -42762,14 +42769,14 @@
     </row>
     <row r="16" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B16" s="120"/>
       <c r="C16" s="126"/>
     </row>
     <row r="17" spans="1:3" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="B17" s="120"/>
       <c r="C17" s="126"/>
@@ -42793,7 +42800,7 @@
         <v>250</v>
       </c>
       <c r="C19" s="126" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -42866,7 +42873,7 @@
         <v>1700</v>
       </c>
       <c r="C26" s="126" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -42877,7 +42884,7 @@
         <v>1120</v>
       </c>
       <c r="C27" s="126" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -42888,7 +42895,7 @@
         <v>2910</v>
       </c>
       <c r="C28" s="126" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -42909,7 +42916,7 @@
         <v>2375</v>
       </c>
       <c r="C30" s="126" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -42974,7 +42981,7 @@
         <v>2685</v>
       </c>
       <c r="C36" s="126" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -42985,7 +42992,7 @@
         <v>2375</v>
       </c>
       <c r="C37" s="126" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -42996,7 +43003,7 @@
         <v>2070</v>
       </c>
       <c r="C38" s="126" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -43004,10 +43011,10 @@
         <v>67</v>
       </c>
       <c r="B39" s="120">
-        <v>4625</v>
+        <v>4790</v>
       </c>
       <c r="C39" s="126" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -43018,7 +43025,7 @@
         <v>265</v>
       </c>
       <c r="C40" s="126" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -43029,7 +43036,7 @@
         <v>305</v>
       </c>
       <c r="C41" s="126" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -43040,7 +43047,7 @@
         <v>305</v>
       </c>
       <c r="C42" s="126" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -43051,7 +43058,7 @@
         <v>770</v>
       </c>
       <c r="C43" s="126" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -43062,7 +43069,7 @@
         <v>770</v>
       </c>
       <c r="C44" s="126" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -43070,10 +43077,10 @@
         <v>12</v>
       </c>
       <c r="B45" s="120">
-        <v>270</v>
+        <v>235</v>
       </c>
       <c r="C45" s="126" t="s">
-        <v>441</v>
+        <v>510</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -43081,10 +43088,10 @@
         <v>14</v>
       </c>
       <c r="B46" s="120">
-        <v>2025</v>
+        <v>2175</v>
       </c>
       <c r="C46" s="126" t="s">
-        <v>440</v>
+        <v>509</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -43092,10 +43099,10 @@
         <v>13</v>
       </c>
       <c r="B47" s="120">
-        <v>1700</v>
+        <v>1490</v>
       </c>
       <c r="C47" s="126" t="s">
-        <v>442</v>
+        <v>511</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -43117,7 +43124,7 @@
         <v>1800</v>
       </c>
       <c r="C49" s="126" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -43128,7 +43135,7 @@
         <v>900</v>
       </c>
       <c r="C50" s="126" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -43192,7 +43199,7 @@
         <v>190</v>
       </c>
       <c r="C56" s="126" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -43203,7 +43210,7 @@
         <v>230</v>
       </c>
       <c r="C57" s="126" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -43235,7 +43242,7 @@
         <v>135</v>
       </c>
       <c r="C60" s="126" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -43246,7 +43253,7 @@
         <v>80</v>
       </c>
       <c r="C61" s="126" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -43257,7 +43264,7 @@
         <v>770</v>
       </c>
       <c r="C62" s="126" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -43268,7 +43275,7 @@
         <v>770</v>
       </c>
       <c r="C63" s="126" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -43279,7 +43286,7 @@
         <v>490</v>
       </c>
       <c r="C64" s="126" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -43290,7 +43297,7 @@
         <v>1960</v>
       </c>
       <c r="C65" s="126" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -43301,7 +43308,7 @@
         <v>1175</v>
       </c>
       <c r="C66" s="126" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -43312,7 +43319,7 @@
         <v>2685</v>
       </c>
       <c r="C67" s="126" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -43323,7 +43330,7 @@
         <v>6425</v>
       </c>
       <c r="C68" s="126" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -43334,7 +43341,7 @@
         <v>895</v>
       </c>
       <c r="C69" s="126" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -43345,7 +43352,7 @@
         <v>540</v>
       </c>
       <c r="C70" s="126" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -43356,7 +43363,7 @@
         <v>1715</v>
       </c>
       <c r="C71" s="126" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -43367,7 +43374,7 @@
         <v>3750</v>
       </c>
       <c r="C72" s="126" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -43378,7 +43385,7 @@
         <v>1430</v>
       </c>
       <c r="C73" s="126" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -43422,7 +43429,7 @@
         <v>1120</v>
       </c>
       <c r="C77" s="126" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -43433,7 +43440,7 @@
         <v>2725</v>
       </c>
       <c r="C78" s="126" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -43444,7 +43451,7 @@
         <v>2035</v>
       </c>
       <c r="C79" s="126" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -43455,7 +43462,7 @@
         <v>690</v>
       </c>
       <c r="C80" s="126" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -43466,7 +43473,7 @@
         <v>2705</v>
       </c>
       <c r="C81" s="126" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -43477,7 +43484,7 @@
         <v>1665</v>
       </c>
       <c r="C82" s="126" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -43488,7 +43495,7 @@
         <v>3250</v>
       </c>
       <c r="C83" s="126" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -43499,7 +43506,7 @@
         <v>2725</v>
       </c>
       <c r="C84" s="126" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -43510,7 +43517,7 @@
         <v>4205</v>
       </c>
       <c r="C85" s="126" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -43521,7 +43528,7 @@
         <v>7080</v>
       </c>
       <c r="C86" s="126" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -43532,7 +43539,7 @@
         <v>3470</v>
       </c>
       <c r="C87" s="126" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -43543,7 +43550,7 @@
         <v>6430</v>
       </c>
       <c r="C88" s="126" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -43633,7 +43640,7 @@
         <v>1800</v>
       </c>
       <c r="C96" s="126" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -43644,7 +43651,7 @@
         <v>900</v>
       </c>
       <c r="C97" s="126" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -43666,7 +43673,7 @@
         <v>925</v>
       </c>
       <c r="C99" s="126" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -43677,7 +43684,7 @@
         <v>1850</v>
       </c>
       <c r="C100" s="126" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -43699,7 +43706,7 @@
         <v>1400</v>
       </c>
       <c r="C102" s="126" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -43710,7 +43717,7 @@
         <v>525</v>
       </c>
       <c r="C103" s="126" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -43721,7 +43728,7 @@
         <v>1025</v>
       </c>
       <c r="C104" s="126" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -43775,7 +43782,7 @@
         <v>2265</v>
       </c>
       <c r="C109" s="126" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -43807,7 +43814,7 @@
         <v>5595</v>
       </c>
       <c r="C112" s="126" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -43818,7 +43825,7 @@
         <v>5595</v>
       </c>
       <c r="C113" s="126" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -43839,7 +43846,7 @@
         <v>1710</v>
       </c>
       <c r="C115" s="126" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -43861,7 +43868,7 @@
         <v>250</v>
       </c>
       <c r="C117" s="126" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -43872,7 +43879,7 @@
         <v>250</v>
       </c>
       <c r="C118" s="126" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -43883,7 +43890,7 @@
         <v>350</v>
       </c>
       <c r="C119" s="126" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -44087,7 +44094,7 @@
         <v>5975</v>
       </c>
       <c r="C154" s="126" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -44115,10 +44122,10 @@
       </c>
       <c r="B157" s="120">
         <f>SUM(B39)</f>
-        <v>4625</v>
+        <v>4790</v>
       </c>
       <c r="C157" s="126" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -44127,10 +44134,10 @@
       </c>
       <c r="B158" s="120">
         <f>SUM(B45:B47)</f>
-        <v>3995</v>
+        <v>3900</v>
       </c>
       <c r="C158" s="126" t="s">
-        <v>443</v>
+        <v>512</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -44142,7 +44149,7 @@
         <v>4445</v>
       </c>
       <c r="C159" s="126" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -44154,7 +44161,7 @@
         <v>990</v>
       </c>
       <c r="C160" s="126" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -44166,7 +44173,7 @@
         <v>18245</v>
       </c>
       <c r="C161" s="126" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -44178,7 +44185,7 @@
         <v>1700</v>
       </c>
       <c r="C162" s="126" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -44190,7 +44197,7 @@
         <v>3625</v>
       </c>
       <c r="C163" s="126" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -44202,7 +44209,7 @@
         <v>6425</v>
       </c>
       <c r="C164" s="126" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -44214,7 +44221,7 @@
         <v>8330</v>
       </c>
       <c r="C165" s="126" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -44226,7 +44233,7 @@
         <v>5060</v>
       </c>
       <c r="C166" s="126" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -44238,7 +44245,7 @@
         <v>4760</v>
       </c>
       <c r="C167" s="126" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -44250,7 +44257,7 @@
         <v>27160</v>
       </c>
       <c r="C168" s="126" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -44262,7 +44269,7 @@
         <v>4800</v>
       </c>
       <c r="C169" s="126" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -44274,7 +44281,7 @@
         <v>6600</v>
       </c>
       <c r="C170" s="126" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -44286,7 +44293,7 @@
         <v>6640</v>
       </c>
       <c r="C171" s="126" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -44298,12 +44305,12 @@
         <v>16160</v>
       </c>
       <c r="C172" s="126" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="34" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="B173" s="49"/>
       <c r="C173" s="126"/>
@@ -44458,7 +44465,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="B153:B154 B156 B158:B159 B162:B163 B165:B168" formulaRange="1"/>
-    <ignoredError sqref="C31:C34 C25 C20 C13:C15 C6 C53 C55 C59 C74:C76 C93 C89:C91 C105:C107 C111 C120 C152:C153 C156 C45:C46 C158 C47" numberStoredAsText="1"/>
+    <ignoredError sqref="C31:C34 C25 C20 C13:C15 C6 C53 C55 C59 C74:C76 C93 C89:C91 C105:C107 C111 C120 C152:C153 C156" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes to tests, frontline pro step
</commit_message>
<xml_diff>
--- a/Regression/templates/PriceProductGroups.xlsx
+++ b/Regression/templates/PriceProductGroups.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="22995" windowHeight="10035" tabRatio="706" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="22995" windowHeight="10035" tabRatio="706" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="AlphazoneMakeCounties" sheetId="1" r:id="rId1"/>
@@ -1211,15 +1211,6 @@
     <t>$650.00</t>
   </si>
   <si>
-    <t>$1,050.00</t>
-  </si>
-  <si>
-    <t>$4,135.00</t>
-  </si>
-  <si>
-    <t>$2,545.00</t>
-  </si>
-  <si>
     <t>$400.00</t>
   </si>
   <si>
@@ -1274,9 +1265,6 @@
     <t>$1,342.00</t>
   </si>
   <si>
-    <t>$7,730.00</t>
-  </si>
-  <si>
     <t>$242.00</t>
   </si>
   <si>
@@ -1572,6 +1560,18 @@
   </si>
   <si>
     <t>34</t>
+  </si>
+  <si>
+    <t>$1,095.00</t>
+  </si>
+  <si>
+    <t>$4,315.00</t>
+  </si>
+  <si>
+    <t>$2,660.00</t>
+  </si>
+  <si>
+    <t>$8,070.00</t>
   </si>
 </sst>
 </file>
@@ -3433,7 +3433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BK3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+    <sheetView topLeftCell="P1" workbookViewId="0">
       <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
@@ -3610,7 +3610,7 @@
         <v>241</v>
       </c>
       <c r="AJ1" s="68" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="AK1" s="68" t="s">
         <v>242</v>
@@ -3664,7 +3664,7 @@
         <v>214</v>
       </c>
       <c r="BB1" s="68" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="BC1" s="68" t="s">
         <v>216</v>
@@ -3696,7 +3696,7 @@
     </row>
     <row r="2" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="B2" s="73">
         <v>42617</v>
@@ -3802,7 +3802,7 @@
         <v>185</v>
       </c>
       <c r="AK2" s="86" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="AL2" s="37"/>
       <c r="AM2" s="35" t="s">
@@ -3881,7 +3881,7 @@
     </row>
     <row r="3" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B3" s="73">
         <v>42617</v>
@@ -3985,7 +3985,7 @@
         <v>185</v>
       </c>
       <c r="AK3" s="86" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="AL3" s="37"/>
       <c r="AM3" s="35" t="s">
@@ -5262,7 +5262,7 @@
       <c r="U6" s="8"/>
       <c r="V6" s="8"/>
       <c r="W6" s="132" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="X6" s="8"/>
       <c r="Y6" s="8"/>
@@ -8984,7 +8984,7 @@
         <v>214</v>
       </c>
       <c r="AL1" s="68" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="AM1" s="68" t="s">
         <v>216</v>
@@ -10186,7 +10186,7 @@
         <v>241</v>
       </c>
       <c r="AI1" s="68" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="AJ1" s="119" t="s">
         <v>242</v>
@@ -10258,7 +10258,7 @@
         <v>214</v>
       </c>
       <c r="BG1" s="68" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="BH1" s="68" t="s">
         <v>216</v>
@@ -14017,7 +14017,7 @@
     </row>
     <row r="2" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B2" s="93" t="s">
         <v>381</v>
@@ -14039,7 +14039,7 @@
     </row>
     <row r="3" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="B3" s="93" t="s">
         <v>381</v>
@@ -14558,7 +14558,7 @@
     </row>
     <row r="19" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="B19" s="93" t="s">
         <v>381</v>
@@ -17303,7 +17303,7 @@
       <c r="D2" s="51"/>
       <c r="E2" s="52">
         <f t="shared" ref="E2:E33" ca="1" si="0">TODAY()</f>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F2" s="51"/>
       <c r="G2" s="51"/>
@@ -17492,7 +17492,7 @@
       <c r="D3" s="51"/>
       <c r="E3" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F3" s="51"/>
       <c r="G3" s="51"/>
@@ -17681,7 +17681,7 @@
       <c r="D4" s="51"/>
       <c r="E4" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="51"/>
@@ -17870,7 +17870,7 @@
       <c r="D5" s="51"/>
       <c r="E5" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F5" s="51"/>
       <c r="G5" s="51"/>
@@ -18061,7 +18061,7 @@
       <c r="D6" s="51"/>
       <c r="E6" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F6" s="51" t="s">
         <v>262</v>
@@ -18276,7 +18276,7 @@
       <c r="D7" s="51"/>
       <c r="E7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
@@ -18477,7 +18477,7 @@
       <c r="D8" s="51"/>
       <c r="E8" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F8" s="51"/>
       <c r="G8" s="51"/>
@@ -18680,7 +18680,7 @@
       <c r="D9" s="51"/>
       <c r="E9" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
@@ -18877,7 +18877,7 @@
       <c r="D10" s="51"/>
       <c r="E10" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
@@ -19128,7 +19128,7 @@
       <c r="D11" s="51"/>
       <c r="E11" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
@@ -19381,7 +19381,7 @@
       <c r="D12" s="51"/>
       <c r="E12" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
@@ -19634,7 +19634,7 @@
       <c r="D13" s="51"/>
       <c r="E13" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F13" s="51"/>
       <c r="G13" s="51"/>
@@ -19867,7 +19867,7 @@
       <c r="D14" s="51"/>
       <c r="E14" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F14" s="51"/>
       <c r="G14" s="51"/>
@@ -20104,7 +20104,7 @@
       <c r="D15" s="51"/>
       <c r="E15" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F15" s="51"/>
       <c r="G15" s="51"/>
@@ -20337,7 +20337,7 @@
       <c r="D16" s="51"/>
       <c r="E16" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F16" s="51"/>
       <c r="G16" s="51"/>
@@ -20562,7 +20562,7 @@
       <c r="D17" s="51"/>
       <c r="E17" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F17" s="51"/>
       <c r="G17" s="51"/>
@@ -20787,7 +20787,7 @@
       <c r="D18" s="51"/>
       <c r="E18" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F18" s="51"/>
       <c r="G18" s="51"/>
@@ -20979,7 +20979,7 @@
       <c r="D19" s="51"/>
       <c r="E19" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F19" s="51"/>
       <c r="G19" s="51"/>
@@ -21168,7 +21168,7 @@
       <c r="D20" s="51"/>
       <c r="E20" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F20" s="51"/>
       <c r="G20" s="51"/>
@@ -21357,7 +21357,7 @@
       <c r="D21" s="51"/>
       <c r="E21" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F21" s="51"/>
       <c r="G21" s="51"/>
@@ -21548,7 +21548,7 @@
       <c r="D22" s="51"/>
       <c r="E22" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F22" s="51"/>
       <c r="G22" s="51"/>
@@ -21737,7 +21737,7 @@
       <c r="D23" s="51"/>
       <c r="E23" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F23" s="51"/>
       <c r="G23" s="51"/>
@@ -21964,7 +21964,7 @@
       <c r="D24" s="51"/>
       <c r="E24" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F24" s="51"/>
       <c r="G24" s="51"/>
@@ -22177,7 +22177,7 @@
       <c r="D25" s="51"/>
       <c r="E25" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F25" s="51"/>
       <c r="G25" s="51"/>
@@ -22390,7 +22390,7 @@
       <c r="D26" s="51"/>
       <c r="E26" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F26" s="51"/>
       <c r="G26" s="51"/>
@@ -22647,7 +22647,7 @@
       <c r="D27" s="51"/>
       <c r="E27" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F27" s="51"/>
       <c r="G27" s="51"/>
@@ -22904,7 +22904,7 @@
       <c r="D28" s="51"/>
       <c r="E28" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F28" s="51"/>
       <c r="G28" s="51"/>
@@ -23143,7 +23143,7 @@
       <c r="D29" s="51"/>
       <c r="E29" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F29" s="51"/>
       <c r="G29" s="51"/>
@@ -23378,7 +23378,7 @@
       <c r="D30" s="51"/>
       <c r="E30" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F30" s="51"/>
       <c r="G30" s="51"/>
@@ -23617,7 +23617,7 @@
       <c r="D31" s="51"/>
       <c r="E31" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F31" s="51"/>
       <c r="G31" s="51"/>
@@ -23854,7 +23854,7 @@
       </c>
       <c r="E32" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F32" s="51"/>
       <c r="G32" s="51"/>
@@ -24063,7 +24063,7 @@
       <c r="D33" s="51"/>
       <c r="E33" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F33" s="51"/>
       <c r="G33" s="51"/>
@@ -24270,7 +24270,7 @@
       <c r="D34" s="51"/>
       <c r="E34" s="52">
         <f t="shared" ref="E34:E65" ca="1" si="1">TODAY()</f>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F34" s="51"/>
       <c r="G34" s="51"/>
@@ -24525,7 +24525,7 @@
       <c r="D35" s="51"/>
       <c r="E35" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F35" s="51"/>
       <c r="G35" s="51"/>
@@ -24790,7 +24790,7 @@
       <c r="D36" s="51"/>
       <c r="E36" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F36" s="51"/>
       <c r="G36" s="51"/>
@@ -25055,7 +25055,7 @@
       <c r="D37" s="51"/>
       <c r="E37" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F37" s="51"/>
       <c r="G37" s="51"/>
@@ -25354,7 +25354,7 @@
       <c r="D38" s="51"/>
       <c r="E38" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F38" s="51"/>
       <c r="G38" s="51"/>
@@ -25563,7 +25563,7 @@
       <c r="D39" s="51"/>
       <c r="E39" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F39" s="51"/>
       <c r="G39" s="51"/>
@@ -25808,7 +25808,7 @@
       <c r="D40" s="51"/>
       <c r="E40" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F40" s="51"/>
       <c r="G40" s="51"/>
@@ -26019,7 +26019,7 @@
       <c r="D41" s="51"/>
       <c r="E41" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F41" s="51"/>
       <c r="G41" s="51"/>
@@ -26226,7 +26226,7 @@
       <c r="D42" s="51"/>
       <c r="E42" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F42" s="51"/>
       <c r="G42" s="51"/>
@@ -26447,7 +26447,7 @@
       <c r="D43" s="51"/>
       <c r="E43" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F43" s="51"/>
       <c r="G43" s="51"/>
@@ -26712,7 +26712,7 @@
       <c r="D44" s="51"/>
       <c r="E44" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F44" s="51"/>
       <c r="G44" s="51"/>
@@ -26977,7 +26977,7 @@
       <c r="D45" s="51"/>
       <c r="E45" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F45" s="51"/>
       <c r="G45" s="51"/>
@@ -27244,7 +27244,7 @@
       </c>
       <c r="E46" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F46" s="51"/>
       <c r="G46" s="51"/>
@@ -27457,7 +27457,7 @@
       </c>
       <c r="E47" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F47" s="51"/>
       <c r="G47" s="51"/>
@@ -27670,7 +27670,7 @@
       </c>
       <c r="E48" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F48" s="51"/>
       <c r="G48" s="51"/>
@@ -27881,7 +27881,7 @@
       </c>
       <c r="E49" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F49" s="51"/>
       <c r="G49" s="51"/>
@@ -28090,7 +28090,7 @@
       <c r="D50" s="51"/>
       <c r="E50" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F50" s="51"/>
       <c r="G50" s="51"/>
@@ -28281,7 +28281,7 @@
       <c r="D51" s="51"/>
       <c r="E51" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F51" s="51"/>
       <c r="G51" s="51"/>
@@ -28478,7 +28478,7 @@
       <c r="D52" s="51"/>
       <c r="E52" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F52" s="51"/>
       <c r="G52" s="51"/>
@@ -28671,7 +28671,7 @@
       <c r="D53" s="51"/>
       <c r="E53" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F53" s="51"/>
       <c r="G53" s="51"/>
@@ -28877,7 +28877,7 @@
       <c r="D54" s="51"/>
       <c r="E54" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F54" s="51"/>
       <c r="G54" s="51"/>
@@ -29082,7 +29082,7 @@
       <c r="D55" s="51"/>
       <c r="E55" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F55" s="51"/>
       <c r="G55" s="51"/>
@@ -29323,7 +29323,7 @@
       <c r="D56" s="51"/>
       <c r="E56" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F56" s="51"/>
       <c r="G56" s="51"/>
@@ -29528,7 +29528,7 @@
       <c r="D57" s="51"/>
       <c r="E57" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F57" s="51"/>
       <c r="G57" s="51"/>
@@ -29722,7 +29722,7 @@
       <c r="D58" s="51"/>
       <c r="E58" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F58" s="51"/>
       <c r="G58" s="51"/>
@@ -29922,7 +29922,7 @@
       <c r="D59" s="51"/>
       <c r="E59" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F59" s="51"/>
       <c r="G59" s="51"/>
@@ -30124,7 +30124,7 @@
       <c r="D60" s="51"/>
       <c r="E60" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F60" s="51"/>
       <c r="G60" s="51"/>
@@ -30321,7 +30321,7 @@
       <c r="D61" s="51"/>
       <c r="E61" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F61" s="51"/>
       <c r="G61" s="51"/>
@@ -30554,7 +30554,7 @@
       <c r="D62" s="51"/>
       <c r="E62" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F62" s="51"/>
       <c r="G62" s="51"/>
@@ -30787,7 +30787,7 @@
       <c r="D63" s="51"/>
       <c r="E63" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F63" s="51"/>
       <c r="G63" s="51"/>
@@ -31024,7 +31024,7 @@
       <c r="D64" s="51"/>
       <c r="E64" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F64" s="51"/>
       <c r="G64" s="51"/>
@@ -31257,7 +31257,7 @@
       <c r="D65" s="51"/>
       <c r="E65" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F65" s="51"/>
       <c r="G65" s="51"/>
@@ -31506,7 +31506,7 @@
       <c r="D66" s="51"/>
       <c r="E66" s="52">
         <f t="shared" ref="E66:E89" ca="1" si="2">TODAY()</f>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F66" s="51"/>
       <c r="G66" s="51"/>
@@ -31759,7 +31759,7 @@
       <c r="D67" s="51"/>
       <c r="E67" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F67" s="51"/>
       <c r="G67" s="51"/>
@@ -31996,7 +31996,7 @@
       <c r="D68" s="51"/>
       <c r="E68" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F68" s="51"/>
       <c r="G68" s="51"/>
@@ -32235,7 +32235,7 @@
       <c r="D69" s="51"/>
       <c r="E69" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F69" s="51"/>
       <c r="G69" s="51"/>
@@ -32474,7 +32474,7 @@
       <c r="D70" s="51"/>
       <c r="E70" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F70" s="51"/>
       <c r="G70" s="51"/>
@@ -32715,7 +32715,7 @@
       <c r="D71" s="51"/>
       <c r="E71" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F71" s="51"/>
       <c r="G71" s="51"/>
@@ -32952,7 +32952,7 @@
       <c r="D72" s="51"/>
       <c r="E72" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F72" s="51"/>
       <c r="G72" s="51"/>
@@ -33141,7 +33141,7 @@
       <c r="D73" s="51"/>
       <c r="E73" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F73" s="51"/>
       <c r="G73" s="51"/>
@@ -33330,7 +33330,7 @@
       <c r="D74" s="51"/>
       <c r="E74" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F74" s="51"/>
       <c r="G74" s="51"/>
@@ -33519,7 +33519,7 @@
       <c r="D75" s="51"/>
       <c r="E75" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F75" s="51"/>
       <c r="G75" s="51"/>
@@ -33768,7 +33768,7 @@
       <c r="D76" s="51"/>
       <c r="E76" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F76" s="51"/>
       <c r="G76" s="51"/>
@@ -34019,7 +34019,7 @@
       <c r="D77" s="51"/>
       <c r="E77" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F77" s="51"/>
       <c r="G77" s="51"/>
@@ -34270,7 +34270,7 @@
       <c r="D78" s="51"/>
       <c r="E78" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F78" s="51"/>
       <c r="G78" s="51"/>
@@ -34501,7 +34501,7 @@
       <c r="D79" s="51"/>
       <c r="E79" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F79" s="51"/>
       <c r="G79" s="51"/>
@@ -34736,7 +34736,7 @@
       <c r="D80" s="51"/>
       <c r="E80" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F80" s="51"/>
       <c r="G80" s="51"/>
@@ -34967,7 +34967,7 @@
       <c r="D81" s="51"/>
       <c r="E81" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F81" s="51"/>
       <c r="G81" s="51"/>
@@ -35210,7 +35210,7 @@
       <c r="D82" s="51"/>
       <c r="E82" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F82" s="51"/>
       <c r="G82" s="51"/>
@@ -35431,7 +35431,7 @@
       <c r="D83" s="51"/>
       <c r="E83" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F83" s="51"/>
       <c r="G83" s="51"/>
@@ -35680,7 +35680,7 @@
       <c r="D84" s="51"/>
       <c r="E84" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F84" s="51"/>
       <c r="G84" s="51"/>
@@ -35929,7 +35929,7 @@
       <c r="D85" s="51"/>
       <c r="E85" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F85" s="51"/>
       <c r="G85" s="51"/>
@@ -36178,7 +36178,7 @@
       <c r="D86" s="51"/>
       <c r="E86" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F86" s="51"/>
       <c r="G86" s="51"/>
@@ -36427,7 +36427,7 @@
       <c r="D87" s="51"/>
       <c r="E87" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F87" s="51"/>
       <c r="G87" s="51"/>
@@ -36618,7 +36618,7 @@
       <c r="D88" s="51"/>
       <c r="E88" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F88" s="51"/>
       <c r="G88" s="51"/>
@@ -36809,7 +36809,7 @@
       <c r="D89" s="51"/>
       <c r="E89" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F89" s="51"/>
       <c r="G89" s="51"/>
@@ -37184,7 +37184,7 @@
       <c r="D91" s="51"/>
       <c r="E91" s="52">
         <f ca="1">TODAY()</f>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F91" s="51"/>
       <c r="G91" s="51"/>
@@ -37559,7 +37559,7 @@
       <c r="D93" s="51"/>
       <c r="E93" s="52">
         <f t="shared" ref="E93:E118" ca="1" si="3">TODAY()</f>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F93" s="51"/>
       <c r="G93" s="51"/>
@@ -37776,7 +37776,7 @@
       <c r="D94" s="51"/>
       <c r="E94" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F94" s="51"/>
       <c r="G94" s="51"/>
@@ -37993,7 +37993,7 @@
       <c r="D95" s="51"/>
       <c r="E95" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F95" s="51"/>
       <c r="G95" s="51"/>
@@ -38208,7 +38208,7 @@
       <c r="D96" s="51"/>
       <c r="E96" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F96" s="51"/>
       <c r="G96" s="51"/>
@@ -38421,7 +38421,7 @@
       <c r="D97" s="51"/>
       <c r="E97" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F97" s="51"/>
       <c r="G97" s="51"/>
@@ -38621,7 +38621,7 @@
       <c r="D98" s="51"/>
       <c r="E98" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F98" s="51"/>
       <c r="G98" s="51"/>
@@ -38821,7 +38821,7 @@
       <c r="D99" s="51"/>
       <c r="E99" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F99" s="51"/>
       <c r="G99" s="51"/>
@@ -39023,7 +39023,7 @@
       <c r="D100" s="51"/>
       <c r="E100" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F100" s="51"/>
       <c r="G100" s="51"/>
@@ -39225,7 +39225,7 @@
       <c r="D101" s="51"/>
       <c r="E101" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F101" s="51"/>
       <c r="G101" s="51"/>
@@ -39427,7 +39427,7 @@
       <c r="D102" s="51"/>
       <c r="E102" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F102" s="51"/>
       <c r="G102" s="51"/>
@@ -39629,7 +39629,7 @@
       <c r="D103" s="51"/>
       <c r="E103" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F103" s="51"/>
       <c r="G103" s="51"/>
@@ -39830,7 +39830,7 @@
       <c r="D104" s="51"/>
       <c r="E104" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F104" s="51"/>
       <c r="G104" s="51"/>
@@ -40047,7 +40047,7 @@
       <c r="D105" s="51"/>
       <c r="E105" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F105" s="51"/>
       <c r="G105" s="51"/>
@@ -40264,7 +40264,7 @@
       <c r="D106" s="51"/>
       <c r="E106" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F106" s="51"/>
       <c r="G106" s="51"/>
@@ -40481,7 +40481,7 @@
       <c r="D107" s="51"/>
       <c r="E107" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F107" s="51"/>
       <c r="G107" s="51"/>
@@ -40698,7 +40698,7 @@
       <c r="D108" s="51"/>
       <c r="E108" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F108" s="51"/>
       <c r="G108" s="51"/>
@@ -40915,7 +40915,7 @@
       <c r="D109" s="51"/>
       <c r="E109" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F109" s="51"/>
       <c r="G109" s="51"/>
@@ -41132,7 +41132,7 @@
       <c r="D110" s="51"/>
       <c r="E110" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F110" s="51"/>
       <c r="G110" s="51"/>
@@ -41349,7 +41349,7 @@
       <c r="D111" s="51"/>
       <c r="E111" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F111" s="51"/>
       <c r="G111" s="51"/>
@@ -41566,7 +41566,7 @@
       <c r="D112" s="51"/>
       <c r="E112" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F112" s="51"/>
       <c r="G112" s="51"/>
@@ -41783,7 +41783,7 @@
       <c r="D113" s="51"/>
       <c r="E113" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F113" s="51"/>
       <c r="G113" s="51"/>
@@ -42000,7 +42000,7 @@
       <c r="D114" s="51"/>
       <c r="E114" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F114" s="51"/>
       <c r="G114" s="51"/>
@@ -42189,7 +42189,7 @@
       <c r="D115" s="51"/>
       <c r="E115" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F115" s="51"/>
       <c r="G115" s="51"/>
@@ -42378,7 +42378,7 @@
       <c r="D116" s="51"/>
       <c r="E116" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F116" s="51"/>
       <c r="G116" s="51"/>
@@ -42567,7 +42567,7 @@
       <c r="D117" s="51"/>
       <c r="E117" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F117" s="51"/>
       <c r="G117" s="51"/>
@@ -42756,7 +42756,7 @@
       <c r="D118" s="51"/>
       <c r="E118" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="F118" s="51"/>
       <c r="G118" s="51"/>
@@ -42966,8 +42966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K202"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="A173" sqref="A173"/>
+    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="C153" sqref="C153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43102,7 +43102,7 @@
         <v>2685</v>
       </c>
       <c r="C10" s="126" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -43113,7 +43113,7 @@
         <v>2995</v>
       </c>
       <c r="C11" s="126" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -43124,7 +43124,7 @@
         <v>2980</v>
       </c>
       <c r="C12" s="126" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -43132,10 +43132,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="120">
-        <v>1050</v>
+        <v>1095</v>
       </c>
       <c r="C13" s="126" t="s">
-        <v>395</v>
+        <v>512</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -43143,10 +43143,10 @@
         <v>8</v>
       </c>
       <c r="B14" s="120">
-        <v>4135</v>
+        <v>4315</v>
       </c>
       <c r="C14" s="126" t="s">
-        <v>396</v>
+        <v>513</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -43154,32 +43154,32 @@
         <v>7</v>
       </c>
       <c r="B15" s="120">
-        <v>2545</v>
+        <v>2660</v>
       </c>
       <c r="C15" s="126" t="s">
-        <v>397</v>
+        <v>514</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="B16" s="120">
         <v>1998</v>
       </c>
       <c r="C16" s="126" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B17" s="120">
         <v>1413</v>
       </c>
       <c r="C17" s="126" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -43190,7 +43190,7 @@
         <v>300</v>
       </c>
       <c r="C18" s="126" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -43201,7 +43201,7 @@
         <v>250</v>
       </c>
       <c r="C19" s="126" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -43212,7 +43212,7 @@
         <v>400</v>
       </c>
       <c r="C20" s="126" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -43263,7 +43263,7 @@
         <v>600</v>
       </c>
       <c r="C25" s="126" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -43274,7 +43274,7 @@
         <v>1700</v>
       </c>
       <c r="C26" s="126" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -43285,7 +43285,7 @@
         <v>1120</v>
       </c>
       <c r="C27" s="126" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -43296,7 +43296,7 @@
         <v>2910</v>
       </c>
       <c r="C28" s="126" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -43317,7 +43317,7 @@
         <v>2375</v>
       </c>
       <c r="C30" s="126" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -43328,7 +43328,7 @@
         <v>1200</v>
       </c>
       <c r="C31" s="126" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -43339,7 +43339,7 @@
         <v>4195</v>
       </c>
       <c r="C32" s="126" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -43350,7 +43350,7 @@
         <v>2995</v>
       </c>
       <c r="C33" s="126" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -43361,7 +43361,7 @@
         <v>242</v>
       </c>
       <c r="C34" s="126" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -43382,7 +43382,7 @@
         <v>2685</v>
       </c>
       <c r="C36" s="126" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -43393,7 +43393,7 @@
         <v>2375</v>
       </c>
       <c r="C37" s="126" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -43404,7 +43404,7 @@
         <v>2070</v>
       </c>
       <c r="C38" s="126" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -43415,7 +43415,7 @@
         <v>4790</v>
       </c>
       <c r="C39" s="126" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -43426,7 +43426,7 @@
         <v>265</v>
       </c>
       <c r="C40" s="126" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -43437,7 +43437,7 @@
         <v>305</v>
       </c>
       <c r="C41" s="126" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -43448,7 +43448,7 @@
         <v>305</v>
       </c>
       <c r="C42" s="126" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -43459,7 +43459,7 @@
         <v>770</v>
       </c>
       <c r="C43" s="126" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -43470,7 +43470,7 @@
         <v>770</v>
       </c>
       <c r="C44" s="126" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -43481,7 +43481,7 @@
         <v>235</v>
       </c>
       <c r="C45" s="126" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -43492,7 +43492,7 @@
         <v>1770</v>
       </c>
       <c r="C46" s="126" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -43503,7 +43503,7 @@
         <v>1490</v>
       </c>
       <c r="C47" s="126" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -43514,7 +43514,7 @@
         <v>1500</v>
       </c>
       <c r="C48" s="126" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -43525,7 +43525,7 @@
         <v>1800</v>
       </c>
       <c r="C49" s="126" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -43536,7 +43536,7 @@
         <v>900</v>
       </c>
       <c r="C50" s="126" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -43547,7 +43547,7 @@
         <v>1500</v>
       </c>
       <c r="C51" s="126" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -43568,7 +43568,7 @@
         <v>450</v>
       </c>
       <c r="C53" s="126" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -43589,7 +43589,7 @@
         <v>200</v>
       </c>
       <c r="C55" s="126" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -43600,7 +43600,7 @@
         <v>190</v>
       </c>
       <c r="C56" s="126" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -43611,7 +43611,7 @@
         <v>230</v>
       </c>
       <c r="C57" s="126" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -43632,7 +43632,7 @@
         <v>300</v>
       </c>
       <c r="C59" s="126" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -43643,7 +43643,7 @@
         <v>135</v>
       </c>
       <c r="C60" s="126" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -43654,7 +43654,7 @@
         <v>80</v>
       </c>
       <c r="C61" s="126" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -43665,7 +43665,7 @@
         <v>770</v>
       </c>
       <c r="C62" s="126" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -43676,7 +43676,7 @@
         <v>770</v>
       </c>
       <c r="C63" s="126" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -43687,7 +43687,7 @@
         <v>785</v>
       </c>
       <c r="C64" s="126" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -43698,7 +43698,7 @@
         <v>3130</v>
       </c>
       <c r="C65" s="126" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -43709,7 +43709,7 @@
         <v>1880</v>
       </c>
       <c r="C66" s="126" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -43720,7 +43720,7 @@
         <v>2685</v>
       </c>
       <c r="C67" s="126" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -43731,7 +43731,7 @@
         <v>6425</v>
       </c>
       <c r="C68" s="126" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -43742,7 +43742,7 @@
         <v>895</v>
       </c>
       <c r="C69" s="126" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -43753,7 +43753,7 @@
         <v>540</v>
       </c>
       <c r="C70" s="126" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -43764,7 +43764,7 @@
         <v>1715</v>
       </c>
       <c r="C71" s="126" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -43775,7 +43775,7 @@
         <v>3750</v>
       </c>
       <c r="C72" s="126" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -43786,7 +43786,7 @@
         <v>1430</v>
       </c>
       <c r="C73" s="126" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -43797,7 +43797,7 @@
         <v>1500</v>
       </c>
       <c r="C74" s="126" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -43808,7 +43808,7 @@
         <v>1100</v>
       </c>
       <c r="C75" s="126" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -43819,7 +43819,7 @@
         <v>1000</v>
       </c>
       <c r="C76" s="126" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -43830,7 +43830,7 @@
         <v>1120</v>
       </c>
       <c r="C77" s="126" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -43841,7 +43841,7 @@
         <v>2725</v>
       </c>
       <c r="C78" s="126" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -43852,7 +43852,7 @@
         <v>2035</v>
       </c>
       <c r="C79" s="126" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -43863,7 +43863,7 @@
         <v>690</v>
       </c>
       <c r="C80" s="126" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -43874,7 +43874,7 @@
         <v>2705</v>
       </c>
       <c r="C81" s="126" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -43885,7 +43885,7 @@
         <v>1665</v>
       </c>
       <c r="C82" s="126" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -43896,7 +43896,7 @@
         <v>3250</v>
       </c>
       <c r="C83" s="126" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -43907,7 +43907,7 @@
         <v>2725</v>
       </c>
       <c r="C84" s="126" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -43918,7 +43918,7 @@
         <v>4205</v>
       </c>
       <c r="C85" s="126" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -43929,7 +43929,7 @@
         <v>7080</v>
       </c>
       <c r="C86" s="126" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -43940,7 +43940,7 @@
         <v>3470</v>
       </c>
       <c r="C87" s="126" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -43951,7 +43951,7 @@
         <v>6430</v>
       </c>
       <c r="C88" s="126" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -43962,7 +43962,7 @@
         <v>400</v>
       </c>
       <c r="C89" s="126" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -43973,7 +43973,7 @@
         <v>800</v>
       </c>
       <c r="C90" s="126" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -43984,7 +43984,7 @@
         <v>600</v>
       </c>
       <c r="C91" s="126" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -44007,7 +44007,7 @@
         <v>500</v>
       </c>
       <c r="C93" s="126" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -44030,7 +44030,7 @@
         <v>1500</v>
       </c>
       <c r="C95" s="126" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -44041,7 +44041,7 @@
         <v>1800</v>
       </c>
       <c r="C96" s="126" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -44052,7 +44052,7 @@
         <v>900</v>
       </c>
       <c r="C97" s="126" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -44063,7 +44063,7 @@
         <v>1500</v>
       </c>
       <c r="C98" s="126" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -44074,7 +44074,7 @@
         <v>925</v>
       </c>
       <c r="C99" s="126" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -44085,7 +44085,7 @@
         <v>1850</v>
       </c>
       <c r="C100" s="126" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -44096,7 +44096,7 @@
         <v>700</v>
       </c>
       <c r="C101" s="126" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -44107,7 +44107,7 @@
         <v>1400</v>
       </c>
       <c r="C102" s="126" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -44118,7 +44118,7 @@
         <v>525</v>
       </c>
       <c r="C103" s="126" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -44129,7 +44129,7 @@
         <v>1025</v>
       </c>
       <c r="C104" s="126" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -44140,7 +44140,7 @@
         <v>99</v>
       </c>
       <c r="C105" s="126" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -44151,7 +44151,7 @@
         <v>4830</v>
       </c>
       <c r="C106" s="126" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -44162,7 +44162,7 @@
         <v>7945</v>
       </c>
       <c r="C107" s="126" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -44183,7 +44183,7 @@
         <v>2265</v>
       </c>
       <c r="C109" s="126" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -44204,7 +44204,7 @@
         <v>700</v>
       </c>
       <c r="C111" s="126" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -44215,7 +44215,7 @@
         <v>5595</v>
       </c>
       <c r="C112" s="126" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -44226,7 +44226,7 @@
         <v>5595</v>
       </c>
       <c r="C113" s="126" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -44247,7 +44247,7 @@
         <v>1710</v>
       </c>
       <c r="C115" s="126" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -44258,7 +44258,7 @@
         <v>300</v>
       </c>
       <c r="C116" s="126" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -44269,7 +44269,7 @@
         <v>250</v>
       </c>
       <c r="C117" s="126" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -44280,7 +44280,7 @@
         <v>250</v>
       </c>
       <c r="C118" s="126" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -44291,7 +44291,7 @@
         <v>350</v>
       </c>
       <c r="C119" s="126" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -44302,7 +44302,7 @@
         <v>400</v>
       </c>
       <c r="C120" s="126" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -44457,7 +44457,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="49" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B151" s="49"/>
       <c r="C151" s="120"/>
@@ -44471,7 +44471,7 @@
         <v>1342</v>
       </c>
       <c r="C152" s="128" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -44480,245 +44480,245 @@
       </c>
       <c r="B153" s="120">
         <f>SUM(B13:B15)</f>
-        <v>7730</v>
+        <v>8070</v>
       </c>
       <c r="C153" s="126" t="s">
-        <v>416</v>
+        <v>515</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="34" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B154" s="120">
         <f>SUM(B11:B12)</f>
         <v>5975</v>
       </c>
       <c r="C154" s="126" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="34" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="B155" s="49"/>
       <c r="C155" s="126"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="34" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="B156" s="120">
         <f>SUM(B31:B33)</f>
         <v>8390</v>
       </c>
       <c r="C156" s="126" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="34" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="B157" s="120">
         <f>SUM(B39)</f>
         <v>4790</v>
       </c>
       <c r="C157" s="126" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="34" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B158" s="120">
         <f>SUM(B45:B47)</f>
         <v>3495</v>
       </c>
       <c r="C158" s="126" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="34" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B159" s="120">
         <f>SUM(B37:B38)</f>
         <v>4445</v>
       </c>
       <c r="C159" s="126" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="34" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B160" s="120">
         <f>SUM(B56,B40,B57,B41)</f>
         <v>990</v>
       </c>
       <c r="C160" s="126" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="34" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B161" s="120">
         <f>SUM(B115,B113,B112,B109,B62,B63,B44,B43)</f>
         <v>18245</v>
       </c>
       <c r="C161" s="126" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="34" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="B162" s="120">
         <f>SUM(B116:B119,B18,B19)</f>
         <v>1700</v>
       </c>
       <c r="C162" s="126" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="34" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="B163" s="129">
         <f>SUM(B64:B66)</f>
         <v>5795</v>
       </c>
       <c r="C163" s="126" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="34" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="B164" s="120">
         <f>SUM(B68)</f>
         <v>6425</v>
       </c>
       <c r="C164" s="126" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="34" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="B165" s="120">
         <f>SUM(B69:B73)</f>
         <v>8330</v>
       </c>
       <c r="C165" s="126" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="34" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="B166" s="120">
         <f>SUM(B80:B82)</f>
         <v>5060</v>
       </c>
       <c r="C166" s="126" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="34" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="B167" s="120">
         <f>SUM(B78:B79)</f>
         <v>4760</v>
       </c>
       <c r="C167" s="126" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="34" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B168" s="120">
         <f>SUM(B83:B88)</f>
         <v>27160</v>
       </c>
       <c r="C168" s="126" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="34" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B169" s="120">
         <f>SUM(B50,B51,B97,B98)</f>
         <v>4800</v>
       </c>
       <c r="C169" s="126" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="34" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B170" s="120">
         <f>SUM(B95,B96,B48,B49)</f>
         <v>6600</v>
       </c>
       <c r="C170" s="126" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="34" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B171" s="120">
         <f>SUM(B104,B103,B102,B101,B100,B99,B60,B61)</f>
         <v>6640</v>
       </c>
       <c r="C171" s="126" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="34" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B172" s="120">
         <f>SUM(B10,B26,B27,B28,B30,B36,B67)</f>
         <v>16160</v>
       </c>
       <c r="C172" s="126" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="34" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="B173" s="120">
         <f>SUM(B16:B17)</f>
         <v>3411</v>
       </c>
       <c r="C173" s="126" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -44871,7 +44871,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="B153:B154 B156 B158:B159 B162:B163 B165:B168 B173" formulaRange="1"/>
-    <ignoredError sqref="C31:C34 C25 C20 C13:C15 C6 C53 C55 C59 C74:C76 C93 C89:C91 C105:C107 C111 C120 C152:C153 C156" numberStoredAsText="1"/>
+    <ignoredError sqref="C31:C34 C25 C20 C6 C53 C55 C59 C74:C76 C93 C89:C91 C105:C107 C111 C120 C152 C156" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes to pricing tests
</commit_message>
<xml_diff>
--- a/Regression/templates/PriceProductGroups.xlsx
+++ b/Regression/templates/PriceProductGroups.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3764" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3763" uniqueCount="516">
   <si>
     <t>KBB Elite</t>
   </si>
@@ -1217,12 +1217,6 @@
     <t>$600.00</t>
   </si>
   <si>
-    <t>$1,200.00</t>
-  </si>
-  <si>
-    <t>$4,195.00</t>
-  </si>
-  <si>
     <t>$2,995.00</t>
   </si>
   <si>
@@ -1280,9 +1274,6 @@
     <t>FordNewCarPriceTotal</t>
   </si>
   <si>
-    <t>$8,390.00</t>
-  </si>
-  <si>
     <t>GMNewCarPriceTotal</t>
   </si>
   <si>
@@ -1337,12 +1328,6 @@
     <t>$2,375.00</t>
   </si>
   <si>
-    <t>$2,070.00</t>
-  </si>
-  <si>
-    <t>$4,445.00</t>
-  </si>
-  <si>
     <t>$190.00</t>
   </si>
   <si>
@@ -1496,9 +1481,6 @@
     <t>/Trade In Marketplace - KBB Buying Center</t>
   </si>
   <si>
-    <t>Escape</t>
-  </si>
-  <si>
     <t>$16,160.00</t>
   </si>
   <si>
@@ -1572,6 +1554,24 @@
   </si>
   <si>
     <t>$8,070.00</t>
+  </si>
+  <si>
+    <t>$1,255.00</t>
+  </si>
+  <si>
+    <t>$4,380.00</t>
+  </si>
+  <si>
+    <t>$8,765.00</t>
+  </si>
+  <si>
+    <t>$2,455.00</t>
+  </si>
+  <si>
+    <t>$2,140.00</t>
+  </si>
+  <si>
+    <t>$4,595.00</t>
   </si>
 </sst>
 </file>
@@ -2304,7 +2304,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2655,9 +2655,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="10" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3373,7 +3370,7 @@
       <c r="M7" s="37"/>
       <c r="N7" s="14"/>
       <c r="X7" s="12"/>
-      <c r="Y7" s="133"/>
+      <c r="Y7" s="132"/>
       <c r="Z7" s="14"/>
       <c r="AA7" s="35" t="s">
         <v>162</v>
@@ -3499,7 +3496,7 @@
     <col min="59" max="59" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="20" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="18" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="14.42578125" style="134" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="14.42578125" style="133" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3610,7 +3607,7 @@
         <v>241</v>
       </c>
       <c r="AJ1" s="68" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="AK1" s="68" t="s">
         <v>242</v>
@@ -3664,7 +3661,7 @@
         <v>214</v>
       </c>
       <c r="BB1" s="68" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="BC1" s="68" t="s">
         <v>216</v>
@@ -3696,7 +3693,7 @@
     </row>
     <row r="2" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="B2" s="73">
         <v>42617</v>
@@ -3802,7 +3799,7 @@
         <v>185</v>
       </c>
       <c r="AK2" s="86" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="AL2" s="37"/>
       <c r="AM2" s="35" t="s">
@@ -3881,7 +3878,7 @@
     </row>
     <row r="3" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="B3" s="73">
         <v>42617</v>
@@ -3985,7 +3982,7 @@
         <v>185</v>
       </c>
       <c r="AK3" s="86" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="AL3" s="37"/>
       <c r="AM3" s="35" t="s">
@@ -4070,7 +4067,7 @@
   <dimension ref="A1:FQ21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4991,7 +4988,7 @@
       <c r="FP4" s="7"/>
       <c r="FQ4" s="7"/>
     </row>
-    <row r="5" spans="1:173" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:173" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
         <v>9</v>
       </c>
@@ -5034,7 +5031,7 @@
       <c r="T5" s="8"/>
       <c r="U5" s="8"/>
       <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
+      <c r="W5" s="15"/>
       <c r="X5" s="8"/>
       <c r="Y5" s="8"/>
       <c r="Z5" s="8"/>
@@ -5218,7 +5215,7 @@
       <c r="FP5" s="7"/>
       <c r="FQ5" s="7"/>
     </row>
-    <row r="6" spans="1:173" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:173" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>11</v>
       </c>
@@ -5260,11 +5257,9 @@
       <c r="S6" s="8"/>
       <c r="T6" s="8"/>
       <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="132" t="s">
-        <v>490</v>
-      </c>
-      <c r="X6" s="8"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="37"/>
+      <c r="X6" s="14"/>
       <c r="Y6" s="8"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="8"/>
@@ -5447,7 +5442,7 @@
       <c r="FP6" s="7"/>
       <c r="FQ6" s="7"/>
     </row>
-    <row r="7" spans="1:173" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:173" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
         <v>10</v>
       </c>
@@ -5490,7 +5485,7 @@
       <c r="T7" s="8"/>
       <c r="U7" s="8"/>
       <c r="V7" s="8"/>
-      <c r="W7" s="8"/>
+      <c r="W7" s="36"/>
       <c r="X7" s="8"/>
       <c r="Y7" s="8"/>
       <c r="Z7" s="8"/>
@@ -8984,7 +8979,7 @@
         <v>214</v>
       </c>
       <c r="AL1" s="68" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="AM1" s="68" t="s">
         <v>216</v>
@@ -10054,7 +10049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CP138"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
@@ -10186,7 +10181,7 @@
         <v>241</v>
       </c>
       <c r="AI1" s="68" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="AJ1" s="119" t="s">
         <v>242</v>
@@ -10258,7 +10253,7 @@
         <v>214</v>
       </c>
       <c r="BG1" s="68" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="BH1" s="68" t="s">
         <v>216</v>
@@ -14017,7 +14012,7 @@
     </row>
     <row r="2" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="B2" s="93" t="s">
         <v>381</v>
@@ -14039,7 +14034,7 @@
     </row>
     <row r="3" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="B3" s="93" t="s">
         <v>381</v>
@@ -14558,7 +14553,7 @@
     </row>
     <row r="19" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="B19" s="93" t="s">
         <v>381</v>
@@ -42966,8 +42961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="C153" sqref="C153"/>
+    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="C159" sqref="C159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43102,7 +43097,7 @@
         <v>2685</v>
       </c>
       <c r="C10" s="126" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -43113,7 +43108,7 @@
         <v>2995</v>
       </c>
       <c r="C11" s="126" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -43124,7 +43119,7 @@
         <v>2980</v>
       </c>
       <c r="C12" s="126" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -43135,7 +43130,7 @@
         <v>1095</v>
       </c>
       <c r="C13" s="126" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -43146,7 +43141,7 @@
         <v>4315</v>
       </c>
       <c r="C14" s="126" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -43157,29 +43152,29 @@
         <v>2660</v>
       </c>
       <c r="C15" s="126" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="B16" s="120">
         <v>1998</v>
       </c>
       <c r="C16" s="126" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="B17" s="120">
         <v>1413</v>
       </c>
       <c r="C17" s="126" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -43190,7 +43185,7 @@
         <v>300</v>
       </c>
       <c r="C18" s="126" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -43201,7 +43196,7 @@
         <v>250</v>
       </c>
       <c r="C19" s="126" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -43274,7 +43269,7 @@
         <v>1700</v>
       </c>
       <c r="C26" s="126" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -43285,7 +43280,7 @@
         <v>1120</v>
       </c>
       <c r="C27" s="126" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -43296,7 +43291,7 @@
         <v>2910</v>
       </c>
       <c r="C28" s="126" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -43317,7 +43312,7 @@
         <v>2375</v>
       </c>
       <c r="C30" s="126" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -43325,10 +43320,10 @@
         <v>9</v>
       </c>
       <c r="B31" s="120">
-        <v>1200</v>
+        <v>1255</v>
       </c>
       <c r="C31" s="126" t="s">
-        <v>397</v>
+        <v>510</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -43336,10 +43331,10 @@
         <v>11</v>
       </c>
       <c r="B32" s="120">
-        <v>4195</v>
+        <v>4380</v>
       </c>
       <c r="C32" s="126" t="s">
-        <v>398</v>
+        <v>511</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -43347,10 +43342,10 @@
         <v>10</v>
       </c>
       <c r="B33" s="120">
-        <v>2995</v>
+        <v>3130</v>
       </c>
       <c r="C33" s="126" t="s">
-        <v>399</v>
+        <v>499</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -43361,7 +43356,7 @@
         <v>242</v>
       </c>
       <c r="C34" s="126" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -43382,7 +43377,7 @@
         <v>2685</v>
       </c>
       <c r="C36" s="126" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -43390,10 +43385,10 @@
         <v>47</v>
       </c>
       <c r="B37" s="120">
-        <v>2375</v>
+        <v>2455</v>
       </c>
       <c r="C37" s="126" t="s">
-        <v>436</v>
+        <v>513</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -43401,10 +43396,10 @@
         <v>48</v>
       </c>
       <c r="B38" s="120">
-        <v>2070</v>
+        <v>2140</v>
       </c>
       <c r="C38" s="126" t="s">
-        <v>437</v>
+        <v>514</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -43415,7 +43410,7 @@
         <v>4790</v>
       </c>
       <c r="C39" s="126" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -43426,7 +43421,7 @@
         <v>265</v>
       </c>
       <c r="C40" s="126" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -43437,7 +43432,7 @@
         <v>305</v>
       </c>
       <c r="C41" s="126" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -43448,7 +43443,7 @@
         <v>305</v>
       </c>
       <c r="C42" s="126" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -43459,7 +43454,7 @@
         <v>770</v>
       </c>
       <c r="C43" s="126" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -43470,7 +43465,7 @@
         <v>770</v>
       </c>
       <c r="C44" s="126" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -43481,7 +43476,7 @@
         <v>235</v>
       </c>
       <c r="C45" s="126" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -43492,7 +43487,7 @@
         <v>1770</v>
       </c>
       <c r="C46" s="126" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -43503,7 +43498,7 @@
         <v>1490</v>
       </c>
       <c r="C47" s="126" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -43514,7 +43509,7 @@
         <v>1500</v>
       </c>
       <c r="C48" s="126" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -43525,7 +43520,7 @@
         <v>1800</v>
       </c>
       <c r="C49" s="126" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -43536,7 +43531,7 @@
         <v>900</v>
       </c>
       <c r="C50" s="126" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -43547,7 +43542,7 @@
         <v>1500</v>
       </c>
       <c r="C51" s="126" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -43568,7 +43563,7 @@
         <v>450</v>
       </c>
       <c r="C53" s="126" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -43589,7 +43584,7 @@
         <v>200</v>
       </c>
       <c r="C55" s="126" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -43600,7 +43595,7 @@
         <v>190</v>
       </c>
       <c r="C56" s="126" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -43611,7 +43606,7 @@
         <v>230</v>
       </c>
       <c r="C57" s="126" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -43632,7 +43627,7 @@
         <v>300</v>
       </c>
       <c r="C59" s="126" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -43643,7 +43638,7 @@
         <v>135</v>
       </c>
       <c r="C60" s="126" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -43654,7 +43649,7 @@
         <v>80</v>
       </c>
       <c r="C61" s="126" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -43665,7 +43660,7 @@
         <v>770</v>
       </c>
       <c r="C62" s="126" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -43676,7 +43671,7 @@
         <v>770</v>
       </c>
       <c r="C63" s="126" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -43687,7 +43682,7 @@
         <v>785</v>
       </c>
       <c r="C64" s="126" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -43698,7 +43693,7 @@
         <v>3130</v>
       </c>
       <c r="C65" s="126" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -43709,7 +43704,7 @@
         <v>1880</v>
       </c>
       <c r="C66" s="126" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -43720,7 +43715,7 @@
         <v>2685</v>
       </c>
       <c r="C67" s="126" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -43731,7 +43726,7 @@
         <v>6425</v>
       </c>
       <c r="C68" s="126" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -43742,7 +43737,7 @@
         <v>895</v>
       </c>
       <c r="C69" s="126" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -43753,7 +43748,7 @@
         <v>540</v>
       </c>
       <c r="C70" s="126" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -43764,7 +43759,7 @@
         <v>1715</v>
       </c>
       <c r="C71" s="126" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -43775,7 +43770,7 @@
         <v>3750</v>
       </c>
       <c r="C72" s="126" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -43786,7 +43781,7 @@
         <v>1430</v>
       </c>
       <c r="C73" s="126" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -43797,7 +43792,7 @@
         <v>1500</v>
       </c>
       <c r="C74" s="126" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -43808,7 +43803,7 @@
         <v>1100</v>
       </c>
       <c r="C75" s="126" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -43819,7 +43814,7 @@
         <v>1000</v>
       </c>
       <c r="C76" s="126" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -43830,7 +43825,7 @@
         <v>1120</v>
       </c>
       <c r="C77" s="126" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -43841,7 +43836,7 @@
         <v>2725</v>
       </c>
       <c r="C78" s="126" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -43852,7 +43847,7 @@
         <v>2035</v>
       </c>
       <c r="C79" s="126" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -43863,7 +43858,7 @@
         <v>690</v>
       </c>
       <c r="C80" s="126" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -43874,7 +43869,7 @@
         <v>2705</v>
       </c>
       <c r="C81" s="126" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -43885,7 +43880,7 @@
         <v>1665</v>
       </c>
       <c r="C82" s="126" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -43896,7 +43891,7 @@
         <v>3250</v>
       </c>
       <c r="C83" s="126" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -43907,7 +43902,7 @@
         <v>2725</v>
       </c>
       <c r="C84" s="126" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -43918,7 +43913,7 @@
         <v>4205</v>
       </c>
       <c r="C85" s="126" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -43929,7 +43924,7 @@
         <v>7080</v>
       </c>
       <c r="C86" s="126" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -43940,7 +43935,7 @@
         <v>3470</v>
       </c>
       <c r="C87" s="126" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -43951,7 +43946,7 @@
         <v>6430</v>
       </c>
       <c r="C88" s="126" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -43973,7 +43968,7 @@
         <v>800</v>
       </c>
       <c r="C90" s="126" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -44007,7 +44002,7 @@
         <v>500</v>
       </c>
       <c r="C93" s="126" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -44030,7 +44025,7 @@
         <v>1500</v>
       </c>
       <c r="C95" s="126" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -44041,7 +44036,7 @@
         <v>1800</v>
       </c>
       <c r="C96" s="126" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -44052,7 +44047,7 @@
         <v>900</v>
       </c>
       <c r="C97" s="126" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -44063,7 +44058,7 @@
         <v>1500</v>
       </c>
       <c r="C98" s="126" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -44074,7 +44069,7 @@
         <v>925</v>
       </c>
       <c r="C99" s="126" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -44085,7 +44080,7 @@
         <v>1850</v>
       </c>
       <c r="C100" s="126" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -44096,7 +44091,7 @@
         <v>700</v>
       </c>
       <c r="C101" s="126" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -44107,7 +44102,7 @@
         <v>1400</v>
       </c>
       <c r="C102" s="126" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -44118,7 +44113,7 @@
         <v>525</v>
       </c>
       <c r="C103" s="126" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -44129,7 +44124,7 @@
         <v>1025</v>
       </c>
       <c r="C104" s="126" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -44140,7 +44135,7 @@
         <v>99</v>
       </c>
       <c r="C105" s="126" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -44151,7 +44146,7 @@
         <v>4830</v>
       </c>
       <c r="C106" s="126" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -44162,7 +44157,7 @@
         <v>7945</v>
       </c>
       <c r="C107" s="126" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -44183,7 +44178,7 @@
         <v>2265</v>
       </c>
       <c r="C109" s="126" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -44204,7 +44199,7 @@
         <v>700</v>
       </c>
       <c r="C111" s="126" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -44215,7 +44210,7 @@
         <v>5595</v>
       </c>
       <c r="C112" s="126" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -44226,7 +44221,7 @@
         <v>5595</v>
       </c>
       <c r="C113" s="126" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -44247,7 +44242,7 @@
         <v>1710</v>
       </c>
       <c r="C115" s="126" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -44258,7 +44253,7 @@
         <v>300</v>
       </c>
       <c r="C116" s="126" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -44269,7 +44264,7 @@
         <v>250</v>
       </c>
       <c r="C117" s="126" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -44280,7 +44275,7 @@
         <v>250</v>
       </c>
       <c r="C118" s="126" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -44291,7 +44286,7 @@
         <v>350</v>
       </c>
       <c r="C119" s="126" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -44457,7 +44452,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="49" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B151" s="49"/>
       <c r="C151" s="120"/>
@@ -44471,7 +44466,7 @@
         <v>1342</v>
       </c>
       <c r="C152" s="128" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -44483,242 +44478,242 @@
         <v>8070</v>
       </c>
       <c r="C153" s="126" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="34" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B154" s="120">
         <f>SUM(B11:B12)</f>
         <v>5975</v>
       </c>
       <c r="C154" s="126" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="34" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B155" s="49"/>
       <c r="C155" s="126"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="34" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B156" s="120">
         <f>SUM(B31:B33)</f>
-        <v>8390</v>
+        <v>8765</v>
       </c>
       <c r="C156" s="126" t="s">
-        <v>418</v>
+        <v>512</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="34" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B157" s="120">
         <f>SUM(B39)</f>
         <v>4790</v>
       </c>
       <c r="C157" s="126" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="34" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B158" s="120">
         <f>SUM(B45:B47)</f>
         <v>3495</v>
       </c>
       <c r="C158" s="126" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="34" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B159" s="120">
         <f>SUM(B37:B38)</f>
-        <v>4445</v>
+        <v>4595</v>
       </c>
       <c r="C159" s="126" t="s">
-        <v>438</v>
+        <v>515</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="34" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B160" s="120">
         <f>SUM(B56,B40,B57,B41)</f>
         <v>990</v>
       </c>
       <c r="C160" s="126" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="34" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="B161" s="120">
         <f>SUM(B115,B113,B112,B109,B62,B63,B44,B43)</f>
         <v>18245</v>
       </c>
       <c r="C161" s="126" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="34" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B162" s="120">
         <f>SUM(B116:B119,B18,B19)</f>
         <v>1700</v>
       </c>
       <c r="C162" s="126" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="34" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B163" s="129">
         <f>SUM(B64:B66)</f>
         <v>5795</v>
       </c>
       <c r="C163" s="126" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="34" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B164" s="120">
         <f>SUM(B68)</f>
         <v>6425</v>
       </c>
       <c r="C164" s="126" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="34" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B165" s="120">
         <f>SUM(B69:B73)</f>
         <v>8330</v>
       </c>
       <c r="C165" s="126" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="34" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B166" s="120">
         <f>SUM(B80:B82)</f>
         <v>5060</v>
       </c>
       <c r="C166" s="126" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="34" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B167" s="120">
         <f>SUM(B78:B79)</f>
         <v>4760</v>
       </c>
       <c r="C167" s="126" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="34" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B168" s="120">
         <f>SUM(B83:B88)</f>
         <v>27160</v>
       </c>
       <c r="C168" s="126" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="34" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B169" s="120">
         <f>SUM(B50,B51,B97,B98)</f>
         <v>4800</v>
       </c>
       <c r="C169" s="126" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="34" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B170" s="120">
         <f>SUM(B95,B96,B48,B49)</f>
         <v>6600</v>
       </c>
       <c r="C170" s="126" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="34" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B171" s="120">
         <f>SUM(B104,B103,B102,B101,B100,B99,B60,B61)</f>
         <v>6640</v>
       </c>
       <c r="C171" s="126" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="34" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B172" s="120">
         <f>SUM(B10,B26,B27,B28,B30,B36,B67)</f>
         <v>16160</v>
       </c>
       <c r="C172" s="126" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="34" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="B173" s="120">
         <f>SUM(B16:B17)</f>
         <v>3411</v>
       </c>
       <c r="C173" s="126" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -44871,7 +44866,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="B153:B154 B156 B158:B159 B162:B163 B165:B168 B173" formulaRange="1"/>
-    <ignoredError sqref="C31:C34 C25 C20 C6 C53 C55 C59 C74:C76 C93 C89:C91 C105:C107 C111 C120 C152 C156" numberStoredAsText="1"/>
+    <ignoredError sqref="C25 C20 C6 C53 C55 C59 C74:C76 C93 C89:C91 C105:C107 C111 C120 C152 C34" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix flat pricing test
</commit_message>
<xml_diff>
--- a/Regression/templates/PriceProductGroups.xlsx
+++ b/Regression/templates/PriceProductGroups.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="22995" windowHeight="10035" tabRatio="706" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="22995" windowHeight="10035" tabRatio="706" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="AlphazoneMakeCounties" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="Sheet1" sheetId="10" r:id="rId10"/>
     <sheet name="MVP" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3870" uniqueCount="517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3870" uniqueCount="518">
   <si>
     <t>KBB Elite</t>
   </si>
@@ -1575,6 +1575,9 @@
   </si>
   <si>
     <t>$14,100.00</t>
+  </si>
+  <si>
+    <t>/FastAds Vehicle Video Platinum 2.0</t>
   </si>
 </sst>
 </file>
@@ -3448,7 +3451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BK7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+    <sheetView topLeftCell="AP1" workbookViewId="0">
       <selection activeCell="AW7" sqref="AW7:AZ7"/>
     </sheetView>
   </sheetViews>
@@ -14417,8 +14420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15076,7 +15079,7 @@
     </row>
     <row r="17" spans="1:54" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
-        <v>83</v>
+        <v>517</v>
       </c>
       <c r="B17" s="93" t="s">
         <v>381</v>
@@ -17916,7 +17919,7 @@
       <c r="D2" s="51"/>
       <c r="E2" s="52">
         <f t="shared" ref="E2:E33" ca="1" si="0">TODAY()</f>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F2" s="51"/>
       <c r="G2" s="51"/>
@@ -18105,7 +18108,7 @@
       <c r="D3" s="51"/>
       <c r="E3" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F3" s="51"/>
       <c r="G3" s="51"/>
@@ -18294,7 +18297,7 @@
       <c r="D4" s="51"/>
       <c r="E4" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="51"/>
@@ -18483,7 +18486,7 @@
       <c r="D5" s="51"/>
       <c r="E5" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F5" s="51"/>
       <c r="G5" s="51"/>
@@ -18674,7 +18677,7 @@
       <c r="D6" s="51"/>
       <c r="E6" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F6" s="51" t="s">
         <v>262</v>
@@ -18889,7 +18892,7 @@
       <c r="D7" s="51"/>
       <c r="E7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
@@ -19090,7 +19093,7 @@
       <c r="D8" s="51"/>
       <c r="E8" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F8" s="51"/>
       <c r="G8" s="51"/>
@@ -19293,7 +19296,7 @@
       <c r="D9" s="51"/>
       <c r="E9" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
@@ -19490,7 +19493,7 @@
       <c r="D10" s="51"/>
       <c r="E10" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
@@ -19741,7 +19744,7 @@
       <c r="D11" s="51"/>
       <c r="E11" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
@@ -19994,7 +19997,7 @@
       <c r="D12" s="51"/>
       <c r="E12" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
@@ -20247,7 +20250,7 @@
       <c r="D13" s="51"/>
       <c r="E13" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F13" s="51"/>
       <c r="G13" s="51"/>
@@ -20480,7 +20483,7 @@
       <c r="D14" s="51"/>
       <c r="E14" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F14" s="51"/>
       <c r="G14" s="51"/>
@@ -20717,7 +20720,7 @@
       <c r="D15" s="51"/>
       <c r="E15" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F15" s="51"/>
       <c r="G15" s="51"/>
@@ -20950,7 +20953,7 @@
       <c r="D16" s="51"/>
       <c r="E16" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F16" s="51"/>
       <c r="G16" s="51"/>
@@ -21175,7 +21178,7 @@
       <c r="D17" s="51"/>
       <c r="E17" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F17" s="51"/>
       <c r="G17" s="51"/>
@@ -21400,7 +21403,7 @@
       <c r="D18" s="51"/>
       <c r="E18" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F18" s="51"/>
       <c r="G18" s="51"/>
@@ -21592,7 +21595,7 @@
       <c r="D19" s="51"/>
       <c r="E19" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F19" s="51"/>
       <c r="G19" s="51"/>
@@ -21781,7 +21784,7 @@
       <c r="D20" s="51"/>
       <c r="E20" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F20" s="51"/>
       <c r="G20" s="51"/>
@@ -21970,7 +21973,7 @@
       <c r="D21" s="51"/>
       <c r="E21" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F21" s="51"/>
       <c r="G21" s="51"/>
@@ -22161,7 +22164,7 @@
       <c r="D22" s="51"/>
       <c r="E22" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F22" s="51"/>
       <c r="G22" s="51"/>
@@ -22350,7 +22353,7 @@
       <c r="D23" s="51"/>
       <c r="E23" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F23" s="51"/>
       <c r="G23" s="51"/>
@@ -22577,7 +22580,7 @@
       <c r="D24" s="51"/>
       <c r="E24" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F24" s="51"/>
       <c r="G24" s="51"/>
@@ -22790,7 +22793,7 @@
       <c r="D25" s="51"/>
       <c r="E25" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F25" s="51"/>
       <c r="G25" s="51"/>
@@ -23003,7 +23006,7 @@
       <c r="D26" s="51"/>
       <c r="E26" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F26" s="51"/>
       <c r="G26" s="51"/>
@@ -23260,7 +23263,7 @@
       <c r="D27" s="51"/>
       <c r="E27" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F27" s="51"/>
       <c r="G27" s="51"/>
@@ -23517,7 +23520,7 @@
       <c r="D28" s="51"/>
       <c r="E28" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F28" s="51"/>
       <c r="G28" s="51"/>
@@ -23756,7 +23759,7 @@
       <c r="D29" s="51"/>
       <c r="E29" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F29" s="51"/>
       <c r="G29" s="51"/>
@@ -23991,7 +23994,7 @@
       <c r="D30" s="51"/>
       <c r="E30" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F30" s="51"/>
       <c r="G30" s="51"/>
@@ -24230,7 +24233,7 @@
       <c r="D31" s="51"/>
       <c r="E31" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F31" s="51"/>
       <c r="G31" s="51"/>
@@ -24467,7 +24470,7 @@
       </c>
       <c r="E32" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F32" s="51"/>
       <c r="G32" s="51"/>
@@ -24676,7 +24679,7 @@
       <c r="D33" s="51"/>
       <c r="E33" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F33" s="51"/>
       <c r="G33" s="51"/>
@@ -24883,7 +24886,7 @@
       <c r="D34" s="51"/>
       <c r="E34" s="52">
         <f t="shared" ref="E34:E65" ca="1" si="1">TODAY()</f>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F34" s="51"/>
       <c r="G34" s="51"/>
@@ -25138,7 +25141,7 @@
       <c r="D35" s="51"/>
       <c r="E35" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F35" s="51"/>
       <c r="G35" s="51"/>
@@ -25403,7 +25406,7 @@
       <c r="D36" s="51"/>
       <c r="E36" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F36" s="51"/>
       <c r="G36" s="51"/>
@@ -25668,7 +25671,7 @@
       <c r="D37" s="51"/>
       <c r="E37" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F37" s="51"/>
       <c r="G37" s="51"/>
@@ -25967,7 +25970,7 @@
       <c r="D38" s="51"/>
       <c r="E38" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F38" s="51"/>
       <c r="G38" s="51"/>
@@ -26176,7 +26179,7 @@
       <c r="D39" s="51"/>
       <c r="E39" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F39" s="51"/>
       <c r="G39" s="51"/>
@@ -26421,7 +26424,7 @@
       <c r="D40" s="51"/>
       <c r="E40" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F40" s="51"/>
       <c r="G40" s="51"/>
@@ -26632,7 +26635,7 @@
       <c r="D41" s="51"/>
       <c r="E41" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F41" s="51"/>
       <c r="G41" s="51"/>
@@ -26839,7 +26842,7 @@
       <c r="D42" s="51"/>
       <c r="E42" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F42" s="51"/>
       <c r="G42" s="51"/>
@@ -27060,7 +27063,7 @@
       <c r="D43" s="51"/>
       <c r="E43" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F43" s="51"/>
       <c r="G43" s="51"/>
@@ -27325,7 +27328,7 @@
       <c r="D44" s="51"/>
       <c r="E44" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F44" s="51"/>
       <c r="G44" s="51"/>
@@ -27590,7 +27593,7 @@
       <c r="D45" s="51"/>
       <c r="E45" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F45" s="51"/>
       <c r="G45" s="51"/>
@@ -27857,7 +27860,7 @@
       </c>
       <c r="E46" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F46" s="51"/>
       <c r="G46" s="51"/>
@@ -28070,7 +28073,7 @@
       </c>
       <c r="E47" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F47" s="51"/>
       <c r="G47" s="51"/>
@@ -28283,7 +28286,7 @@
       </c>
       <c r="E48" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F48" s="51"/>
       <c r="G48" s="51"/>
@@ -28494,7 +28497,7 @@
       </c>
       <c r="E49" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F49" s="51"/>
       <c r="G49" s="51"/>
@@ -28703,7 +28706,7 @@
       <c r="D50" s="51"/>
       <c r="E50" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F50" s="51"/>
       <c r="G50" s="51"/>
@@ -28894,7 +28897,7 @@
       <c r="D51" s="51"/>
       <c r="E51" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F51" s="51"/>
       <c r="G51" s="51"/>
@@ -29091,7 +29094,7 @@
       <c r="D52" s="51"/>
       <c r="E52" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F52" s="51"/>
       <c r="G52" s="51"/>
@@ -29284,7 +29287,7 @@
       <c r="D53" s="51"/>
       <c r="E53" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F53" s="51"/>
       <c r="G53" s="51"/>
@@ -29490,7 +29493,7 @@
       <c r="D54" s="51"/>
       <c r="E54" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F54" s="51"/>
       <c r="G54" s="51"/>
@@ -29695,7 +29698,7 @@
       <c r="D55" s="51"/>
       <c r="E55" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F55" s="51"/>
       <c r="G55" s="51"/>
@@ -29936,7 +29939,7 @@
       <c r="D56" s="51"/>
       <c r="E56" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F56" s="51"/>
       <c r="G56" s="51"/>
@@ -30141,7 +30144,7 @@
       <c r="D57" s="51"/>
       <c r="E57" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F57" s="51"/>
       <c r="G57" s="51"/>
@@ -30335,7 +30338,7 @@
       <c r="D58" s="51"/>
       <c r="E58" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F58" s="51"/>
       <c r="G58" s="51"/>
@@ -30535,7 +30538,7 @@
       <c r="D59" s="51"/>
       <c r="E59" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F59" s="51"/>
       <c r="G59" s="51"/>
@@ -30737,7 +30740,7 @@
       <c r="D60" s="51"/>
       <c r="E60" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F60" s="51"/>
       <c r="G60" s="51"/>
@@ -30934,7 +30937,7 @@
       <c r="D61" s="51"/>
       <c r="E61" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F61" s="51"/>
       <c r="G61" s="51"/>
@@ -31167,7 +31170,7 @@
       <c r="D62" s="51"/>
       <c r="E62" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F62" s="51"/>
       <c r="G62" s="51"/>
@@ -31400,7 +31403,7 @@
       <c r="D63" s="51"/>
       <c r="E63" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F63" s="51"/>
       <c r="G63" s="51"/>
@@ -31637,7 +31640,7 @@
       <c r="D64" s="51"/>
       <c r="E64" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F64" s="51"/>
       <c r="G64" s="51"/>
@@ -31870,7 +31873,7 @@
       <c r="D65" s="51"/>
       <c r="E65" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F65" s="51"/>
       <c r="G65" s="51"/>
@@ -32119,7 +32122,7 @@
       <c r="D66" s="51"/>
       <c r="E66" s="52">
         <f t="shared" ref="E66:E89" ca="1" si="2">TODAY()</f>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F66" s="51"/>
       <c r="G66" s="51"/>
@@ -32372,7 +32375,7 @@
       <c r="D67" s="51"/>
       <c r="E67" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F67" s="51"/>
       <c r="G67" s="51"/>
@@ -32609,7 +32612,7 @@
       <c r="D68" s="51"/>
       <c r="E68" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F68" s="51"/>
       <c r="G68" s="51"/>
@@ -32848,7 +32851,7 @@
       <c r="D69" s="51"/>
       <c r="E69" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F69" s="51"/>
       <c r="G69" s="51"/>
@@ -33087,7 +33090,7 @@
       <c r="D70" s="51"/>
       <c r="E70" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F70" s="51"/>
       <c r="G70" s="51"/>
@@ -33328,7 +33331,7 @@
       <c r="D71" s="51"/>
       <c r="E71" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F71" s="51"/>
       <c r="G71" s="51"/>
@@ -33565,7 +33568,7 @@
       <c r="D72" s="51"/>
       <c r="E72" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F72" s="51"/>
       <c r="G72" s="51"/>
@@ -33754,7 +33757,7 @@
       <c r="D73" s="51"/>
       <c r="E73" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F73" s="51"/>
       <c r="G73" s="51"/>
@@ -33943,7 +33946,7 @@
       <c r="D74" s="51"/>
       <c r="E74" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F74" s="51"/>
       <c r="G74" s="51"/>
@@ -34132,7 +34135,7 @@
       <c r="D75" s="51"/>
       <c r="E75" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F75" s="51"/>
       <c r="G75" s="51"/>
@@ -34381,7 +34384,7 @@
       <c r="D76" s="51"/>
       <c r="E76" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F76" s="51"/>
       <c r="G76" s="51"/>
@@ -34632,7 +34635,7 @@
       <c r="D77" s="51"/>
       <c r="E77" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F77" s="51"/>
       <c r="G77" s="51"/>
@@ -34883,7 +34886,7 @@
       <c r="D78" s="51"/>
       <c r="E78" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F78" s="51"/>
       <c r="G78" s="51"/>
@@ -35114,7 +35117,7 @@
       <c r="D79" s="51"/>
       <c r="E79" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F79" s="51"/>
       <c r="G79" s="51"/>
@@ -35349,7 +35352,7 @@
       <c r="D80" s="51"/>
       <c r="E80" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F80" s="51"/>
       <c r="G80" s="51"/>
@@ -35580,7 +35583,7 @@
       <c r="D81" s="51"/>
       <c r="E81" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F81" s="51"/>
       <c r="G81" s="51"/>
@@ -35823,7 +35826,7 @@
       <c r="D82" s="51"/>
       <c r="E82" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F82" s="51"/>
       <c r="G82" s="51"/>
@@ -36044,7 +36047,7 @@
       <c r="D83" s="51"/>
       <c r="E83" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F83" s="51"/>
       <c r="G83" s="51"/>
@@ -36293,7 +36296,7 @@
       <c r="D84" s="51"/>
       <c r="E84" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F84" s="51"/>
       <c r="G84" s="51"/>
@@ -36542,7 +36545,7 @@
       <c r="D85" s="51"/>
       <c r="E85" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F85" s="51"/>
       <c r="G85" s="51"/>
@@ -36791,7 +36794,7 @@
       <c r="D86" s="51"/>
       <c r="E86" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F86" s="51"/>
       <c r="G86" s="51"/>
@@ -37040,7 +37043,7 @@
       <c r="D87" s="51"/>
       <c r="E87" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F87" s="51"/>
       <c r="G87" s="51"/>
@@ -37231,7 +37234,7 @@
       <c r="D88" s="51"/>
       <c r="E88" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F88" s="51"/>
       <c r="G88" s="51"/>
@@ -37422,7 +37425,7 @@
       <c r="D89" s="51"/>
       <c r="E89" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F89" s="51"/>
       <c r="G89" s="51"/>
@@ -37797,7 +37800,7 @@
       <c r="D91" s="51"/>
       <c r="E91" s="52">
         <f ca="1">TODAY()</f>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F91" s="51"/>
       <c r="G91" s="51"/>
@@ -38172,7 +38175,7 @@
       <c r="D93" s="51"/>
       <c r="E93" s="52">
         <f t="shared" ref="E93:E118" ca="1" si="3">TODAY()</f>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F93" s="51"/>
       <c r="G93" s="51"/>
@@ -38389,7 +38392,7 @@
       <c r="D94" s="51"/>
       <c r="E94" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F94" s="51"/>
       <c r="G94" s="51"/>
@@ -38606,7 +38609,7 @@
       <c r="D95" s="51"/>
       <c r="E95" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F95" s="51"/>
       <c r="G95" s="51"/>
@@ -38821,7 +38824,7 @@
       <c r="D96" s="51"/>
       <c r="E96" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F96" s="51"/>
       <c r="G96" s="51"/>
@@ -39034,7 +39037,7 @@
       <c r="D97" s="51"/>
       <c r="E97" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F97" s="51"/>
       <c r="G97" s="51"/>
@@ -39234,7 +39237,7 @@
       <c r="D98" s="51"/>
       <c r="E98" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F98" s="51"/>
       <c r="G98" s="51"/>
@@ -39434,7 +39437,7 @@
       <c r="D99" s="51"/>
       <c r="E99" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F99" s="51"/>
       <c r="G99" s="51"/>
@@ -39636,7 +39639,7 @@
       <c r="D100" s="51"/>
       <c r="E100" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F100" s="51"/>
       <c r="G100" s="51"/>
@@ -39838,7 +39841,7 @@
       <c r="D101" s="51"/>
       <c r="E101" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F101" s="51"/>
       <c r="G101" s="51"/>
@@ -40040,7 +40043,7 @@
       <c r="D102" s="51"/>
       <c r="E102" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F102" s="51"/>
       <c r="G102" s="51"/>
@@ -40242,7 +40245,7 @@
       <c r="D103" s="51"/>
       <c r="E103" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F103" s="51"/>
       <c r="G103" s="51"/>
@@ -40443,7 +40446,7 @@
       <c r="D104" s="51"/>
       <c r="E104" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F104" s="51"/>
       <c r="G104" s="51"/>
@@ -40660,7 +40663,7 @@
       <c r="D105" s="51"/>
       <c r="E105" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F105" s="51"/>
       <c r="G105" s="51"/>
@@ -40877,7 +40880,7 @@
       <c r="D106" s="51"/>
       <c r="E106" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F106" s="51"/>
       <c r="G106" s="51"/>
@@ -41094,7 +41097,7 @@
       <c r="D107" s="51"/>
       <c r="E107" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F107" s="51"/>
       <c r="G107" s="51"/>
@@ -41311,7 +41314,7 @@
       <c r="D108" s="51"/>
       <c r="E108" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F108" s="51"/>
       <c r="G108" s="51"/>
@@ -41528,7 +41531,7 @@
       <c r="D109" s="51"/>
       <c r="E109" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F109" s="51"/>
       <c r="G109" s="51"/>
@@ -41745,7 +41748,7 @@
       <c r="D110" s="51"/>
       <c r="E110" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F110" s="51"/>
       <c r="G110" s="51"/>
@@ -41962,7 +41965,7 @@
       <c r="D111" s="51"/>
       <c r="E111" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F111" s="51"/>
       <c r="G111" s="51"/>
@@ -42179,7 +42182,7 @@
       <c r="D112" s="51"/>
       <c r="E112" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F112" s="51"/>
       <c r="G112" s="51"/>
@@ -42396,7 +42399,7 @@
       <c r="D113" s="51"/>
       <c r="E113" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F113" s="51"/>
       <c r="G113" s="51"/>
@@ -42613,7 +42616,7 @@
       <c r="D114" s="51"/>
       <c r="E114" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F114" s="51"/>
       <c r="G114" s="51"/>
@@ -42802,7 +42805,7 @@
       <c r="D115" s="51"/>
       <c r="E115" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F115" s="51"/>
       <c r="G115" s="51"/>
@@ -42991,7 +42994,7 @@
       <c r="D116" s="51"/>
       <c r="E116" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F116" s="51"/>
       <c r="G116" s="51"/>
@@ -43180,7 +43183,7 @@
       <c r="D117" s="51"/>
       <c r="E117" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F117" s="51"/>
       <c r="G117" s="51"/>
@@ -43369,7 +43372,7 @@
       <c r="D118" s="51"/>
       <c r="E118" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42600</v>
+        <v>42628</v>
       </c>
       <c r="F118" s="51"/>
       <c r="G118" s="51"/>

</xml_diff>